<commit_message>
62 left pir 50k sent bank
</commit_message>
<xml_diff>
--- a/Office Statement Expense & Expenditure.xlsx
+++ b/Office Statement Expense & Expenditure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Najeeb Associates\000FFICE\Office Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E48BCBE-65A6-4E8C-A023-7F21DE5D2CC8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DE22BB-6E41-49E4-88A7-A3788C06556F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="904" activeTab="15" xr2:uid="{B2A19E3B-6786-4ED5-96A6-D1A6BAD18668}"/>
   </bookViews>
@@ -2943,13 +2943,7 @@
     <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2958,19 +2952,13 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2982,6 +2970,18 @@
     <xf numFmtId="0" fontId="17" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2991,8 +2991,17 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3012,23 +3021,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3044,21 +3059,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -14743,37 +14743,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A140:I140"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="F141:I141"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="F163:H163"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="F113:I113"/>
-    <mergeCell ref="A133:C133"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="A105:C105"/>
+    <mergeCell ref="F105:H105"/>
     <mergeCell ref="A62:I62"/>
     <mergeCell ref="A63:I63"/>
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="F64:I64"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="F79:H79"/>
-    <mergeCell ref="A86:I86"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="A105:C105"/>
-    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="F56:H56"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="F113:I113"/>
+    <mergeCell ref="A133:C133"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="A140:I140"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="F141:I141"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="F163:H163"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="53" orientation="portrait" r:id="rId1"/>
@@ -14803,18 +14803,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="297" t="s">
+      <c r="A1" s="303" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="298"/>
-      <c r="C1" s="298"/>
+      <c r="B1" s="304"/>
+      <c r="C1" s="304"/>
       <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="290" t="s">
+      <c r="E1" s="305" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="290"/>
+      <c r="F1" s="305"/>
       <c r="G1" s="14">
         <v>50000</v>
       </c>
@@ -14933,17 +14933,17 @@
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A5" s="303">
+      <c r="A5" s="308">
         <v>3</v>
       </c>
-      <c r="B5" s="304">
+      <c r="B5" s="309">
         <v>44063</v>
       </c>
-      <c r="C5" s="305" t="s">
+      <c r="C5" s="310" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="306"/>
-      <c r="E5" s="307"/>
+      <c r="D5" s="311"/>
+      <c r="E5" s="312"/>
       <c r="F5" s="4">
         <v>11640</v>
       </c>
@@ -14965,11 +14965,11 @@
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A6" s="303"/>
-      <c r="B6" s="304"/>
-      <c r="C6" s="305"/>
-      <c r="D6" s="306"/>
-      <c r="E6" s="307"/>
+      <c r="A6" s="308"/>
+      <c r="B6" s="309"/>
+      <c r="C6" s="310"/>
+      <c r="D6" s="311"/>
+      <c r="E6" s="312"/>
       <c r="F6" s="4">
         <v>1700</v>
       </c>
@@ -14991,10 +14991,10 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A7" s="303">
+      <c r="A7" s="308">
         <v>4</v>
       </c>
-      <c r="B7" s="304">
+      <c r="B7" s="309">
         <v>44064</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -15023,8 +15023,8 @@
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A8" s="303"/>
-      <c r="B8" s="304"/>
+      <c r="A8" s="308"/>
+      <c r="B8" s="309"/>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -15085,10 +15085,10 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A10" s="303">
+      <c r="A10" s="308">
         <v>6</v>
       </c>
-      <c r="B10" s="304">
+      <c r="B10" s="309">
         <v>44066</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -15117,8 +15117,8 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A11" s="303"/>
-      <c r="B11" s="304"/>
+      <c r="A11" s="308"/>
+      <c r="B11" s="309"/>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
@@ -15150,7 +15150,7 @@
       <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="304">
+      <c r="B12" s="309">
         <v>44067</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -15182,7 +15182,7 @@
       <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="B13" s="304"/>
+      <c r="B13" s="309"/>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
@@ -15275,12 +15275,12 @@
       <c r="S15" s="8"/>
     </row>
     <row r="16" spans="1:19" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="299" t="s">
+      <c r="A16" s="290" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="299"/>
-      <c r="C16" s="299"/>
-      <c r="D16" s="300"/>
+      <c r="B16" s="290"/>
+      <c r="C16" s="290"/>
+      <c r="D16" s="291"/>
       <c r="E16" s="16">
         <f>SUM(E3:E15)</f>
         <v>0</v>
@@ -15307,10 +15307,10 @@
       <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="301"/>
-      <c r="B17" s="301"/>
-      <c r="C17" s="301"/>
-      <c r="D17" s="302"/>
+      <c r="A17" s="292"/>
+      <c r="B17" s="292"/>
+      <c r="C17" s="292"/>
+      <c r="D17" s="293"/>
       <c r="E17" s="17" t="s">
         <v>61</v>
       </c>
@@ -15355,18 +15355,18 @@
       <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="297" t="s">
+      <c r="A19" s="303" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="298"/>
-      <c r="C19" s="298"/>
+      <c r="B19" s="304"/>
+      <c r="C19" s="304"/>
       <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="290" t="s">
+      <c r="E19" s="305" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="290"/>
+      <c r="F19" s="305"/>
       <c r="G19" s="14">
         <v>31780</v>
       </c>
@@ -15451,10 +15451,10 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A22" s="294">
+      <c r="A22" s="297">
         <v>12</v>
       </c>
-      <c r="B22" s="291">
+      <c r="B22" s="294">
         <v>44076</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -15483,8 +15483,8 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A23" s="295"/>
-      <c r="B23" s="292"/>
+      <c r="A23" s="298"/>
+      <c r="B23" s="295"/>
       <c r="C23" s="21" t="s">
         <v>21</v>
       </c>
@@ -15511,8 +15511,8 @@
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A24" s="296"/>
-      <c r="B24" s="293"/>
+      <c r="A24" s="299"/>
+      <c r="B24" s="296"/>
       <c r="C24" s="21" t="s">
         <v>22</v>
       </c>
@@ -15541,10 +15541,10 @@
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A25" s="294">
+      <c r="A25" s="297">
         <v>13</v>
       </c>
-      <c r="B25" s="291">
+      <c r="B25" s="294">
         <v>44077</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -15575,8 +15575,8 @@
       <c r="S25" s="8"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A26" s="296"/>
-      <c r="B26" s="293"/>
+      <c r="A26" s="299"/>
+      <c r="B26" s="296"/>
       <c r="C26" s="21" t="s">
         <v>26</v>
       </c>
@@ -15605,10 +15605,10 @@
       <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A27" s="294">
+      <c r="A27" s="297">
         <v>14</v>
       </c>
-      <c r="B27" s="291">
+      <c r="B27" s="294">
         <v>44078</v>
       </c>
       <c r="C27" s="21" t="s">
@@ -15637,8 +15637,8 @@
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A28" s="296"/>
-      <c r="B28" s="293"/>
+      <c r="A28" s="299"/>
+      <c r="B28" s="296"/>
       <c r="C28" s="21" t="s">
         <v>28</v>
       </c>
@@ -15667,10 +15667,10 @@
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A29" s="294">
+      <c r="A29" s="297">
         <v>15</v>
       </c>
-      <c r="B29" s="291">
+      <c r="B29" s="294">
         <v>44079</v>
       </c>
       <c r="C29" s="21" t="s">
@@ -15699,8 +15699,8 @@
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A30" s="295"/>
-      <c r="B30" s="292"/>
+      <c r="A30" s="298"/>
+      <c r="B30" s="295"/>
       <c r="C30" s="21" t="s">
         <v>30</v>
       </c>
@@ -15729,8 +15729,8 @@
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A31" s="295"/>
-      <c r="B31" s="292"/>
+      <c r="A31" s="298"/>
+      <c r="B31" s="295"/>
       <c r="C31" s="21" t="s">
         <v>60</v>
       </c>
@@ -15757,8 +15757,8 @@
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A32" s="296"/>
-      <c r="B32" s="293"/>
+      <c r="A32" s="299"/>
+      <c r="B32" s="296"/>
       <c r="C32" s="23" t="s">
         <v>31</v>
       </c>
@@ -15785,10 +15785,10 @@
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A33" s="294">
+      <c r="A33" s="297">
         <v>16</v>
       </c>
-      <c r="B33" s="291">
+      <c r="B33" s="294">
         <v>44080</v>
       </c>
       <c r="C33" s="21" t="s">
@@ -15819,8 +15819,8 @@
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A34" s="295"/>
-      <c r="B34" s="292"/>
+      <c r="A34" s="298"/>
+      <c r="B34" s="295"/>
       <c r="C34" s="21" t="s">
         <v>33</v>
       </c>
@@ -15849,8 +15849,8 @@
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A35" s="295"/>
-      <c r="B35" s="292"/>
+      <c r="A35" s="298"/>
+      <c r="B35" s="295"/>
       <c r="C35" s="21" t="s">
         <v>36</v>
       </c>
@@ -15879,8 +15879,8 @@
       <c r="S35" s="8"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A36" s="295"/>
-      <c r="B36" s="292"/>
+      <c r="A36" s="298"/>
+      <c r="B36" s="295"/>
       <c r="C36" s="21" t="s">
         <v>37</v>
       </c>
@@ -15909,8 +15909,8 @@
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A37" s="296"/>
-      <c r="B37" s="293"/>
+      <c r="A37" s="299"/>
+      <c r="B37" s="296"/>
       <c r="C37" s="21" t="s">
         <v>39</v>
       </c>
@@ -15937,10 +15937,10 @@
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A38" s="294">
+      <c r="A38" s="297">
         <v>17</v>
       </c>
-      <c r="B38" s="291">
+      <c r="B38" s="294">
         <v>44081</v>
       </c>
       <c r="C38" s="21" t="s">
@@ -15969,8 +15969,8 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A39" s="295"/>
-      <c r="B39" s="292"/>
+      <c r="A39" s="298"/>
+      <c r="B39" s="295"/>
       <c r="C39" s="21" t="s">
         <v>28</v>
       </c>
@@ -15997,8 +15997,8 @@
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A40" s="296"/>
-      <c r="B40" s="293"/>
+      <c r="A40" s="299"/>
+      <c r="B40" s="296"/>
       <c r="C40" s="21" t="s">
         <v>40</v>
       </c>
@@ -16027,10 +16027,10 @@
       <c r="S40" s="8"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A41" s="294">
+      <c r="A41" s="297">
         <v>18</v>
       </c>
-      <c r="B41" s="291">
+      <c r="B41" s="294">
         <v>44082</v>
       </c>
       <c r="C41" s="21" t="s">
@@ -16059,8 +16059,8 @@
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A42" s="296"/>
-      <c r="B42" s="293"/>
+      <c r="A42" s="299"/>
+      <c r="B42" s="296"/>
       <c r="C42" s="21" t="s">
         <v>42</v>
       </c>
@@ -16087,10 +16087,10 @@
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A43" s="294">
+      <c r="A43" s="297">
         <v>19</v>
       </c>
-      <c r="B43" s="291">
+      <c r="B43" s="294">
         <v>44083</v>
       </c>
       <c r="C43" s="21" t="s">
@@ -16119,8 +16119,8 @@
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A44" s="296"/>
-      <c r="B44" s="293"/>
+      <c r="A44" s="299"/>
+      <c r="B44" s="296"/>
       <c r="C44" s="21" t="s">
         <v>44</v>
       </c>
@@ -16147,10 +16147,10 @@
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A45" s="294">
+      <c r="A45" s="297">
         <v>20</v>
       </c>
-      <c r="B45" s="291">
+      <c r="B45" s="294">
         <v>44084</v>
       </c>
       <c r="C45" s="21" t="s">
@@ -16179,8 +16179,8 @@
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A46" s="296"/>
-      <c r="B46" s="293"/>
+      <c r="A46" s="299"/>
+      <c r="B46" s="296"/>
       <c r="C46" s="21" t="s">
         <v>45</v>
       </c>
@@ -16207,10 +16207,10 @@
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A47" s="294">
+      <c r="A47" s="297">
         <v>21</v>
       </c>
-      <c r="B47" s="291">
+      <c r="B47" s="294">
         <v>44085</v>
       </c>
       <c r="C47" s="21" t="s">
@@ -16239,8 +16239,8 @@
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A48" s="295"/>
-      <c r="B48" s="292"/>
+      <c r="A48" s="298"/>
+      <c r="B48" s="295"/>
       <c r="C48" s="21" t="s">
         <v>46</v>
       </c>
@@ -16267,8 +16267,8 @@
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A49" s="295"/>
-      <c r="B49" s="292"/>
+      <c r="A49" s="298"/>
+      <c r="B49" s="295"/>
       <c r="C49" s="21" t="s">
         <v>47</v>
       </c>
@@ -16295,8 +16295,8 @@
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A50" s="295"/>
-      <c r="B50" s="292"/>
+      <c r="A50" s="298"/>
+      <c r="B50" s="295"/>
       <c r="C50" s="23" t="s">
         <v>31</v>
       </c>
@@ -16323,8 +16323,8 @@
       <c r="S50" s="8"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A51" s="296"/>
-      <c r="B51" s="293"/>
+      <c r="A51" s="299"/>
+      <c r="B51" s="296"/>
       <c r="C51" s="21" t="s">
         <v>44</v>
       </c>
@@ -16353,10 +16353,10 @@
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A52" s="294">
+      <c r="A52" s="297">
         <v>22</v>
       </c>
-      <c r="B52" s="291">
+      <c r="B52" s="294">
         <v>44086</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -16387,8 +16387,8 @@
       <c r="S52" s="8"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A53" s="296"/>
-      <c r="B53" s="293"/>
+      <c r="A53" s="299"/>
+      <c r="B53" s="296"/>
       <c r="C53" s="21" t="s">
         <v>50</v>
       </c>
@@ -16415,10 +16415,10 @@
       <c r="S53" s="8"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A54" s="294">
+      <c r="A54" s="297">
         <v>23</v>
       </c>
-      <c r="B54" s="291">
+      <c r="B54" s="294">
         <v>44087</v>
       </c>
       <c r="C54" s="21" t="s">
@@ -16447,8 +16447,8 @@
       <c r="S54" s="8"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A55" s="295"/>
-      <c r="B55" s="292"/>
+      <c r="A55" s="298"/>
+      <c r="B55" s="295"/>
       <c r="C55" s="21" t="s">
         <v>28</v>
       </c>
@@ -16475,8 +16475,8 @@
       <c r="S55" s="8"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A56" s="295"/>
-      <c r="B56" s="292"/>
+      <c r="A56" s="298"/>
+      <c r="B56" s="295"/>
       <c r="C56" s="21" t="s">
         <v>51</v>
       </c>
@@ -16503,8 +16503,8 @@
       <c r="S56" s="8"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A57" s="295"/>
-      <c r="B57" s="292"/>
+      <c r="A57" s="298"/>
+      <c r="B57" s="295"/>
       <c r="C57" s="23" t="s">
         <v>31</v>
       </c>
@@ -16629,10 +16629,10 @@
       <c r="S60" s="8"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A61" s="294">
+      <c r="A61" s="297">
         <v>27</v>
       </c>
-      <c r="B61" s="291">
+      <c r="B61" s="294">
         <v>44091</v>
       </c>
       <c r="C61" s="21" t="s">
@@ -16661,8 +16661,8 @@
       <c r="S61" s="8"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A62" s="296"/>
-      <c r="B62" s="293"/>
+      <c r="A62" s="299"/>
+      <c r="B62" s="296"/>
       <c r="C62" s="21" t="s">
         <v>44</v>
       </c>
@@ -16721,10 +16721,10 @@
       <c r="S63" s="8"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A64" s="294">
+      <c r="A64" s="297">
         <v>29</v>
       </c>
-      <c r="B64" s="291">
+      <c r="B64" s="294">
         <v>44093</v>
       </c>
       <c r="C64" s="21" t="s">
@@ -16753,8 +16753,8 @@
       <c r="S64" s="8"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A65" s="296"/>
-      <c r="B65" s="293"/>
+      <c r="A65" s="299"/>
+      <c r="B65" s="296"/>
       <c r="C65" s="21" t="s">
         <v>18</v>
       </c>
@@ -16949,10 +16949,10 @@
       <c r="B71" s="28">
         <v>44101</v>
       </c>
-      <c r="C71" s="308" t="s">
+      <c r="C71" s="306" t="s">
         <v>65</v>
       </c>
-      <c r="D71" s="309"/>
+      <c r="D71" s="307"/>
       <c r="E71" s="26">
         <v>0</v>
       </c>
@@ -16977,10 +16977,10 @@
       <c r="S71" s="8"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A72" s="294">
+      <c r="A72" s="297">
         <v>37</v>
       </c>
-      <c r="B72" s="291">
+      <c r="B72" s="294">
         <v>44103</v>
       </c>
       <c r="C72" s="21" t="s">
@@ -17009,12 +17009,12 @@
       <c r="S72" s="8"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A73" s="296"/>
-      <c r="B73" s="293"/>
-      <c r="C73" s="308" t="s">
+      <c r="A73" s="299"/>
+      <c r="B73" s="296"/>
+      <c r="C73" s="306" t="s">
         <v>75</v>
       </c>
-      <c r="D73" s="309"/>
+      <c r="D73" s="307"/>
       <c r="E73" s="6">
         <v>100000</v>
       </c>
@@ -17071,12 +17071,12 @@
       <c r="S74" s="8"/>
     </row>
     <row r="75" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A75" s="299" t="s">
+      <c r="A75" s="290" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="299"/>
-      <c r="C75" s="299"/>
-      <c r="D75" s="300"/>
+      <c r="B75" s="290"/>
+      <c r="C75" s="290"/>
+      <c r="D75" s="291"/>
       <c r="E75" s="16">
         <f>SUM(E21:E74)</f>
         <v>132000</v>
@@ -17103,10 +17103,10 @@
       <c r="S75" s="8"/>
     </row>
     <row r="76" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="301"/>
-      <c r="B76" s="301"/>
-      <c r="C76" s="301"/>
-      <c r="D76" s="302"/>
+      <c r="A76" s="292"/>
+      <c r="B76" s="292"/>
+      <c r="C76" s="292"/>
+      <c r="D76" s="293"/>
       <c r="E76" s="17" t="s">
         <v>61</v>
       </c>
@@ -17151,18 +17151,18 @@
       <c r="S77" s="8"/>
     </row>
     <row r="78" spans="1:19" ht="27.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="297" t="s">
+      <c r="A78" s="303" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="298"/>
-      <c r="C78" s="298"/>
+      <c r="B78" s="304"/>
+      <c r="C78" s="304"/>
       <c r="D78" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E78" s="290" t="s">
+      <c r="E78" s="305" t="s">
         <v>0</v>
       </c>
-      <c r="F78" s="290"/>
+      <c r="F78" s="305"/>
       <c r="G78" s="14">
         <f>G75</f>
         <v>137640</v>
@@ -17216,10 +17216,10 @@
       <c r="S79" s="8"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A80" s="294">
+      <c r="A80" s="297">
         <v>39</v>
       </c>
-      <c r="B80" s="291">
+      <c r="B80" s="294">
         <v>44105</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -17248,8 +17248,8 @@
       <c r="S80" s="8"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A81" s="295"/>
-      <c r="B81" s="292"/>
+      <c r="A81" s="298"/>
+      <c r="B81" s="295"/>
       <c r="C81" s="1" t="s">
         <v>70</v>
       </c>
@@ -17276,8 +17276,8 @@
       <c r="S81" s="8"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A82" s="295"/>
-      <c r="B82" s="292"/>
+      <c r="A82" s="298"/>
+      <c r="B82" s="295"/>
       <c r="C82" s="34" t="s">
         <v>76</v>
       </c>
@@ -17306,9 +17306,9 @@
       <c r="S82" s="8"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A83" s="295"/>
-      <c r="B83" s="292"/>
-      <c r="C83" s="310" t="s">
+      <c r="A83" s="298"/>
+      <c r="B83" s="295"/>
+      <c r="C83" s="300" t="s">
         <v>77</v>
       </c>
       <c r="D83" s="32" t="s">
@@ -17336,9 +17336,9 @@
       <c r="S83" s="8"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A84" s="295"/>
-      <c r="B84" s="292"/>
-      <c r="C84" s="311"/>
+      <c r="A84" s="298"/>
+      <c r="B84" s="295"/>
+      <c r="C84" s="301"/>
       <c r="D84" s="32" t="s">
         <v>71</v>
       </c>
@@ -17364,9 +17364,9 @@
       <c r="S84" s="8"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A85" s="295"/>
-      <c r="B85" s="292"/>
-      <c r="C85" s="311"/>
+      <c r="A85" s="298"/>
+      <c r="B85" s="295"/>
+      <c r="C85" s="301"/>
       <c r="D85" s="32" t="s">
         <v>73</v>
       </c>
@@ -17392,9 +17392,9 @@
       <c r="S85" s="8"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A86" s="296"/>
-      <c r="B86" s="293"/>
-      <c r="C86" s="312"/>
+      <c r="A86" s="299"/>
+      <c r="B86" s="296"/>
+      <c r="C86" s="302"/>
       <c r="D86" s="32" t="s">
         <v>74</v>
       </c>
@@ -17452,10 +17452,10 @@
       <c r="S87" s="8"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A88" s="294">
+      <c r="A88" s="297">
         <v>41</v>
       </c>
-      <c r="B88" s="291">
+      <c r="B88" s="294">
         <v>44108</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -17484,8 +17484,8 @@
       <c r="S88" s="8"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A89" s="296"/>
-      <c r="B89" s="293"/>
+      <c r="A89" s="299"/>
+      <c r="B89" s="296"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="4"/>
@@ -17574,10 +17574,10 @@
       <c r="S91" s="8"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A92" s="294">
+      <c r="A92" s="297">
         <v>44</v>
       </c>
-      <c r="B92" s="291">
+      <c r="B92" s="294">
         <v>44112</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -17606,8 +17606,8 @@
       <c r="S92" s="8"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A93" s="295"/>
-      <c r="B93" s="292"/>
+      <c r="A93" s="298"/>
+      <c r="B93" s="295"/>
       <c r="C93" s="1" t="s">
         <v>113</v>
       </c>
@@ -17634,8 +17634,8 @@
       <c r="S93" s="8"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A94" s="295"/>
-      <c r="B94" s="292"/>
+      <c r="A94" s="298"/>
+      <c r="B94" s="295"/>
       <c r="C94" s="1" t="s">
         <v>98</v>
       </c>
@@ -17664,8 +17664,8 @@
       <c r="S94" s="8"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A95" s="296"/>
-      <c r="B95" s="293"/>
+      <c r="A95" s="299"/>
+      <c r="B95" s="296"/>
       <c r="C95" s="1" t="s">
         <v>111</v>
       </c>
@@ -18124,12 +18124,12 @@
       <c r="S113" s="8"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A114" s="299" t="s">
+      <c r="A114" s="290" t="s">
         <v>57</v>
       </c>
-      <c r="B114" s="299"/>
-      <c r="C114" s="299"/>
-      <c r="D114" s="300"/>
+      <c r="B114" s="290"/>
+      <c r="C114" s="290"/>
+      <c r="D114" s="291"/>
       <c r="E114" s="16">
         <f>SUM(E80:E113)</f>
         <v>600000</v>
@@ -18156,10 +18156,10 @@
       <c r="S114" s="8"/>
     </row>
     <row r="115" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="301"/>
-      <c r="B115" s="301"/>
-      <c r="C115" s="301"/>
-      <c r="D115" s="302"/>
+      <c r="A115" s="292"/>
+      <c r="B115" s="292"/>
+      <c r="C115" s="292"/>
+      <c r="D115" s="293"/>
       <c r="E115" s="17" t="s">
         <v>61</v>
       </c>
@@ -21341,6 +21341,50 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A16:D17"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="C73:D73"/>
     <mergeCell ref="A114:D115"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A38:A40"/>
@@ -21355,50 +21399,6 @@
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="B92:B95"/>
     <mergeCell ref="A92:A95"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A16:D17"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="73" orientation="portrait" r:id="rId1"/>
@@ -24341,7 +24341,7 @@
   <dimension ref="B2:O21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -24388,7 +24388,7 @@
         <v>179</v>
       </c>
       <c r="F3" s="72">
-        <v>5000</v>
+        <v>55000</v>
       </c>
     </row>
     <row r="4" spans="2:15" x14ac:dyDescent="0.5">
@@ -24403,7 +24403,7 @@
         <v>261</v>
       </c>
       <c r="F4" s="72">
-        <v>1800</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.5">
@@ -24427,7 +24427,7 @@
         <v>444</v>
       </c>
       <c r="F6" s="72">
-        <v>112000</v>
+        <v>62000</v>
       </c>
     </row>
     <row r="7" spans="2:15" x14ac:dyDescent="0.5">
@@ -24519,7 +24519,7 @@
       </c>
       <c r="I14" s="181">
         <f>C19-F19</f>
-        <v>52370</v>
+        <v>52570</v>
       </c>
     </row>
     <row r="15" spans="2:15" x14ac:dyDescent="0.5">
@@ -24575,7 +24575,7 @@
       </c>
       <c r="F19" s="253">
         <f>SUM(F2:F18)</f>
-        <v>1728800</v>
+        <v>1728600</v>
       </c>
       <c r="L19" s="72">
         <v>956</v>
@@ -31789,19 +31789,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="284" t="s">
+      <c r="A1" s="280" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="285"/>
-      <c r="C1" s="285"/>
-      <c r="D1" s="285"/>
-      <c r="E1" s="286"/>
-      <c r="G1" s="282" t="s">
+      <c r="B1" s="281"/>
+      <c r="C1" s="281"/>
+      <c r="D1" s="281"/>
+      <c r="E1" s="282"/>
+      <c r="G1" s="279" t="s">
         <v>429</v>
       </c>
-      <c r="H1" s="282"/>
-      <c r="I1" s="282"/>
-      <c r="J1" s="282"/>
+      <c r="H1" s="279"/>
+      <c r="I1" s="279"/>
+      <c r="J1" s="279"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -31823,18 +31823,18 @@
         <v>4</v>
       </c>
       <c r="F2" s="238"/>
-      <c r="G2" s="283" t="s">
+      <c r="G2" s="274" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="283"/>
-      <c r="I2" s="283"/>
-      <c r="J2" s="283"/>
+      <c r="H2" s="274"/>
+      <c r="I2" s="274"/>
+      <c r="J2" s="274"/>
       <c r="K2" s="238"/>
       <c r="L2" s="238"/>
       <c r="M2" s="238"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A3" s="277">
+      <c r="A3" s="275">
         <v>1</v>
       </c>
       <c r="B3" s="211">
@@ -31846,7 +31846,7 @@
       <c r="D3" s="209">
         <v>30000</v>
       </c>
-      <c r="E3" s="275">
+      <c r="E3" s="277">
         <f>D4-D3</f>
         <v>-30000</v>
       </c>
@@ -31867,11 +31867,11 @@
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A4" s="278"/>
+      <c r="A4" s="276"/>
       <c r="B4" s="213"/>
       <c r="C4" s="214"/>
       <c r="D4" s="210"/>
-      <c r="E4" s="276"/>
+      <c r="E4" s="278"/>
       <c r="G4" s="230">
         <v>1</v>
       </c>
@@ -31907,7 +31907,7 @@
       <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A6" s="277">
+      <c r="A6" s="275">
         <v>2</v>
       </c>
       <c r="B6" s="211">
@@ -31919,7 +31919,7 @@
       <c r="D6" s="209">
         <v>5000</v>
       </c>
-      <c r="E6" s="275">
+      <c r="E6" s="277">
         <f>D7-D6</f>
         <v>-5000</v>
       </c>
@@ -31940,11 +31940,11 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A7" s="278"/>
+      <c r="A7" s="276"/>
       <c r="B7" s="213"/>
       <c r="C7" s="214"/>
       <c r="D7" s="210"/>
-      <c r="E7" s="276"/>
+      <c r="E7" s="278"/>
       <c r="G7" s="230">
         <v>3</v>
       </c>
@@ -31980,7 +31980,7 @@
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A9" s="277">
+      <c r="A9" s="275">
         <v>4</v>
       </c>
       <c r="B9" s="211">
@@ -31992,7 +31992,7 @@
       <c r="D9" s="209">
         <v>3070</v>
       </c>
-      <c r="E9" s="275">
+      <c r="E9" s="277">
         <f>D10-D9</f>
         <v>-3070</v>
       </c>
@@ -32013,11 +32013,11 @@
       <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A10" s="278"/>
+      <c r="A10" s="276"/>
       <c r="B10" s="213"/>
       <c r="C10" s="214"/>
       <c r="D10" s="210"/>
-      <c r="E10" s="276"/>
+      <c r="E10" s="278"/>
       <c r="G10" s="230">
         <v>5</v>
       </c>
@@ -32057,7 +32057,7 @@
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A12" s="277">
+      <c r="A12" s="275">
         <v>5</v>
       </c>
       <c r="B12" s="211">
@@ -32069,7 +32069,7 @@
       <c r="D12" s="209">
         <v>5000</v>
       </c>
-      <c r="E12" s="275">
+      <c r="E12" s="277">
         <f>D13-D12</f>
         <v>-5000</v>
       </c>
@@ -32090,11 +32090,11 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A13" s="278"/>
+      <c r="A13" s="276"/>
       <c r="B13" s="213"/>
       <c r="C13" s="214"/>
       <c r="D13" s="210"/>
-      <c r="E13" s="276"/>
+      <c r="E13" s="278"/>
       <c r="G13" s="1"/>
       <c r="H13" s="233"/>
       <c r="I13" s="1"/>
@@ -32118,7 +32118,7 @@
       <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A15" s="277">
+      <c r="A15" s="275">
         <v>6</v>
       </c>
       <c r="B15" s="211">
@@ -32130,7 +32130,7 @@
       <c r="D15" s="209">
         <v>5000</v>
       </c>
-      <c r="E15" s="275">
+      <c r="E15" s="277">
         <f>D16-D15</f>
         <v>-5000</v>
       </c>
@@ -32143,11 +32143,11 @@
       <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A16" s="278"/>
+      <c r="A16" s="276"/>
       <c r="B16" s="213"/>
       <c r="C16" s="214"/>
       <c r="D16" s="210"/>
-      <c r="E16" s="276"/>
+      <c r="E16" s="278"/>
       <c r="G16" s="1"/>
       <c r="H16" s="234"/>
       <c r="I16" s="1"/>
@@ -32171,7 +32171,7 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A18" s="277">
+      <c r="A18" s="275">
         <v>7</v>
       </c>
       <c r="B18" s="211">
@@ -32183,7 +32183,7 @@
       <c r="D18" s="209">
         <v>5000</v>
       </c>
-      <c r="E18" s="275">
+      <c r="E18" s="277">
         <f>D19-D18</f>
         <v>-5000</v>
       </c>
@@ -32201,11 +32201,11 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A19" s="278"/>
+      <c r="A19" s="276"/>
       <c r="B19" s="213"/>
       <c r="C19" s="214"/>
       <c r="D19" s="210"/>
-      <c r="E19" s="276"/>
+      <c r="E19" s="278"/>
       <c r="G19" s="55"/>
       <c r="H19" s="236"/>
       <c r="I19" s="55"/>
@@ -32220,18 +32220,18 @@
       <c r="C20" s="8"/>
       <c r="D20" s="240"/>
       <c r="E20" s="242"/>
-      <c r="G20" s="283" t="s">
+      <c r="G20" s="274" t="s">
         <v>411</v>
       </c>
-      <c r="H20" s="283"/>
-      <c r="I20" s="283"/>
-      <c r="J20" s="283"/>
+      <c r="H20" s="274"/>
+      <c r="I20" s="274"/>
+      <c r="J20" s="274"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A21" s="277">
+      <c r="A21" s="275">
         <v>8</v>
       </c>
       <c r="B21" s="211">
@@ -32243,7 +32243,7 @@
       <c r="D21" s="209">
         <v>600</v>
       </c>
-      <c r="E21" s="275">
+      <c r="E21" s="277">
         <f>D22-D21</f>
         <v>-600</v>
       </c>
@@ -32264,11 +32264,11 @@
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A22" s="278"/>
+      <c r="A22" s="276"/>
       <c r="B22" s="213"/>
       <c r="C22" s="214"/>
       <c r="D22" s="210"/>
-      <c r="E22" s="276"/>
+      <c r="E22" s="278"/>
       <c r="G22" s="231">
         <v>1</v>
       </c>
@@ -32308,7 +32308,7 @@
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A24" s="277">
+      <c r="A24" s="275">
         <v>9</v>
       </c>
       <c r="B24" s="211">
@@ -32320,7 +32320,7 @@
       <c r="D24" s="209">
         <v>5000</v>
       </c>
-      <c r="E24" s="275">
+      <c r="E24" s="277">
         <f>D25-D24</f>
         <v>-5000</v>
       </c>
@@ -32333,11 +32333,11 @@
       <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A25" s="278"/>
+      <c r="A25" s="276"/>
       <c r="B25" s="213"/>
       <c r="C25" s="214"/>
       <c r="D25" s="210"/>
-      <c r="E25" s="276"/>
+      <c r="E25" s="278"/>
       <c r="G25" s="231"/>
       <c r="H25" s="234"/>
       <c r="I25" s="1"/>
@@ -32361,7 +32361,7 @@
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A27" s="277">
+      <c r="A27" s="275">
         <v>10</v>
       </c>
       <c r="B27" s="211">
@@ -32373,7 +32373,7 @@
       <c r="D27" s="209">
         <v>5000</v>
       </c>
-      <c r="E27" s="275">
+      <c r="E27" s="277">
         <f>D28-D27</f>
         <v>-5000</v>
       </c>
@@ -32386,11 +32386,11 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A28" s="278"/>
+      <c r="A28" s="276"/>
       <c r="B28" s="213"/>
       <c r="C28" s="214"/>
       <c r="D28" s="210"/>
-      <c r="E28" s="276"/>
+      <c r="E28" s="278"/>
       <c r="G28" s="231"/>
       <c r="H28" s="234"/>
       <c r="I28" s="1"/>
@@ -32414,7 +32414,7 @@
       <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A30" s="277">
+      <c r="A30" s="275">
         <v>11</v>
       </c>
       <c r="B30" s="211">
@@ -32426,7 +32426,7 @@
       <c r="D30" s="209">
         <v>5000</v>
       </c>
-      <c r="E30" s="275">
+      <c r="E30" s="277">
         <f>D31-D30</f>
         <v>-5000</v>
       </c>
@@ -32439,11 +32439,11 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A31" s="278"/>
+      <c r="A31" s="276"/>
       <c r="B31" s="213"/>
       <c r="C31" s="214"/>
       <c r="D31" s="210"/>
-      <c r="E31" s="276"/>
+      <c r="E31" s="278"/>
       <c r="G31" s="1"/>
       <c r="H31" s="233"/>
       <c r="I31" s="1"/>
@@ -32467,13 +32467,13 @@
       <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A33" s="277">
+      <c r="A33" s="275">
         <v>12</v>
       </c>
       <c r="B33" s="211"/>
       <c r="C33" s="212"/>
       <c r="D33" s="209"/>
-      <c r="E33" s="275">
+      <c r="E33" s="277">
         <f>D34-D33</f>
         <v>0</v>
       </c>
@@ -32486,11 +32486,11 @@
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A34" s="278"/>
+      <c r="A34" s="276"/>
       <c r="B34" s="213"/>
       <c r="C34" s="214"/>
       <c r="D34" s="210"/>
-      <c r="E34" s="276"/>
+      <c r="E34" s="278"/>
       <c r="G34" s="1"/>
       <c r="H34" s="234"/>
       <c r="I34" s="1"/>
@@ -32514,13 +32514,13 @@
       <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A36" s="277">
+      <c r="A36" s="275">
         <v>13</v>
       </c>
       <c r="B36" s="211"/>
       <c r="C36" s="212"/>
       <c r="D36" s="209"/>
-      <c r="E36" s="275">
+      <c r="E36" s="277">
         <f>D37-D36</f>
         <v>0</v>
       </c>
@@ -32538,11 +32538,11 @@
       <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A37" s="278"/>
+      <c r="A37" s="276"/>
       <c r="B37" s="213"/>
       <c r="C37" s="214"/>
       <c r="D37" s="210"/>
-      <c r="E37" s="276"/>
+      <c r="E37" s="278"/>
       <c r="G37" s="8"/>
       <c r="H37" s="241"/>
       <c r="I37" s="8"/>
@@ -32566,13 +32566,13 @@
       <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A39" s="277">
+      <c r="A39" s="275">
         <v>14</v>
       </c>
       <c r="B39" s="211"/>
       <c r="C39" s="212"/>
       <c r="D39" s="209"/>
-      <c r="E39" s="275">
+      <c r="E39" s="277">
         <f>D40-D39</f>
         <v>0</v>
       </c>
@@ -32585,11 +32585,11 @@
       <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A40" s="278"/>
+      <c r="A40" s="276"/>
       <c r="B40" s="213"/>
       <c r="C40" s="214"/>
       <c r="D40" s="210"/>
-      <c r="E40" s="276"/>
+      <c r="E40" s="278"/>
       <c r="G40" s="8"/>
       <c r="H40" s="241"/>
       <c r="I40" s="8"/>
@@ -32613,13 +32613,13 @@
       <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A42" s="277">
+      <c r="A42" s="275">
         <v>15</v>
       </c>
       <c r="B42" s="211"/>
       <c r="C42" s="212"/>
       <c r="D42" s="209"/>
-      <c r="E42" s="275">
+      <c r="E42" s="277">
         <f>D43-D42</f>
         <v>0</v>
       </c>
@@ -32632,11 +32632,11 @@
       <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A43" s="278"/>
+      <c r="A43" s="276"/>
       <c r="B43" s="213"/>
       <c r="C43" s="214"/>
       <c r="D43" s="210"/>
-      <c r="E43" s="276"/>
+      <c r="E43" s="278"/>
       <c r="G43" s="8"/>
       <c r="H43" s="241"/>
       <c r="I43" s="8"/>
@@ -32660,12 +32660,12 @@
       <c r="M44" s="8"/>
     </row>
     <row r="45" spans="1:13" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="279" t="s">
+      <c r="A45" s="284" t="s">
         <v>412</v>
       </c>
-      <c r="B45" s="280"/>
-      <c r="C45" s="280"/>
-      <c r="D45" s="281"/>
+      <c r="B45" s="285"/>
+      <c r="C45" s="285"/>
+      <c r="D45" s="286"/>
       <c r="E45" s="219">
         <f>SUM(E3:E44)</f>
         <v>-68670</v>
@@ -32682,8 +32682,8 @@
       <c r="A46" s="79"/>
       <c r="B46" s="239"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="274"/>
-      <c r="E46" s="274"/>
+      <c r="D46" s="283"/>
+      <c r="E46" s="283"/>
       <c r="G46" s="8"/>
       <c r="H46" s="241"/>
       <c r="I46" s="8"/>
@@ -32868,17 +32868,15 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G18:I18"/>
@@ -32895,15 +32893,17 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -35731,11 +35731,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A78:I78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="F71:H71"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="A51:C51"/>
@@ -35751,11 +35751,11 @@
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="A78:I78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="F91:H91"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -39589,31 +39589,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A80:I80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F31:H31"/>
     <mergeCell ref="A40:I40"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="F41:I41"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="F55:H55"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A62:I62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="A80:I80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="F91:H91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added Mazhar 18x bwc files 1060k
</commit_message>
<xml_diff>
--- a/Office Statement Expense & Expenditure.xlsx
+++ b/Office Statement Expense & Expenditure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Najeeb Associates\000FFICE\Office Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0DE22BB-6E41-49E4-88A7-A3788C06556F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0941E80C-DC06-4100-8D64-5AC2C603EDF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="904" activeTab="15" xr2:uid="{B2A19E3B-6786-4ED5-96A6-D1A6BAD18668}"/>
   </bookViews>
@@ -204,8 +204,34 @@
 </comments>
 </file>
 
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Azan Laptop Store</author>
+  </authors>
+  <commentList>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{1020D6EC-431A-4CE8-A22E-FDEEA83BCE3F}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Mazhar Purchased per file 81k Total: 14,58,000/=
+The current market rate is 59k
+Total Amount comes to be: 10,62,000/=</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="936" uniqueCount="447">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="943" uniqueCount="452">
   <si>
     <t>Opning Balance</t>
   </si>
@@ -1546,6 +1572,21 @@
   </si>
   <si>
     <t>Sunny Goind Home - Gave me 209k + 3x 7 marla files yesterday</t>
+  </si>
+  <si>
+    <t>Tea For Guest</t>
+  </si>
+  <si>
+    <t>Received 18x BWC Files at G16 Home - Time 10:00 pm night</t>
+  </si>
+  <si>
+    <t>Received Cash from Mazhar with files</t>
+  </si>
+  <si>
+    <t>Mazhar gave cash</t>
+  </si>
+  <si>
+    <t>18x 7marla old files</t>
   </si>
 </sst>
 </file>
@@ -2228,7 +2269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="318">
+  <cellXfs count="319">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2907,6 +2948,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3394,8 +3438,8 @@
   </sheetPr>
   <dimension ref="A1:N895"/>
   <sheetViews>
-    <sheetView topLeftCell="A146" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D160" sqref="D160"/>
+    <sheetView topLeftCell="A140" zoomScale="133" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="H154" sqref="H154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -3412,17 +3456,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
@@ -3430,19 +3474,19 @@
       <c r="N1" s="8"/>
     </row>
     <row r="2" spans="1:14" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -4168,21 +4212,21 @@
       <c r="N33" s="8"/>
     </row>
     <row r="34" spans="1:14" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A34" s="268" t="s">
+      <c r="A34" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B34" s="269"/>
-      <c r="C34" s="269"/>
+      <c r="B34" s="270"/>
+      <c r="C34" s="270"/>
       <c r="D34" s="44">
         <f>SUM(D4:D33)</f>
         <v>457640</v>
       </c>
       <c r="E34" s="50"/>
-      <c r="F34" s="268" t="s">
+      <c r="F34" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G34" s="269"/>
-      <c r="H34" s="270"/>
+      <c r="G34" s="270"/>
+      <c r="H34" s="271"/>
       <c r="I34" s="44">
         <f>SUM(I4:I33)</f>
         <v>175535</v>
@@ -4305,17 +4349,17 @@
       <c r="N40" s="8"/>
     </row>
     <row r="41" spans="1:14" ht="34.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A41" s="262" t="s">
+      <c r="A41" s="263" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="263"/>
-      <c r="C41" s="263"/>
-      <c r="D41" s="263"/>
-      <c r="E41" s="263"/>
-      <c r="F41" s="263"/>
-      <c r="G41" s="263"/>
-      <c r="H41" s="263"/>
-      <c r="I41" s="264"/>
+      <c r="B41" s="264"/>
+      <c r="C41" s="264"/>
+      <c r="D41" s="264"/>
+      <c r="E41" s="264"/>
+      <c r="F41" s="264"/>
+      <c r="G41" s="264"/>
+      <c r="H41" s="264"/>
+      <c r="I41" s="265"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
@@ -4323,19 +4367,19 @@
       <c r="N41" s="8"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A42" s="265" t="s">
+      <c r="A42" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B42" s="266"/>
-      <c r="C42" s="266"/>
-      <c r="D42" s="267"/>
+      <c r="B42" s="267"/>
+      <c r="C42" s="267"/>
+      <c r="D42" s="268"/>
       <c r="E42" s="43"/>
-      <c r="F42" s="265" t="s">
+      <c r="F42" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G42" s="266"/>
-      <c r="H42" s="266"/>
-      <c r="I42" s="267"/>
+      <c r="G42" s="267"/>
+      <c r="H42" s="267"/>
+      <c r="I42" s="268"/>
       <c r="J42" s="8"/>
       <c r="K42" s="8"/>
       <c r="L42" s="8"/>
@@ -4664,21 +4708,21 @@
       <c r="N55" s="8"/>
     </row>
     <row r="56" spans="1:14" ht="17.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A56" s="268" t="s">
+      <c r="A56" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B56" s="269"/>
-      <c r="C56" s="269"/>
+      <c r="B56" s="270"/>
+      <c r="C56" s="270"/>
       <c r="D56" s="44">
         <f>SUM(D44:D55)</f>
         <v>302105</v>
       </c>
       <c r="E56" s="50"/>
-      <c r="F56" s="268" t="s">
+      <c r="F56" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G56" s="269"/>
-      <c r="H56" s="270"/>
+      <c r="G56" s="270"/>
+      <c r="H56" s="271"/>
       <c r="I56" s="44">
         <f>SUM(I44:I55)</f>
         <v>8700</v>
@@ -4785,15 +4829,15 @@
       <c r="N61" s="8"/>
     </row>
     <row r="62" spans="1:14" ht="70" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="271"/>
-      <c r="B62" s="271"/>
-      <c r="C62" s="271"/>
-      <c r="D62" s="271"/>
-      <c r="E62" s="271"/>
-      <c r="F62" s="271"/>
-      <c r="G62" s="271"/>
-      <c r="H62" s="271"/>
-      <c r="I62" s="271"/>
+      <c r="A62" s="272"/>
+      <c r="B62" s="272"/>
+      <c r="C62" s="272"/>
+      <c r="D62" s="272"/>
+      <c r="E62" s="272"/>
+      <c r="F62" s="272"/>
+      <c r="G62" s="272"/>
+      <c r="H62" s="272"/>
+      <c r="I62" s="272"/>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
@@ -4801,17 +4845,17 @@
       <c r="N62" s="8"/>
     </row>
     <row r="63" spans="1:14" ht="34.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A63" s="262" t="s">
+      <c r="A63" s="263" t="s">
         <v>185</v>
       </c>
-      <c r="B63" s="263"/>
-      <c r="C63" s="263"/>
-      <c r="D63" s="263"/>
-      <c r="E63" s="263"/>
-      <c r="F63" s="263"/>
-      <c r="G63" s="263"/>
-      <c r="H63" s="263"/>
-      <c r="I63" s="264"/>
+      <c r="B63" s="264"/>
+      <c r="C63" s="264"/>
+      <c r="D63" s="264"/>
+      <c r="E63" s="264"/>
+      <c r="F63" s="264"/>
+      <c r="G63" s="264"/>
+      <c r="H63" s="264"/>
+      <c r="I63" s="265"/>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
@@ -4819,19 +4863,19 @@
       <c r="N63" s="8"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A64" s="265" t="s">
+      <c r="A64" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B64" s="266"/>
-      <c r="C64" s="266"/>
-      <c r="D64" s="267"/>
+      <c r="B64" s="267"/>
+      <c r="C64" s="267"/>
+      <c r="D64" s="268"/>
       <c r="E64" s="43"/>
-      <c r="F64" s="265" t="s">
+      <c r="F64" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G64" s="266"/>
-      <c r="H64" s="266"/>
-      <c r="I64" s="267"/>
+      <c r="G64" s="267"/>
+      <c r="H64" s="267"/>
+      <c r="I64" s="268"/>
       <c r="J64" s="8"/>
       <c r="K64" s="8"/>
       <c r="L64" s="8"/>
@@ -5192,21 +5236,21 @@
       <c r="N78" s="8"/>
     </row>
     <row r="79" spans="1:14" ht="18.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A79" s="268" t="s">
+      <c r="A79" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B79" s="269"/>
-      <c r="C79" s="269"/>
+      <c r="B79" s="270"/>
+      <c r="C79" s="270"/>
       <c r="D79" s="44">
         <f>SUM(D66:D78)</f>
         <v>658405</v>
       </c>
       <c r="E79" s="50"/>
-      <c r="F79" s="268" t="s">
+      <c r="F79" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G79" s="269"/>
-      <c r="H79" s="270"/>
+      <c r="G79" s="270"/>
+      <c r="H79" s="271"/>
       <c r="I79" s="44">
         <f>SUM(I66:I78)</f>
         <v>73560</v>
@@ -5329,17 +5373,17 @@
       <c r="N85" s="8"/>
     </row>
     <row r="86" spans="1:14" ht="37" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A86" s="262" t="s">
+      <c r="A86" s="263" t="s">
         <v>282</v>
       </c>
-      <c r="B86" s="263"/>
-      <c r="C86" s="263"/>
-      <c r="D86" s="263"/>
-      <c r="E86" s="263"/>
-      <c r="F86" s="263"/>
-      <c r="G86" s="263"/>
-      <c r="H86" s="263"/>
-      <c r="I86" s="264"/>
+      <c r="B86" s="264"/>
+      <c r="C86" s="264"/>
+      <c r="D86" s="264"/>
+      <c r="E86" s="264"/>
+      <c r="F86" s="264"/>
+      <c r="G86" s="264"/>
+      <c r="H86" s="264"/>
+      <c r="I86" s="265"/>
       <c r="J86" s="8"/>
       <c r="K86" s="8"/>
       <c r="L86" s="8"/>
@@ -5347,19 +5391,19 @@
       <c r="N86" s="8"/>
     </row>
     <row r="87" spans="1:14" ht="18" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A87" s="265" t="s">
+      <c r="A87" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B87" s="266"/>
-      <c r="C87" s="266"/>
-      <c r="D87" s="267"/>
+      <c r="B87" s="267"/>
+      <c r="C87" s="267"/>
+      <c r="D87" s="268"/>
       <c r="E87" s="43"/>
-      <c r="F87" s="265" t="s">
+      <c r="F87" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G87" s="266"/>
-      <c r="H87" s="266"/>
-      <c r="I87" s="267"/>
+      <c r="G87" s="267"/>
+      <c r="H87" s="267"/>
+      <c r="I87" s="268"/>
       <c r="J87" s="8"/>
       <c r="K87" s="8"/>
       <c r="L87" s="8"/>
@@ -5798,21 +5842,21 @@
       <c r="N104" s="8"/>
     </row>
     <row r="105" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A105" s="268" t="s">
+      <c r="A105" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B105" s="269"/>
-      <c r="C105" s="269"/>
+      <c r="B105" s="270"/>
+      <c r="C105" s="270"/>
       <c r="D105" s="44">
         <f>SUM(D89:D104)</f>
         <v>935345</v>
       </c>
       <c r="E105" s="50"/>
-      <c r="F105" s="268" t="s">
+      <c r="F105" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G105" s="269"/>
-      <c r="H105" s="270"/>
+      <c r="G105" s="270"/>
+      <c r="H105" s="271"/>
       <c r="I105" s="44">
         <f>SUM(I89:I104)</f>
         <v>14647</v>
@@ -5935,17 +5979,17 @@
       <c r="N111" s="8"/>
     </row>
     <row r="112" spans="1:14" ht="29.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A112" s="262" t="s">
+      <c r="A112" s="263" t="s">
         <v>347</v>
       </c>
-      <c r="B112" s="263"/>
-      <c r="C112" s="263"/>
-      <c r="D112" s="263"/>
-      <c r="E112" s="263"/>
-      <c r="F112" s="263"/>
-      <c r="G112" s="263"/>
-      <c r="H112" s="263"/>
-      <c r="I112" s="264"/>
+      <c r="B112" s="264"/>
+      <c r="C112" s="264"/>
+      <c r="D112" s="264"/>
+      <c r="E112" s="264"/>
+      <c r="F112" s="264"/>
+      <c r="G112" s="264"/>
+      <c r="H112" s="264"/>
+      <c r="I112" s="265"/>
       <c r="J112" s="8"/>
       <c r="K112" s="8"/>
       <c r="L112" s="8"/>
@@ -5953,19 +5997,19 @@
       <c r="N112" s="8"/>
     </row>
     <row r="113" spans="1:14" ht="19.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A113" s="265" t="s">
+      <c r="A113" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B113" s="266"/>
-      <c r="C113" s="266"/>
-      <c r="D113" s="267"/>
+      <c r="B113" s="267"/>
+      <c r="C113" s="267"/>
+      <c r="D113" s="268"/>
       <c r="E113" s="43"/>
-      <c r="F113" s="265" t="s">
+      <c r="F113" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G113" s="266"/>
-      <c r="H113" s="266"/>
-      <c r="I113" s="267"/>
+      <c r="G113" s="267"/>
+      <c r="H113" s="267"/>
+      <c r="I113" s="268"/>
       <c r="J113" s="8"/>
       <c r="K113" s="8"/>
       <c r="L113" s="8"/>
@@ -6474,21 +6518,21 @@
       <c r="N132" s="8"/>
     </row>
     <row r="133" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A133" s="268" t="s">
+      <c r="A133" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B133" s="269"/>
-      <c r="C133" s="269"/>
+      <c r="B133" s="270"/>
+      <c r="C133" s="270"/>
       <c r="D133" s="44">
         <f>SUM(D115:D132)</f>
         <v>1433998</v>
       </c>
       <c r="E133" s="50"/>
-      <c r="F133" s="268" t="s">
+      <c r="F133" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G133" s="269"/>
-      <c r="H133" s="270"/>
+      <c r="G133" s="270"/>
+      <c r="H133" s="271"/>
       <c r="I133" s="44">
         <f>SUM(I115:I132)</f>
         <v>2100</v>
@@ -6611,17 +6655,17 @@
       <c r="N139" s="8"/>
     </row>
     <row r="140" spans="1:14" ht="36.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A140" s="262" t="s">
+      <c r="A140" s="263" t="s">
         <v>396</v>
       </c>
-      <c r="B140" s="263"/>
-      <c r="C140" s="263"/>
-      <c r="D140" s="263"/>
-      <c r="E140" s="263"/>
-      <c r="F140" s="263"/>
-      <c r="G140" s="263"/>
-      <c r="H140" s="263"/>
-      <c r="I140" s="264"/>
+      <c r="B140" s="264"/>
+      <c r="C140" s="264"/>
+      <c r="D140" s="264"/>
+      <c r="E140" s="264"/>
+      <c r="F140" s="264"/>
+      <c r="G140" s="264"/>
+      <c r="H140" s="264"/>
+      <c r="I140" s="265"/>
       <c r="J140" s="8"/>
       <c r="K140" s="8"/>
       <c r="L140" s="8"/>
@@ -6629,19 +6673,19 @@
       <c r="N140" s="8"/>
     </row>
     <row r="141" spans="1:14" ht="19.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A141" s="265" t="s">
+      <c r="A141" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B141" s="266"/>
-      <c r="C141" s="266"/>
-      <c r="D141" s="267"/>
+      <c r="B141" s="267"/>
+      <c r="C141" s="267"/>
+      <c r="D141" s="268"/>
       <c r="E141" s="43"/>
-      <c r="F141" s="265" t="s">
+      <c r="F141" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G141" s="266"/>
-      <c r="H141" s="266"/>
-      <c r="I141" s="267"/>
+      <c r="G141" s="267"/>
+      <c r="H141" s="267"/>
+      <c r="I141" s="268"/>
       <c r="J141" s="8"/>
       <c r="K141" s="8"/>
       <c r="L141" s="8"/>
@@ -6894,8 +6938,12 @@
       <c r="N149" s="8"/>
     </row>
     <row r="150" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A150" s="226"/>
-      <c r="B150" s="39"/>
+      <c r="A150" s="226">
+        <v>6</v>
+      </c>
+      <c r="B150" s="39">
+        <v>44279</v>
+      </c>
       <c r="C150" s="1"/>
       <c r="D150" s="40"/>
       <c r="E150" s="38"/>
@@ -7121,10 +7169,18 @@
       <c r="C160" s="70"/>
       <c r="D160" s="71"/>
       <c r="E160" s="38"/>
-      <c r="F160" s="174"/>
-      <c r="G160" s="175"/>
-      <c r="H160" s="70"/>
-      <c r="I160" s="71"/>
+      <c r="F160" s="174">
+        <v>13</v>
+      </c>
+      <c r="G160" s="39">
+        <v>44278</v>
+      </c>
+      <c r="H160" s="70" t="s">
+        <v>447</v>
+      </c>
+      <c r="I160" s="71">
+        <v>120</v>
+      </c>
       <c r="J160" s="8"/>
       <c r="K160" s="8"/>
       <c r="L160" s="8"/>
@@ -7164,24 +7220,24 @@
       <c r="N162" s="8"/>
     </row>
     <row r="163" spans="1:14" x14ac:dyDescent="0.5">
-      <c r="A163" s="268" t="s">
+      <c r="A163" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B163" s="269"/>
-      <c r="C163" s="269"/>
+      <c r="B163" s="270"/>
+      <c r="C163" s="270"/>
       <c r="D163" s="44">
         <f>SUM(D143:D162)</f>
         <v>1449298</v>
       </c>
       <c r="E163" s="50"/>
-      <c r="F163" s="268" t="s">
+      <c r="F163" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G163" s="269"/>
-      <c r="H163" s="270"/>
+      <c r="G163" s="270"/>
+      <c r="H163" s="271"/>
       <c r="I163" s="44">
         <f>SUM(I143:I162)</f>
-        <v>1699</v>
+        <v>1819</v>
       </c>
       <c r="J163" s="8"/>
       <c r="K163" s="8"/>
@@ -7234,7 +7290,7 @@
       </c>
       <c r="D166" s="58">
         <f>I163</f>
-        <v>1699</v>
+        <v>1819</v>
       </c>
       <c r="E166" s="8"/>
       <c r="F166" s="53"/>
@@ -7271,7 +7327,7 @@
       </c>
       <c r="D168" s="62">
         <f>D165-D166</f>
-        <v>1447599</v>
+        <v>1447479</v>
       </c>
       <c r="E168" s="8"/>
       <c r="F168" s="8"/>
@@ -14803,18 +14859,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="303" t="s">
+      <c r="A1" s="304" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="304"/>
-      <c r="C1" s="304"/>
+      <c r="B1" s="305"/>
+      <c r="C1" s="305"/>
       <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="305" t="s">
+      <c r="E1" s="306" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="305"/>
+      <c r="F1" s="306"/>
       <c r="G1" s="14">
         <v>50000</v>
       </c>
@@ -14933,17 +14989,17 @@
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A5" s="308">
+      <c r="A5" s="309">
         <v>3</v>
       </c>
-      <c r="B5" s="309">
+      <c r="B5" s="310">
         <v>44063</v>
       </c>
-      <c r="C5" s="310" t="s">
+      <c r="C5" s="311" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="311"/>
-      <c r="E5" s="312"/>
+      <c r="D5" s="312"/>
+      <c r="E5" s="313"/>
       <c r="F5" s="4">
         <v>11640</v>
       </c>
@@ -14965,11 +15021,11 @@
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A6" s="308"/>
-      <c r="B6" s="309"/>
-      <c r="C6" s="310"/>
-      <c r="D6" s="311"/>
-      <c r="E6" s="312"/>
+      <c r="A6" s="309"/>
+      <c r="B6" s="310"/>
+      <c r="C6" s="311"/>
+      <c r="D6" s="312"/>
+      <c r="E6" s="313"/>
       <c r="F6" s="4">
         <v>1700</v>
       </c>
@@ -14991,10 +15047,10 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A7" s="308">
+      <c r="A7" s="309">
         <v>4</v>
       </c>
-      <c r="B7" s="309">
+      <c r="B7" s="310">
         <v>44064</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -15023,8 +15079,8 @@
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A8" s="308"/>
-      <c r="B8" s="309"/>
+      <c r="A8" s="309"/>
+      <c r="B8" s="310"/>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -15085,10 +15141,10 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A10" s="308">
+      <c r="A10" s="309">
         <v>6</v>
       </c>
-      <c r="B10" s="309">
+      <c r="B10" s="310">
         <v>44066</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -15117,8 +15173,8 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A11" s="308"/>
-      <c r="B11" s="309"/>
+      <c r="A11" s="309"/>
+      <c r="B11" s="310"/>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
@@ -15150,7 +15206,7 @@
       <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="309">
+      <c r="B12" s="310">
         <v>44067</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -15182,7 +15238,7 @@
       <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="B13" s="309"/>
+      <c r="B13" s="310"/>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
@@ -15275,12 +15331,12 @@
       <c r="S15" s="8"/>
     </row>
     <row r="16" spans="1:19" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="290" t="s">
+      <c r="A16" s="291" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="290"/>
-      <c r="C16" s="290"/>
-      <c r="D16" s="291"/>
+      <c r="B16" s="291"/>
+      <c r="C16" s="291"/>
+      <c r="D16" s="292"/>
       <c r="E16" s="16">
         <f>SUM(E3:E15)</f>
         <v>0</v>
@@ -15307,10 +15363,10 @@
       <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="292"/>
-      <c r="B17" s="292"/>
-      <c r="C17" s="292"/>
-      <c r="D17" s="293"/>
+      <c r="A17" s="293"/>
+      <c r="B17" s="293"/>
+      <c r="C17" s="293"/>
+      <c r="D17" s="294"/>
       <c r="E17" s="17" t="s">
         <v>61</v>
       </c>
@@ -15355,18 +15411,18 @@
       <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="303" t="s">
+      <c r="A19" s="304" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="304"/>
-      <c r="C19" s="304"/>
+      <c r="B19" s="305"/>
+      <c r="C19" s="305"/>
       <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="305" t="s">
+      <c r="E19" s="306" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="305"/>
+      <c r="F19" s="306"/>
       <c r="G19" s="14">
         <v>31780</v>
       </c>
@@ -15451,10 +15507,10 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A22" s="297">
+      <c r="A22" s="298">
         <v>12</v>
       </c>
-      <c r="B22" s="294">
+      <c r="B22" s="295">
         <v>44076</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -15483,8 +15539,8 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A23" s="298"/>
-      <c r="B23" s="295"/>
+      <c r="A23" s="299"/>
+      <c r="B23" s="296"/>
       <c r="C23" s="21" t="s">
         <v>21</v>
       </c>
@@ -15511,8 +15567,8 @@
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A24" s="299"/>
-      <c r="B24" s="296"/>
+      <c r="A24" s="300"/>
+      <c r="B24" s="297"/>
       <c r="C24" s="21" t="s">
         <v>22</v>
       </c>
@@ -15541,10 +15597,10 @@
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A25" s="297">
+      <c r="A25" s="298">
         <v>13</v>
       </c>
-      <c r="B25" s="294">
+      <c r="B25" s="295">
         <v>44077</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -15575,8 +15631,8 @@
       <c r="S25" s="8"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A26" s="299"/>
-      <c r="B26" s="296"/>
+      <c r="A26" s="300"/>
+      <c r="B26" s="297"/>
       <c r="C26" s="21" t="s">
         <v>26</v>
       </c>
@@ -15605,10 +15661,10 @@
       <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A27" s="297">
+      <c r="A27" s="298">
         <v>14</v>
       </c>
-      <c r="B27" s="294">
+      <c r="B27" s="295">
         <v>44078</v>
       </c>
       <c r="C27" s="21" t="s">
@@ -15637,8 +15693,8 @@
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A28" s="299"/>
-      <c r="B28" s="296"/>
+      <c r="A28" s="300"/>
+      <c r="B28" s="297"/>
       <c r="C28" s="21" t="s">
         <v>28</v>
       </c>
@@ -15667,10 +15723,10 @@
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A29" s="297">
+      <c r="A29" s="298">
         <v>15</v>
       </c>
-      <c r="B29" s="294">
+      <c r="B29" s="295">
         <v>44079</v>
       </c>
       <c r="C29" s="21" t="s">
@@ -15699,8 +15755,8 @@
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A30" s="298"/>
-      <c r="B30" s="295"/>
+      <c r="A30" s="299"/>
+      <c r="B30" s="296"/>
       <c r="C30" s="21" t="s">
         <v>30</v>
       </c>
@@ -15729,8 +15785,8 @@
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A31" s="298"/>
-      <c r="B31" s="295"/>
+      <c r="A31" s="299"/>
+      <c r="B31" s="296"/>
       <c r="C31" s="21" t="s">
         <v>60</v>
       </c>
@@ -15757,8 +15813,8 @@
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A32" s="299"/>
-      <c r="B32" s="296"/>
+      <c r="A32" s="300"/>
+      <c r="B32" s="297"/>
       <c r="C32" s="23" t="s">
         <v>31</v>
       </c>
@@ -15785,10 +15841,10 @@
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A33" s="297">
+      <c r="A33" s="298">
         <v>16</v>
       </c>
-      <c r="B33" s="294">
+      <c r="B33" s="295">
         <v>44080</v>
       </c>
       <c r="C33" s="21" t="s">
@@ -15819,8 +15875,8 @@
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A34" s="298"/>
-      <c r="B34" s="295"/>
+      <c r="A34" s="299"/>
+      <c r="B34" s="296"/>
       <c r="C34" s="21" t="s">
         <v>33</v>
       </c>
@@ -15849,8 +15905,8 @@
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A35" s="298"/>
-      <c r="B35" s="295"/>
+      <c r="A35" s="299"/>
+      <c r="B35" s="296"/>
       <c r="C35" s="21" t="s">
         <v>36</v>
       </c>
@@ -15879,8 +15935,8 @@
       <c r="S35" s="8"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A36" s="298"/>
-      <c r="B36" s="295"/>
+      <c r="A36" s="299"/>
+      <c r="B36" s="296"/>
       <c r="C36" s="21" t="s">
         <v>37</v>
       </c>
@@ -15909,8 +15965,8 @@
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A37" s="299"/>
-      <c r="B37" s="296"/>
+      <c r="A37" s="300"/>
+      <c r="B37" s="297"/>
       <c r="C37" s="21" t="s">
         <v>39</v>
       </c>
@@ -15937,10 +15993,10 @@
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A38" s="297">
+      <c r="A38" s="298">
         <v>17</v>
       </c>
-      <c r="B38" s="294">
+      <c r="B38" s="295">
         <v>44081</v>
       </c>
       <c r="C38" s="21" t="s">
@@ -15969,8 +16025,8 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A39" s="298"/>
-      <c r="B39" s="295"/>
+      <c r="A39" s="299"/>
+      <c r="B39" s="296"/>
       <c r="C39" s="21" t="s">
         <v>28</v>
       </c>
@@ -15997,8 +16053,8 @@
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A40" s="299"/>
-      <c r="B40" s="296"/>
+      <c r="A40" s="300"/>
+      <c r="B40" s="297"/>
       <c r="C40" s="21" t="s">
         <v>40</v>
       </c>
@@ -16027,10 +16083,10 @@
       <c r="S40" s="8"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A41" s="297">
+      <c r="A41" s="298">
         <v>18</v>
       </c>
-      <c r="B41" s="294">
+      <c r="B41" s="295">
         <v>44082</v>
       </c>
       <c r="C41" s="21" t="s">
@@ -16059,8 +16115,8 @@
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A42" s="299"/>
-      <c r="B42" s="296"/>
+      <c r="A42" s="300"/>
+      <c r="B42" s="297"/>
       <c r="C42" s="21" t="s">
         <v>42</v>
       </c>
@@ -16087,10 +16143,10 @@
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A43" s="297">
+      <c r="A43" s="298">
         <v>19</v>
       </c>
-      <c r="B43" s="294">
+      <c r="B43" s="295">
         <v>44083</v>
       </c>
       <c r="C43" s="21" t="s">
@@ -16119,8 +16175,8 @@
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A44" s="299"/>
-      <c r="B44" s="296"/>
+      <c r="A44" s="300"/>
+      <c r="B44" s="297"/>
       <c r="C44" s="21" t="s">
         <v>44</v>
       </c>
@@ -16147,10 +16203,10 @@
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A45" s="297">
+      <c r="A45" s="298">
         <v>20</v>
       </c>
-      <c r="B45" s="294">
+      <c r="B45" s="295">
         <v>44084</v>
       </c>
       <c r="C45" s="21" t="s">
@@ -16179,8 +16235,8 @@
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A46" s="299"/>
-      <c r="B46" s="296"/>
+      <c r="A46" s="300"/>
+      <c r="B46" s="297"/>
       <c r="C46" s="21" t="s">
         <v>45</v>
       </c>
@@ -16207,10 +16263,10 @@
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A47" s="297">
+      <c r="A47" s="298">
         <v>21</v>
       </c>
-      <c r="B47" s="294">
+      <c r="B47" s="295">
         <v>44085</v>
       </c>
       <c r="C47" s="21" t="s">
@@ -16239,8 +16295,8 @@
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A48" s="298"/>
-      <c r="B48" s="295"/>
+      <c r="A48" s="299"/>
+      <c r="B48" s="296"/>
       <c r="C48" s="21" t="s">
         <v>46</v>
       </c>
@@ -16267,8 +16323,8 @@
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A49" s="298"/>
-      <c r="B49" s="295"/>
+      <c r="A49" s="299"/>
+      <c r="B49" s="296"/>
       <c r="C49" s="21" t="s">
         <v>47</v>
       </c>
@@ -16295,8 +16351,8 @@
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A50" s="298"/>
-      <c r="B50" s="295"/>
+      <c r="A50" s="299"/>
+      <c r="B50" s="296"/>
       <c r="C50" s="23" t="s">
         <v>31</v>
       </c>
@@ -16323,8 +16379,8 @@
       <c r="S50" s="8"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A51" s="299"/>
-      <c r="B51" s="296"/>
+      <c r="A51" s="300"/>
+      <c r="B51" s="297"/>
       <c r="C51" s="21" t="s">
         <v>44</v>
       </c>
@@ -16353,10 +16409,10 @@
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A52" s="297">
+      <c r="A52" s="298">
         <v>22</v>
       </c>
-      <c r="B52" s="294">
+      <c r="B52" s="295">
         <v>44086</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -16387,8 +16443,8 @@
       <c r="S52" s="8"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A53" s="299"/>
-      <c r="B53" s="296"/>
+      <c r="A53" s="300"/>
+      <c r="B53" s="297"/>
       <c r="C53" s="21" t="s">
         <v>50</v>
       </c>
@@ -16415,10 +16471,10 @@
       <c r="S53" s="8"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A54" s="297">
+      <c r="A54" s="298">
         <v>23</v>
       </c>
-      <c r="B54" s="294">
+      <c r="B54" s="295">
         <v>44087</v>
       </c>
       <c r="C54" s="21" t="s">
@@ -16447,8 +16503,8 @@
       <c r="S54" s="8"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A55" s="298"/>
-      <c r="B55" s="295"/>
+      <c r="A55" s="299"/>
+      <c r="B55" s="296"/>
       <c r="C55" s="21" t="s">
         <v>28</v>
       </c>
@@ -16475,8 +16531,8 @@
       <c r="S55" s="8"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A56" s="298"/>
-      <c r="B56" s="295"/>
+      <c r="A56" s="299"/>
+      <c r="B56" s="296"/>
       <c r="C56" s="21" t="s">
         <v>51</v>
       </c>
@@ -16503,8 +16559,8 @@
       <c r="S56" s="8"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A57" s="298"/>
-      <c r="B57" s="295"/>
+      <c r="A57" s="299"/>
+      <c r="B57" s="296"/>
       <c r="C57" s="23" t="s">
         <v>31</v>
       </c>
@@ -16629,10 +16685,10 @@
       <c r="S60" s="8"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A61" s="297">
+      <c r="A61" s="298">
         <v>27</v>
       </c>
-      <c r="B61" s="294">
+      <c r="B61" s="295">
         <v>44091</v>
       </c>
       <c r="C61" s="21" t="s">
@@ -16661,8 +16717,8 @@
       <c r="S61" s="8"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A62" s="299"/>
-      <c r="B62" s="296"/>
+      <c r="A62" s="300"/>
+      <c r="B62" s="297"/>
       <c r="C62" s="21" t="s">
         <v>44</v>
       </c>
@@ -16721,10 +16777,10 @@
       <c r="S63" s="8"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A64" s="297">
+      <c r="A64" s="298">
         <v>29</v>
       </c>
-      <c r="B64" s="294">
+      <c r="B64" s="295">
         <v>44093</v>
       </c>
       <c r="C64" s="21" t="s">
@@ -16753,8 +16809,8 @@
       <c r="S64" s="8"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A65" s="299"/>
-      <c r="B65" s="296"/>
+      <c r="A65" s="300"/>
+      <c r="B65" s="297"/>
       <c r="C65" s="21" t="s">
         <v>18</v>
       </c>
@@ -16949,10 +17005,10 @@
       <c r="B71" s="28">
         <v>44101</v>
       </c>
-      <c r="C71" s="306" t="s">
+      <c r="C71" s="307" t="s">
         <v>65</v>
       </c>
-      <c r="D71" s="307"/>
+      <c r="D71" s="308"/>
       <c r="E71" s="26">
         <v>0</v>
       </c>
@@ -16977,10 +17033,10 @@
       <c r="S71" s="8"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A72" s="297">
+      <c r="A72" s="298">
         <v>37</v>
       </c>
-      <c r="B72" s="294">
+      <c r="B72" s="295">
         <v>44103</v>
       </c>
       <c r="C72" s="21" t="s">
@@ -17009,12 +17065,12 @@
       <c r="S72" s="8"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A73" s="299"/>
-      <c r="B73" s="296"/>
-      <c r="C73" s="306" t="s">
+      <c r="A73" s="300"/>
+      <c r="B73" s="297"/>
+      <c r="C73" s="307" t="s">
         <v>75</v>
       </c>
-      <c r="D73" s="307"/>
+      <c r="D73" s="308"/>
       <c r="E73" s="6">
         <v>100000</v>
       </c>
@@ -17071,12 +17127,12 @@
       <c r="S74" s="8"/>
     </row>
     <row r="75" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A75" s="290" t="s">
+      <c r="A75" s="291" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="290"/>
-      <c r="C75" s="290"/>
-      <c r="D75" s="291"/>
+      <c r="B75" s="291"/>
+      <c r="C75" s="291"/>
+      <c r="D75" s="292"/>
       <c r="E75" s="16">
         <f>SUM(E21:E74)</f>
         <v>132000</v>
@@ -17103,10 +17159,10 @@
       <c r="S75" s="8"/>
     </row>
     <row r="76" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="292"/>
-      <c r="B76" s="292"/>
-      <c r="C76" s="292"/>
-      <c r="D76" s="293"/>
+      <c r="A76" s="293"/>
+      <c r="B76" s="293"/>
+      <c r="C76" s="293"/>
+      <c r="D76" s="294"/>
       <c r="E76" s="17" t="s">
         <v>61</v>
       </c>
@@ -17151,18 +17207,18 @@
       <c r="S77" s="8"/>
     </row>
     <row r="78" spans="1:19" ht="27.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="303" t="s">
+      <c r="A78" s="304" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="304"/>
-      <c r="C78" s="304"/>
+      <c r="B78" s="305"/>
+      <c r="C78" s="305"/>
       <c r="D78" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E78" s="305" t="s">
+      <c r="E78" s="306" t="s">
         <v>0</v>
       </c>
-      <c r="F78" s="305"/>
+      <c r="F78" s="306"/>
       <c r="G78" s="14">
         <f>G75</f>
         <v>137640</v>
@@ -17216,10 +17272,10 @@
       <c r="S79" s="8"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A80" s="297">
+      <c r="A80" s="298">
         <v>39</v>
       </c>
-      <c r="B80" s="294">
+      <c r="B80" s="295">
         <v>44105</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -17248,8 +17304,8 @@
       <c r="S80" s="8"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A81" s="298"/>
-      <c r="B81" s="295"/>
+      <c r="A81" s="299"/>
+      <c r="B81" s="296"/>
       <c r="C81" s="1" t="s">
         <v>70</v>
       </c>
@@ -17276,8 +17332,8 @@
       <c r="S81" s="8"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A82" s="298"/>
-      <c r="B82" s="295"/>
+      <c r="A82" s="299"/>
+      <c r="B82" s="296"/>
       <c r="C82" s="34" t="s">
         <v>76</v>
       </c>
@@ -17306,9 +17362,9 @@
       <c r="S82" s="8"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A83" s="298"/>
-      <c r="B83" s="295"/>
-      <c r="C83" s="300" t="s">
+      <c r="A83" s="299"/>
+      <c r="B83" s="296"/>
+      <c r="C83" s="301" t="s">
         <v>77</v>
       </c>
       <c r="D83" s="32" t="s">
@@ -17336,9 +17392,9 @@
       <c r="S83" s="8"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A84" s="298"/>
-      <c r="B84" s="295"/>
-      <c r="C84" s="301"/>
+      <c r="A84" s="299"/>
+      <c r="B84" s="296"/>
+      <c r="C84" s="302"/>
       <c r="D84" s="32" t="s">
         <v>71</v>
       </c>
@@ -17364,9 +17420,9 @@
       <c r="S84" s="8"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A85" s="298"/>
-      <c r="B85" s="295"/>
-      <c r="C85" s="301"/>
+      <c r="A85" s="299"/>
+      <c r="B85" s="296"/>
+      <c r="C85" s="302"/>
       <c r="D85" s="32" t="s">
         <v>73</v>
       </c>
@@ -17392,9 +17448,9 @@
       <c r="S85" s="8"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A86" s="299"/>
-      <c r="B86" s="296"/>
-      <c r="C86" s="302"/>
+      <c r="A86" s="300"/>
+      <c r="B86" s="297"/>
+      <c r="C86" s="303"/>
       <c r="D86" s="32" t="s">
         <v>74</v>
       </c>
@@ -17452,10 +17508,10 @@
       <c r="S87" s="8"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A88" s="297">
+      <c r="A88" s="298">
         <v>41</v>
       </c>
-      <c r="B88" s="294">
+      <c r="B88" s="295">
         <v>44108</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -17484,8 +17540,8 @@
       <c r="S88" s="8"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A89" s="299"/>
-      <c r="B89" s="296"/>
+      <c r="A89" s="300"/>
+      <c r="B89" s="297"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="4"/>
@@ -17574,10 +17630,10 @@
       <c r="S91" s="8"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A92" s="297">
+      <c r="A92" s="298">
         <v>44</v>
       </c>
-      <c r="B92" s="294">
+      <c r="B92" s="295">
         <v>44112</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -17606,8 +17662,8 @@
       <c r="S92" s="8"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A93" s="298"/>
-      <c r="B93" s="295"/>
+      <c r="A93" s="299"/>
+      <c r="B93" s="296"/>
       <c r="C93" s="1" t="s">
         <v>113</v>
       </c>
@@ -17634,8 +17690,8 @@
       <c r="S93" s="8"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A94" s="298"/>
-      <c r="B94" s="295"/>
+      <c r="A94" s="299"/>
+      <c r="B94" s="296"/>
       <c r="C94" s="1" t="s">
         <v>98</v>
       </c>
@@ -17664,8 +17720,8 @@
       <c r="S94" s="8"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A95" s="299"/>
-      <c r="B95" s="296"/>
+      <c r="A95" s="300"/>
+      <c r="B95" s="297"/>
       <c r="C95" s="1" t="s">
         <v>111</v>
       </c>
@@ -18124,12 +18180,12 @@
       <c r="S113" s="8"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A114" s="290" t="s">
+      <c r="A114" s="291" t="s">
         <v>57</v>
       </c>
-      <c r="B114" s="290"/>
-      <c r="C114" s="290"/>
-      <c r="D114" s="291"/>
+      <c r="B114" s="291"/>
+      <c r="C114" s="291"/>
+      <c r="D114" s="292"/>
       <c r="E114" s="16">
         <f>SUM(E80:E113)</f>
         <v>600000</v>
@@ -18156,10 +18212,10 @@
       <c r="S114" s="8"/>
     </row>
     <row r="115" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="292"/>
-      <c r="B115" s="292"/>
-      <c r="C115" s="292"/>
-      <c r="D115" s="293"/>
+      <c r="A115" s="293"/>
+      <c r="B115" s="293"/>
+      <c r="C115" s="293"/>
+      <c r="D115" s="294"/>
       <c r="E115" s="17" t="s">
         <v>61</v>
       </c>
@@ -21423,12 +21479,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="313" t="s">
+      <c r="A1" s="314" t="s">
         <v>270</v>
       </c>
-      <c r="B1" s="313"/>
-      <c r="C1" s="313"/>
-      <c r="D1" s="313"/>
+      <c r="B1" s="314"/>
+      <c r="C1" s="314"/>
+      <c r="D1" s="314"/>
     </row>
     <row r="2" spans="1:4" ht="19.95" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A2" s="146" t="s">
@@ -21670,7 +21726,7 @@
       <c r="A3" s="107">
         <v>1</v>
       </c>
-      <c r="B3" s="314">
+      <c r="B3" s="315">
         <v>44123</v>
       </c>
       <c r="C3" s="108"/>
@@ -21680,7 +21736,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A4" s="110"/>
-      <c r="B4" s="315"/>
+      <c r="B4" s="316"/>
       <c r="C4" s="111"/>
       <c r="D4" s="112" t="s">
         <v>202</v>
@@ -21688,7 +21744,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A5" s="110"/>
-      <c r="B5" s="315"/>
+      <c r="B5" s="316"/>
       <c r="C5" s="111"/>
       <c r="D5" s="113" t="s">
         <v>203</v>
@@ -21696,7 +21752,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A6" s="110"/>
-      <c r="B6" s="315"/>
+      <c r="B6" s="316"/>
       <c r="C6" s="111"/>
       <c r="D6" s="113" t="s">
         <v>204</v>
@@ -21704,7 +21760,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A7" s="110"/>
-      <c r="B7" s="315"/>
+      <c r="B7" s="316"/>
       <c r="C7" s="111"/>
       <c r="D7" s="113" t="s">
         <v>205</v>
@@ -21712,7 +21768,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A8" s="110"/>
-      <c r="B8" s="315"/>
+      <c r="B8" s="316"/>
       <c r="C8" s="111"/>
       <c r="D8" s="113" t="s">
         <v>206</v>
@@ -21720,7 +21776,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A9" s="110"/>
-      <c r="B9" s="315"/>
+      <c r="B9" s="316"/>
       <c r="C9" s="111"/>
       <c r="D9" s="113" t="s">
         <v>207</v>
@@ -21728,7 +21784,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A10" s="110"/>
-      <c r="B10" s="315"/>
+      <c r="B10" s="316"/>
       <c r="C10" s="111"/>
       <c r="D10" s="113" t="s">
         <v>208</v>
@@ -21736,7 +21792,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A11" s="110"/>
-      <c r="B11" s="315"/>
+      <c r="B11" s="316"/>
       <c r="C11" s="111"/>
       <c r="D11" s="113" t="s">
         <v>209</v>
@@ -21784,7 +21840,7 @@
       <c r="A17" s="121">
         <v>2</v>
       </c>
-      <c r="B17" s="316">
+      <c r="B17" s="317">
         <v>44124</v>
       </c>
       <c r="C17" s="108"/>
@@ -21794,7 +21850,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A18" s="123"/>
-      <c r="B18" s="316"/>
+      <c r="B18" s="317"/>
       <c r="C18" s="124"/>
       <c r="D18" s="125" t="s">
         <v>213</v>
@@ -21802,7 +21858,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A19" s="123"/>
-      <c r="B19" s="316"/>
+      <c r="B19" s="317"/>
       <c r="C19" s="124"/>
       <c r="D19" s="125" t="s">
         <v>214</v>
@@ -21810,7 +21866,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A20" s="123"/>
-      <c r="B20" s="316"/>
+      <c r="B20" s="317"/>
       <c r="C20" s="124"/>
       <c r="D20" s="125" t="s">
         <v>215</v>
@@ -21818,7 +21874,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A21" s="123"/>
-      <c r="B21" s="316"/>
+      <c r="B21" s="317"/>
       <c r="C21" s="124"/>
       <c r="D21" s="125" t="s">
         <v>205</v>
@@ -21826,7 +21882,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A22" s="123"/>
-      <c r="B22" s="316"/>
+      <c r="B22" s="317"/>
       <c r="C22" s="124"/>
       <c r="D22" s="125" t="s">
         <v>216</v>
@@ -21834,7 +21890,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A23" s="123"/>
-      <c r="B23" s="316"/>
+      <c r="B23" s="317"/>
       <c r="C23" s="124"/>
       <c r="D23" s="125" t="s">
         <v>217</v>
@@ -21842,7 +21898,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A24" s="123"/>
-      <c r="B24" s="316"/>
+      <c r="B24" s="317"/>
       <c r="C24" s="124"/>
       <c r="D24" s="125" t="s">
         <v>218</v>
@@ -21884,7 +21940,7 @@
       <c r="A29" s="121">
         <v>3</v>
       </c>
-      <c r="B29" s="317">
+      <c r="B29" s="318">
         <v>44126</v>
       </c>
       <c r="C29" s="108"/>
@@ -21894,7 +21950,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A30" s="123"/>
-      <c r="B30" s="316"/>
+      <c r="B30" s="317"/>
       <c r="C30" s="124"/>
       <c r="D30" s="125" t="s">
         <v>223</v>
@@ -21902,7 +21958,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A31" s="123"/>
-      <c r="B31" s="316"/>
+      <c r="B31" s="317"/>
       <c r="C31" s="124"/>
       <c r="D31" s="125" t="s">
         <v>224</v>
@@ -21910,7 +21966,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A32" s="123"/>
-      <c r="B32" s="316"/>
+      <c r="B32" s="317"/>
       <c r="C32" s="124"/>
       <c r="D32" s="125" t="s">
         <v>225</v>
@@ -21918,7 +21974,7 @@
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A33" s="123"/>
-      <c r="B33" s="316"/>
+      <c r="B33" s="317"/>
       <c r="C33" s="124"/>
       <c r="D33" s="125" t="s">
         <v>226</v>
@@ -21926,7 +21982,7 @@
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A34" s="123"/>
-      <c r="B34" s="316"/>
+      <c r="B34" s="317"/>
       <c r="C34" s="124"/>
       <c r="D34" s="125" t="s">
         <v>227</v>
@@ -21934,7 +21990,7 @@
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A35" s="123"/>
-      <c r="B35" s="316"/>
+      <c r="B35" s="317"/>
       <c r="C35" s="124"/>
       <c r="D35" s="125" t="s">
         <v>228</v>
@@ -21950,43 +22006,43 @@
       <c r="A37" s="121">
         <v>3</v>
       </c>
-      <c r="B37" s="317"/>
+      <c r="B37" s="318"/>
       <c r="C37" s="108"/>
       <c r="D37" s="122"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A38" s="123"/>
-      <c r="B38" s="316"/>
+      <c r="B38" s="317"/>
       <c r="C38" s="124"/>
       <c r="D38" s="125"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A39" s="123"/>
-      <c r="B39" s="316"/>
+      <c r="B39" s="317"/>
       <c r="C39" s="124"/>
       <c r="D39" s="125"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A40" s="123"/>
-      <c r="B40" s="316"/>
+      <c r="B40" s="317"/>
       <c r="C40" s="124"/>
       <c r="D40" s="125"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A41" s="123"/>
-      <c r="B41" s="316"/>
+      <c r="B41" s="317"/>
       <c r="C41" s="124"/>
       <c r="D41" s="125"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A42" s="123"/>
-      <c r="B42" s="316"/>
+      <c r="B42" s="317"/>
       <c r="C42" s="124"/>
       <c r="D42" s="125"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.5">
       <c r="A43" s="123"/>
-      <c r="B43" s="316"/>
+      <c r="B43" s="317"/>
       <c r="C43" s="124"/>
       <c r="D43" s="125"/>
     </row>
@@ -22091,36 +22147,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -22227,21 +22283,21 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="287" t="s">
+      <c r="A7" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="288"/>
-      <c r="C7" s="288"/>
+      <c r="B7" s="289"/>
+      <c r="C7" s="289"/>
       <c r="D7" s="44">
         <f>SUM(D4:D6)</f>
         <v>50000</v>
       </c>
       <c r="E7" s="50"/>
-      <c r="F7" s="287" t="s">
+      <c r="F7" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="288"/>
-      <c r="H7" s="289"/>
+      <c r="G7" s="289"/>
+      <c r="H7" s="290"/>
       <c r="I7" s="44">
         <f>SUM(I4:I6)</f>
         <v>50000</v>
@@ -22846,11 +22902,11 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9048F5A1-D0E4-4154-BAE0-2D93FAD46A94}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9048F5A1-D0E4-4154-BAE0-2D93FAD46A94}">
   <dimension ref="A1:M56"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -22867,36 +22923,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>157</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -23149,10 +23205,18 @@
       <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A11" s="74"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="40"/>
+      <c r="A11" s="262">
+        <v>8</v>
+      </c>
+      <c r="B11" s="39">
+        <v>44279</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="D11" s="40">
+        <v>1062000</v>
+      </c>
       <c r="E11" s="38"/>
       <c r="F11" s="188">
         <v>8</v>
@@ -23174,7 +23238,9 @@
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>449</v>
+      </c>
       <c r="D12" s="40"/>
       <c r="E12" s="38"/>
       <c r="F12" s="74">
@@ -23255,21 +23321,21 @@
       <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="287" t="s">
+      <c r="A17" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="288"/>
-      <c r="C17" s="288"/>
+      <c r="B17" s="289"/>
+      <c r="C17" s="289"/>
       <c r="D17" s="44">
         <f>SUM(D4:D16)</f>
-        <v>283000</v>
+        <v>1345000</v>
       </c>
       <c r="E17" s="50"/>
-      <c r="F17" s="287" t="s">
+      <c r="F17" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="288"/>
-      <c r="H17" s="289"/>
+      <c r="G17" s="289"/>
+      <c r="H17" s="290"/>
       <c r="I17" s="44">
         <f>SUM(I4:I16)</f>
         <v>283215</v>
@@ -23302,7 +23368,7 @@
       </c>
       <c r="D19" s="58">
         <f>D17</f>
-        <v>283000</v>
+        <v>1345000</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="53"/>
@@ -23357,7 +23423,7 @@
       </c>
       <c r="D22" s="62">
         <f>D19-D20</f>
-        <v>-215</v>
+        <v>1061785</v>
       </c>
       <c r="E22" s="8"/>
       <c r="F22" s="53"/>
@@ -23870,6 +23936,7 @@
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -24338,10 +24405,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8095CE61-3623-466A-A99B-F028ACAC31F9}">
-  <dimension ref="B2:O21"/>
+  <dimension ref="B2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -24349,34 +24416,40 @@
     <col min="2" max="2" width="13.703125" customWidth="1"/>
     <col min="3" max="3" width="10.9375" style="72" customWidth="1"/>
     <col min="4" max="4" width="12.5859375" customWidth="1"/>
-    <col min="5" max="5" width="10.703125" customWidth="1"/>
-    <col min="6" max="6" width="11.52734375" style="72" customWidth="1"/>
+    <col min="5" max="5" width="16.76171875" customWidth="1"/>
+    <col min="6" max="6" width="13.703125" style="72" customWidth="1"/>
     <col min="7" max="7" width="4.46875" customWidth="1"/>
     <col min="8" max="8" width="9" customWidth="1"/>
     <col min="9" max="9" width="9.17578125" customWidth="1"/>
-    <col min="10" max="10" width="1.76171875" customWidth="1"/>
-    <col min="12" max="13" width="8.87890625" style="72"/>
-    <col min="14" max="14" width="11.8203125" customWidth="1"/>
-    <col min="15" max="15" width="8.9375" style="72"/>
+    <col min="10" max="10" width="8.9375" style="72"/>
+    <col min="11" max="12" width="8.87890625" style="72"/>
+    <col min="13" max="13" width="11.8203125" customWidth="1"/>
+    <col min="14" max="14" width="8.9375" style="72"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B2" s="84" t="s">
         <v>31</v>
       </c>
       <c r="C2" s="179">
         <f>BOFC!D168</f>
-        <v>1447599</v>
+        <v>1447479</v>
       </c>
       <c r="E2" t="s">
         <v>311</v>
       </c>
       <c r="F2" s="72">
-        <v>745000</v>
+        <v>790000</v>
       </c>
       <c r="H2" s="72"/>
-    </row>
-    <row r="3" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="I2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J2" s="72">
+        <v>1062000</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B3" s="84" t="s">
         <v>307</v>
       </c>
@@ -24390,8 +24463,14 @@
       <c r="F3" s="72">
         <v>55000</v>
       </c>
-    </row>
-    <row r="4" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="I3" t="s">
+        <v>311</v>
+      </c>
+      <c r="J3" s="72">
+        <v>42000</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B4" s="84" t="s">
         <v>442</v>
       </c>
@@ -24403,10 +24482,10 @@
         <v>261</v>
       </c>
       <c r="F4" s="72">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" x14ac:dyDescent="0.5">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
         <v>308</v>
       </c>
@@ -24414,8 +24493,12 @@
         <f>Jhangir!D19</f>
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="J5" s="72">
+        <f>SUM(J2:J4)</f>
+        <v>1104000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
         <v>278</v>
       </c>
@@ -24427,10 +24510,10 @@
         <v>444</v>
       </c>
       <c r="F6" s="72">
-        <v>62000</v>
-      </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.5">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B7" t="s">
         <v>305</v>
       </c>
@@ -24439,7 +24522,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="8" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
         <v>306</v>
       </c>
@@ -24448,7 +24531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:15" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="2:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>274</v>
       </c>
@@ -24459,7 +24542,7 @@
       <c r="H9" s="180"/>
       <c r="I9" s="181"/>
     </row>
-    <row r="10" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="10" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B10" t="s">
         <v>309</v>
       </c>
@@ -24467,9 +24550,14 @@
         <f>Kamil!D78</f>
         <v>0</v>
       </c>
-      <c r="K10" s="72"/>
-    </row>
-    <row r="11" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="E10" t="s">
+        <v>451</v>
+      </c>
+      <c r="F10" s="72">
+        <v>1062000</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B11" t="s">
         <v>112</v>
       </c>
@@ -24477,12 +24565,15 @@
         <f>Shehzad!D23</f>
         <v>0</v>
       </c>
-      <c r="L11" s="72">
+      <c r="E11" t="s">
+        <v>450</v>
+      </c>
+      <c r="K11" s="72">
         <v>507</v>
       </c>
-      <c r="O11" s="179"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.5">
+      <c r="N11" s="179"/>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B12" t="s">
         <v>320</v>
       </c>
@@ -24490,39 +24581,39 @@
         <f>Kamil!D96</f>
         <v>0</v>
       </c>
-      <c r="K12" s="80" t="s">
+      <c r="J12" s="189" t="s">
         <v>369</v>
       </c>
-      <c r="L12" s="72">
+      <c r="K12" s="72">
         <v>493</v>
       </c>
     </row>
-    <row r="13" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="13" spans="2:14" x14ac:dyDescent="0.5">
       <c r="E13" s="72"/>
-      <c r="K13" s="80" t="s">
+      <c r="J13" s="189" t="s">
         <v>369</v>
       </c>
-      <c r="L13" s="72">
+      <c r="K13" s="72">
         <v>720</v>
       </c>
     </row>
-    <row r="14" spans="2:15" ht="15.7" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="2:14" ht="15.7" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>175</v>
       </c>
       <c r="C14" s="72">
         <f>Mazhar!D22</f>
-        <v>-215</v>
+        <v>1061785</v>
       </c>
       <c r="H14" s="180" t="s">
         <v>4</v>
       </c>
       <c r="I14" s="181">
         <f>C19-F19</f>
-        <v>52570</v>
-      </c>
-    </row>
-    <row r="15" spans="2:15" x14ac:dyDescent="0.5">
+        <v>55050</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B15" t="s">
         <v>121</v>
       </c>
@@ -24530,11 +24621,11 @@
         <f>Farooq!D12</f>
         <v>-3000</v>
       </c>
-      <c r="L15" s="72">
+      <c r="K15" s="72">
         <v>572</v>
       </c>
     </row>
-    <row r="16" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="16" spans="2:14" x14ac:dyDescent="0.5">
       <c r="B16" t="s">
         <v>310</v>
       </c>
@@ -24543,7 +24634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B17" s="84" t="s">
         <v>307</v>
       </c>
@@ -24558,16 +24649,16 @@
         <v>865000</v>
       </c>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:12" x14ac:dyDescent="0.5">
       <c r="C18" s="243"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:12" x14ac:dyDescent="0.5">
       <c r="B19" s="252" t="s">
         <v>144</v>
       </c>
       <c r="C19" s="253">
         <f>SUM(C2:C18)</f>
-        <v>1781170</v>
+        <v>2843050</v>
       </c>
       <c r="D19" s="252"/>
       <c r="E19" s="252" t="s">
@@ -24575,16 +24666,16 @@
       </c>
       <c r="F19" s="253">
         <f>SUM(F2:F18)</f>
-        <v>1728600</v>
-      </c>
-      <c r="L19" s="72">
+        <v>2788000</v>
+      </c>
+      <c r="K19" s="72">
         <v>956</v>
       </c>
-      <c r="M19" s="72" t="s">
+      <c r="L19" s="72" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="21" spans="2:13" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:12" x14ac:dyDescent="0.5">
       <c r="C21" s="179"/>
       <c r="D21" s="179"/>
     </row>
@@ -24599,7 +24690,7 @@
   <dimension ref="E4:O19"/>
   <sheetViews>
     <sheetView topLeftCell="D2" zoomScale="122" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -24770,13 +24861,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>383</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -24784,13 +24875,13 @@
       <c r="J1" s="8"/>
     </row>
     <row r="2" spans="1:10" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="266"/>
-      <c r="E2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="267"/>
+      <c r="E2" s="268"/>
       <c r="F2" s="8"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
@@ -25012,11 +25103,11 @@
       <c r="J17" s="8"/>
     </row>
     <row r="18" spans="1:10" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="268" t="s">
+      <c r="A18" s="269" t="s">
         <v>144</v>
       </c>
-      <c r="B18" s="269"/>
-      <c r="C18" s="269"/>
+      <c r="B18" s="270"/>
+      <c r="C18" s="270"/>
       <c r="D18" s="44">
         <f>SUM(D4:D17)</f>
         <v>182000</v>
@@ -25049,11 +25140,11 @@
       <c r="C20" s="224" t="s">
         <v>392</v>
       </c>
-      <c r="D20" s="273">
+      <c r="D20" s="274">
         <f>D18+E18</f>
         <v>196000</v>
       </c>
-      <c r="E20" s="273"/>
+      <c r="E20" s="274"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
@@ -25064,8 +25155,8 @@
       <c r="A21" s="8"/>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
-      <c r="D21" s="272"/>
-      <c r="E21" s="272"/>
+      <c r="D21" s="273"/>
+      <c r="E21" s="273"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
@@ -31789,19 +31880,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="280" t="s">
+      <c r="A1" s="281" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="281"/>
-      <c r="C1" s="281"/>
-      <c r="D1" s="281"/>
-      <c r="E1" s="282"/>
-      <c r="G1" s="279" t="s">
+      <c r="B1" s="282"/>
+      <c r="C1" s="282"/>
+      <c r="D1" s="282"/>
+      <c r="E1" s="283"/>
+      <c r="G1" s="280" t="s">
         <v>429</v>
       </c>
-      <c r="H1" s="279"/>
-      <c r="I1" s="279"/>
-      <c r="J1" s="279"/>
+      <c r="H1" s="280"/>
+      <c r="I1" s="280"/>
+      <c r="J1" s="280"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -31823,18 +31914,18 @@
         <v>4</v>
       </c>
       <c r="F2" s="238"/>
-      <c r="G2" s="274" t="s">
+      <c r="G2" s="275" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="274"/>
-      <c r="I2" s="274"/>
-      <c r="J2" s="274"/>
+      <c r="H2" s="275"/>
+      <c r="I2" s="275"/>
+      <c r="J2" s="275"/>
       <c r="K2" s="238"/>
       <c r="L2" s="238"/>
       <c r="M2" s="238"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A3" s="275">
+      <c r="A3" s="276">
         <v>1</v>
       </c>
       <c r="B3" s="211">
@@ -31846,7 +31937,7 @@
       <c r="D3" s="209">
         <v>30000</v>
       </c>
-      <c r="E3" s="277">
+      <c r="E3" s="278">
         <f>D4-D3</f>
         <v>-30000</v>
       </c>
@@ -31867,11 +31958,11 @@
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A4" s="276"/>
+      <c r="A4" s="277"/>
       <c r="B4" s="213"/>
       <c r="C4" s="214"/>
       <c r="D4" s="210"/>
-      <c r="E4" s="278"/>
+      <c r="E4" s="279"/>
       <c r="G4" s="230">
         <v>1</v>
       </c>
@@ -31907,7 +31998,7 @@
       <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A6" s="275">
+      <c r="A6" s="276">
         <v>2</v>
       </c>
       <c r="B6" s="211">
@@ -31919,7 +32010,7 @@
       <c r="D6" s="209">
         <v>5000</v>
       </c>
-      <c r="E6" s="277">
+      <c r="E6" s="278">
         <f>D7-D6</f>
         <v>-5000</v>
       </c>
@@ -31940,11 +32031,11 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A7" s="276"/>
+      <c r="A7" s="277"/>
       <c r="B7" s="213"/>
       <c r="C7" s="214"/>
       <c r="D7" s="210"/>
-      <c r="E7" s="278"/>
+      <c r="E7" s="279"/>
       <c r="G7" s="230">
         <v>3</v>
       </c>
@@ -31980,7 +32071,7 @@
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A9" s="275">
+      <c r="A9" s="276">
         <v>4</v>
       </c>
       <c r="B9" s="211">
@@ -31992,7 +32083,7 @@
       <c r="D9" s="209">
         <v>3070</v>
       </c>
-      <c r="E9" s="277">
+      <c r="E9" s="278">
         <f>D10-D9</f>
         <v>-3070</v>
       </c>
@@ -32013,11 +32104,11 @@
       <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A10" s="276"/>
+      <c r="A10" s="277"/>
       <c r="B10" s="213"/>
       <c r="C10" s="214"/>
       <c r="D10" s="210"/>
-      <c r="E10" s="278"/>
+      <c r="E10" s="279"/>
       <c r="G10" s="230">
         <v>5</v>
       </c>
@@ -32057,7 +32148,7 @@
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A12" s="275">
+      <c r="A12" s="276">
         <v>5</v>
       </c>
       <c r="B12" s="211">
@@ -32069,7 +32160,7 @@
       <c r="D12" s="209">
         <v>5000</v>
       </c>
-      <c r="E12" s="277">
+      <c r="E12" s="278">
         <f>D13-D12</f>
         <v>-5000</v>
       </c>
@@ -32090,11 +32181,11 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A13" s="276"/>
+      <c r="A13" s="277"/>
       <c r="B13" s="213"/>
       <c r="C13" s="214"/>
       <c r="D13" s="210"/>
-      <c r="E13" s="278"/>
+      <c r="E13" s="279"/>
       <c r="G13" s="1"/>
       <c r="H13" s="233"/>
       <c r="I13" s="1"/>
@@ -32118,7 +32209,7 @@
       <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A15" s="275">
+      <c r="A15" s="276">
         <v>6</v>
       </c>
       <c r="B15" s="211">
@@ -32130,7 +32221,7 @@
       <c r="D15" s="209">
         <v>5000</v>
       </c>
-      <c r="E15" s="277">
+      <c r="E15" s="278">
         <f>D16-D15</f>
         <v>-5000</v>
       </c>
@@ -32143,11 +32234,11 @@
       <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A16" s="276"/>
+      <c r="A16" s="277"/>
       <c r="B16" s="213"/>
       <c r="C16" s="214"/>
       <c r="D16" s="210"/>
-      <c r="E16" s="278"/>
+      <c r="E16" s="279"/>
       <c r="G16" s="1"/>
       <c r="H16" s="234"/>
       <c r="I16" s="1"/>
@@ -32171,7 +32262,7 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A18" s="275">
+      <c r="A18" s="276">
         <v>7</v>
       </c>
       <c r="B18" s="211">
@@ -32183,15 +32274,15 @@
       <c r="D18" s="209">
         <v>5000</v>
       </c>
-      <c r="E18" s="277">
+      <c r="E18" s="278">
         <f>D19-D18</f>
         <v>-5000</v>
       </c>
-      <c r="G18" s="268" t="s">
+      <c r="G18" s="269" t="s">
         <v>144</v>
       </c>
-      <c r="H18" s="269"/>
-      <c r="I18" s="269"/>
+      <c r="H18" s="270"/>
+      <c r="I18" s="270"/>
       <c r="J18" s="44">
         <f>SUM(J4:J17)</f>
         <v>0</v>
@@ -32201,11 +32292,11 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A19" s="276"/>
+      <c r="A19" s="277"/>
       <c r="B19" s="213"/>
       <c r="C19" s="214"/>
       <c r="D19" s="210"/>
-      <c r="E19" s="278"/>
+      <c r="E19" s="279"/>
       <c r="G19" s="55"/>
       <c r="H19" s="236"/>
       <c r="I19" s="55"/>
@@ -32220,18 +32311,18 @@
       <c r="C20" s="8"/>
       <c r="D20" s="240"/>
       <c r="E20" s="242"/>
-      <c r="G20" s="274" t="s">
+      <c r="G20" s="275" t="s">
         <v>411</v>
       </c>
-      <c r="H20" s="274"/>
-      <c r="I20" s="274"/>
-      <c r="J20" s="274"/>
+      <c r="H20" s="275"/>
+      <c r="I20" s="275"/>
+      <c r="J20" s="275"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A21" s="275">
+      <c r="A21" s="276">
         <v>8</v>
       </c>
       <c r="B21" s="211">
@@ -32243,7 +32334,7 @@
       <c r="D21" s="209">
         <v>600</v>
       </c>
-      <c r="E21" s="277">
+      <c r="E21" s="278">
         <f>D22-D21</f>
         <v>-600</v>
       </c>
@@ -32264,11 +32355,11 @@
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A22" s="276"/>
+      <c r="A22" s="277"/>
       <c r="B22" s="213"/>
       <c r="C22" s="214"/>
       <c r="D22" s="210"/>
-      <c r="E22" s="278"/>
+      <c r="E22" s="279"/>
       <c r="G22" s="231">
         <v>1</v>
       </c>
@@ -32308,7 +32399,7 @@
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A24" s="275">
+      <c r="A24" s="276">
         <v>9</v>
       </c>
       <c r="B24" s="211">
@@ -32320,7 +32411,7 @@
       <c r="D24" s="209">
         <v>5000</v>
       </c>
-      <c r="E24" s="277">
+      <c r="E24" s="278">
         <f>D25-D24</f>
         <v>-5000</v>
       </c>
@@ -32333,11 +32424,11 @@
       <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A25" s="276"/>
+      <c r="A25" s="277"/>
       <c r="B25" s="213"/>
       <c r="C25" s="214"/>
       <c r="D25" s="210"/>
-      <c r="E25" s="278"/>
+      <c r="E25" s="279"/>
       <c r="G25" s="231"/>
       <c r="H25" s="234"/>
       <c r="I25" s="1"/>
@@ -32361,7 +32452,7 @@
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A27" s="275">
+      <c r="A27" s="276">
         <v>10</v>
       </c>
       <c r="B27" s="211">
@@ -32373,7 +32464,7 @@
       <c r="D27" s="209">
         <v>5000</v>
       </c>
-      <c r="E27" s="277">
+      <c r="E27" s="278">
         <f>D28-D27</f>
         <v>-5000</v>
       </c>
@@ -32386,11 +32477,11 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A28" s="276"/>
+      <c r="A28" s="277"/>
       <c r="B28" s="213"/>
       <c r="C28" s="214"/>
       <c r="D28" s="210"/>
-      <c r="E28" s="278"/>
+      <c r="E28" s="279"/>
       <c r="G28" s="231"/>
       <c r="H28" s="234"/>
       <c r="I28" s="1"/>
@@ -32414,7 +32505,7 @@
       <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A30" s="275">
+      <c r="A30" s="276">
         <v>11</v>
       </c>
       <c r="B30" s="211">
@@ -32426,7 +32517,7 @@
       <c r="D30" s="209">
         <v>5000</v>
       </c>
-      <c r="E30" s="277">
+      <c r="E30" s="278">
         <f>D31-D30</f>
         <v>-5000</v>
       </c>
@@ -32439,11 +32530,11 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A31" s="276"/>
+      <c r="A31" s="277"/>
       <c r="B31" s="213"/>
       <c r="C31" s="214"/>
       <c r="D31" s="210"/>
-      <c r="E31" s="278"/>
+      <c r="E31" s="279"/>
       <c r="G31" s="1"/>
       <c r="H31" s="233"/>
       <c r="I31" s="1"/>
@@ -32467,13 +32558,13 @@
       <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A33" s="275">
+      <c r="A33" s="276">
         <v>12</v>
       </c>
       <c r="B33" s="211"/>
       <c r="C33" s="212"/>
       <c r="D33" s="209"/>
-      <c r="E33" s="277">
+      <c r="E33" s="278">
         <f>D34-D33</f>
         <v>0</v>
       </c>
@@ -32486,11 +32577,11 @@
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A34" s="276"/>
+      <c r="A34" s="277"/>
       <c r="B34" s="213"/>
       <c r="C34" s="214"/>
       <c r="D34" s="210"/>
-      <c r="E34" s="278"/>
+      <c r="E34" s="279"/>
       <c r="G34" s="1"/>
       <c r="H34" s="234"/>
       <c r="I34" s="1"/>
@@ -32514,21 +32605,21 @@
       <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A36" s="275">
+      <c r="A36" s="276">
         <v>13</v>
       </c>
       <c r="B36" s="211"/>
       <c r="C36" s="212"/>
       <c r="D36" s="209"/>
-      <c r="E36" s="277">
+      <c r="E36" s="278">
         <f>D37-D36</f>
         <v>0</v>
       </c>
-      <c r="G36" s="268" t="s">
+      <c r="G36" s="269" t="s">
         <v>144</v>
       </c>
-      <c r="H36" s="269"/>
-      <c r="I36" s="269"/>
+      <c r="H36" s="270"/>
+      <c r="I36" s="270"/>
       <c r="J36" s="44">
         <f>SUM(J22:J35)</f>
         <v>0</v>
@@ -32538,11 +32629,11 @@
       <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A37" s="276"/>
+      <c r="A37" s="277"/>
       <c r="B37" s="213"/>
       <c r="C37" s="214"/>
       <c r="D37" s="210"/>
-      <c r="E37" s="278"/>
+      <c r="E37" s="279"/>
       <c r="G37" s="8"/>
       <c r="H37" s="241"/>
       <c r="I37" s="8"/>
@@ -32566,13 +32657,13 @@
       <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A39" s="275">
+      <c r="A39" s="276">
         <v>14</v>
       </c>
       <c r="B39" s="211"/>
       <c r="C39" s="212"/>
       <c r="D39" s="209"/>
-      <c r="E39" s="277">
+      <c r="E39" s="278">
         <f>D40-D39</f>
         <v>0</v>
       </c>
@@ -32585,11 +32676,11 @@
       <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A40" s="276"/>
+      <c r="A40" s="277"/>
       <c r="B40" s="213"/>
       <c r="C40" s="214"/>
       <c r="D40" s="210"/>
-      <c r="E40" s="278"/>
+      <c r="E40" s="279"/>
       <c r="G40" s="8"/>
       <c r="H40" s="241"/>
       <c r="I40" s="8"/>
@@ -32613,13 +32704,13 @@
       <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A42" s="275">
+      <c r="A42" s="276">
         <v>15</v>
       </c>
       <c r="B42" s="211"/>
       <c r="C42" s="212"/>
       <c r="D42" s="209"/>
-      <c r="E42" s="277">
+      <c r="E42" s="278">
         <f>D43-D42</f>
         <v>0</v>
       </c>
@@ -32632,11 +32723,11 @@
       <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A43" s="276"/>
+      <c r="A43" s="277"/>
       <c r="B43" s="213"/>
       <c r="C43" s="214"/>
       <c r="D43" s="210"/>
-      <c r="E43" s="278"/>
+      <c r="E43" s="279"/>
       <c r="G43" s="8"/>
       <c r="H43" s="241"/>
       <c r="I43" s="8"/>
@@ -32660,12 +32751,12 @@
       <c r="M44" s="8"/>
     </row>
     <row r="45" spans="1:13" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="284" t="s">
+      <c r="A45" s="285" t="s">
         <v>412</v>
       </c>
-      <c r="B45" s="285"/>
-      <c r="C45" s="285"/>
-      <c r="D45" s="286"/>
+      <c r="B45" s="286"/>
+      <c r="C45" s="286"/>
+      <c r="D45" s="287"/>
       <c r="E45" s="219">
         <f>SUM(E3:E44)</f>
         <v>-68670</v>
@@ -32682,8 +32773,8 @@
       <c r="A46" s="79"/>
       <c r="B46" s="239"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="283"/>
-      <c r="E46" s="283"/>
+      <c r="D46" s="284"/>
+      <c r="E46" s="284"/>
       <c r="G46" s="8"/>
       <c r="H46" s="241"/>
       <c r="I46" s="8"/>
@@ -32933,36 +33024,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="34" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -33191,21 +33282,21 @@
       <c r="M10" s="8"/>
     </row>
     <row r="11" spans="1:13" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A11" s="268" t="s">
+      <c r="A11" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B11" s="269"/>
-      <c r="C11" s="269"/>
+      <c r="B11" s="270"/>
+      <c r="C11" s="270"/>
       <c r="D11" s="44">
         <f>SUM(D4:D10)</f>
         <v>371000</v>
       </c>
       <c r="E11" s="50"/>
-      <c r="F11" s="268" t="s">
+      <c r="F11" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G11" s="269"/>
-      <c r="H11" s="270"/>
+      <c r="G11" s="270"/>
+      <c r="H11" s="271"/>
       <c r="I11" s="44">
         <f>SUM(I4:I10)</f>
         <v>365000</v>
@@ -33321,36 +33412,36 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" ht="33.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="262" t="s">
+      <c r="A18" s="263" t="s">
         <v>149</v>
       </c>
-      <c r="B18" s="263"/>
-      <c r="C18" s="263"/>
-      <c r="D18" s="263"/>
-      <c r="E18" s="263"/>
-      <c r="F18" s="263"/>
-      <c r="G18" s="263"/>
-      <c r="H18" s="263"/>
-      <c r="I18" s="264"/>
+      <c r="B18" s="264"/>
+      <c r="C18" s="264"/>
+      <c r="D18" s="264"/>
+      <c r="E18" s="264"/>
+      <c r="F18" s="264"/>
+      <c r="G18" s="264"/>
+      <c r="H18" s="264"/>
+      <c r="I18" s="265"/>
       <c r="J18" s="8"/>
       <c r="K18" s="8"/>
       <c r="L18" s="8"/>
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A19" s="265" t="s">
+      <c r="A19" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="266"/>
-      <c r="C19" s="266"/>
-      <c r="D19" s="267"/>
+      <c r="B19" s="267"/>
+      <c r="C19" s="267"/>
+      <c r="D19" s="268"/>
       <c r="E19" s="43"/>
-      <c r="F19" s="265" t="s">
+      <c r="F19" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G19" s="266"/>
-      <c r="H19" s="266"/>
-      <c r="I19" s="267"/>
+      <c r="G19" s="267"/>
+      <c r="H19" s="267"/>
+      <c r="I19" s="268"/>
       <c r="J19" s="8"/>
       <c r="K19" s="8"/>
       <c r="L19" s="8"/>
@@ -33629,21 +33720,21 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" ht="19" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A31" s="268" t="s">
+      <c r="A31" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="269"/>
-      <c r="C31" s="269"/>
+      <c r="B31" s="270"/>
+      <c r="C31" s="270"/>
       <c r="D31" s="44">
         <f>SUM(D21:D30)</f>
         <v>163560</v>
       </c>
       <c r="E31" s="50"/>
-      <c r="F31" s="268" t="s">
+      <c r="F31" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G31" s="269"/>
-      <c r="H31" s="270"/>
+      <c r="G31" s="270"/>
+      <c r="H31" s="271"/>
       <c r="I31" s="44">
         <f>SUM(I21:I30)</f>
         <v>225060</v>
@@ -33758,36 +33849,36 @@
       <c r="M37" s="8"/>
     </row>
     <row r="38" spans="1:13" ht="30.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A38" s="262" t="s">
+      <c r="A38" s="263" t="s">
         <v>185</v>
       </c>
-      <c r="B38" s="263"/>
-      <c r="C38" s="263"/>
-      <c r="D38" s="263"/>
-      <c r="E38" s="263"/>
-      <c r="F38" s="263"/>
-      <c r="G38" s="263"/>
-      <c r="H38" s="263"/>
-      <c r="I38" s="264"/>
+      <c r="B38" s="264"/>
+      <c r="C38" s="264"/>
+      <c r="D38" s="264"/>
+      <c r="E38" s="264"/>
+      <c r="F38" s="264"/>
+      <c r="G38" s="264"/>
+      <c r="H38" s="264"/>
+      <c r="I38" s="265"/>
       <c r="J38" s="8"/>
       <c r="K38" s="8"/>
       <c r="L38" s="8"/>
       <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A39" s="265" t="s">
+      <c r="A39" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B39" s="266"/>
-      <c r="C39" s="266"/>
-      <c r="D39" s="267"/>
+      <c r="B39" s="267"/>
+      <c r="C39" s="267"/>
+      <c r="D39" s="268"/>
       <c r="E39" s="43"/>
-      <c r="F39" s="265" t="s">
+      <c r="F39" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G39" s="266"/>
-      <c r="H39" s="266"/>
-      <c r="I39" s="267"/>
+      <c r="G39" s="267"/>
+      <c r="H39" s="267"/>
+      <c r="I39" s="268"/>
       <c r="J39" s="8"/>
       <c r="K39" s="8"/>
       <c r="L39" s="8"/>
@@ -34066,21 +34157,21 @@
       <c r="M50" s="8"/>
     </row>
     <row r="51" spans="1:13" ht="17.45" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A51" s="268" t="s">
+      <c r="A51" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B51" s="269"/>
-      <c r="C51" s="269"/>
+      <c r="B51" s="270"/>
+      <c r="C51" s="270"/>
       <c r="D51" s="44">
         <f>SUM(D41:D50)</f>
         <v>266150</v>
       </c>
       <c r="E51" s="50"/>
-      <c r="F51" s="268" t="s">
+      <c r="F51" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G51" s="269"/>
-      <c r="H51" s="270"/>
+      <c r="G51" s="270"/>
+      <c r="H51" s="271"/>
       <c r="I51" s="44">
         <f>SUM(I41:I50)</f>
         <v>7850</v>
@@ -34196,36 +34287,36 @@
       <c r="M57" s="8"/>
     </row>
     <row r="58" spans="1:13" ht="32.700000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A58" s="262" t="s">
+      <c r="A58" s="263" t="s">
         <v>282</v>
       </c>
-      <c r="B58" s="263"/>
-      <c r="C58" s="263"/>
-      <c r="D58" s="263"/>
-      <c r="E58" s="263"/>
-      <c r="F58" s="263"/>
-      <c r="G58" s="263"/>
-      <c r="H58" s="263"/>
-      <c r="I58" s="264"/>
+      <c r="B58" s="264"/>
+      <c r="C58" s="264"/>
+      <c r="D58" s="264"/>
+      <c r="E58" s="264"/>
+      <c r="F58" s="264"/>
+      <c r="G58" s="264"/>
+      <c r="H58" s="264"/>
+      <c r="I58" s="265"/>
       <c r="J58" s="8"/>
       <c r="K58" s="8"/>
       <c r="L58" s="8"/>
       <c r="M58" s="8"/>
     </row>
     <row r="59" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A59" s="265" t="s">
+      <c r="A59" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B59" s="266"/>
-      <c r="C59" s="266"/>
-      <c r="D59" s="267"/>
+      <c r="B59" s="267"/>
+      <c r="C59" s="267"/>
+      <c r="D59" s="268"/>
       <c r="E59" s="43"/>
-      <c r="F59" s="265" t="s">
+      <c r="F59" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G59" s="266"/>
-      <c r="H59" s="266"/>
-      <c r="I59" s="267"/>
+      <c r="G59" s="267"/>
+      <c r="H59" s="267"/>
+      <c r="I59" s="268"/>
       <c r="J59" s="8"/>
       <c r="K59" s="8"/>
       <c r="L59" s="8"/>
@@ -34484,21 +34575,21 @@
       <c r="M70" s="8"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A71" s="268" t="s">
+      <c r="A71" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B71" s="269"/>
-      <c r="C71" s="269"/>
+      <c r="B71" s="270"/>
+      <c r="C71" s="270"/>
       <c r="D71" s="44">
         <f>SUM(D61:D70)</f>
         <v>288300</v>
       </c>
       <c r="E71" s="50"/>
-      <c r="F71" s="268" t="s">
+      <c r="F71" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G71" s="269"/>
-      <c r="H71" s="270"/>
+      <c r="G71" s="270"/>
+      <c r="H71" s="271"/>
       <c r="I71" s="44">
         <f>SUM(I61:I70)</f>
         <v>48344</v>
@@ -34614,36 +34705,36 @@
       <c r="M77" s="8"/>
     </row>
     <row r="78" spans="1:13" ht="38.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="262" t="s">
+      <c r="A78" s="263" t="s">
         <v>347</v>
       </c>
-      <c r="B78" s="263"/>
-      <c r="C78" s="263"/>
-      <c r="D78" s="263"/>
-      <c r="E78" s="263"/>
-      <c r="F78" s="263"/>
-      <c r="G78" s="263"/>
-      <c r="H78" s="263"/>
-      <c r="I78" s="264"/>
+      <c r="B78" s="264"/>
+      <c r="C78" s="264"/>
+      <c r="D78" s="264"/>
+      <c r="E78" s="264"/>
+      <c r="F78" s="264"/>
+      <c r="G78" s="264"/>
+      <c r="H78" s="264"/>
+      <c r="I78" s="265"/>
       <c r="J78" s="8"/>
       <c r="K78" s="8"/>
       <c r="L78" s="8"/>
       <c r="M78" s="8"/>
     </row>
     <row r="79" spans="1:13" ht="17.100000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A79" s="265" t="s">
+      <c r="A79" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B79" s="266"/>
-      <c r="C79" s="266"/>
-      <c r="D79" s="267"/>
+      <c r="B79" s="267"/>
+      <c r="C79" s="267"/>
+      <c r="D79" s="268"/>
       <c r="E79" s="43"/>
-      <c r="F79" s="265" t="s">
+      <c r="F79" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G79" s="266"/>
-      <c r="H79" s="266"/>
-      <c r="I79" s="267"/>
+      <c r="G79" s="267"/>
+      <c r="H79" s="267"/>
+      <c r="I79" s="268"/>
       <c r="J79" s="8"/>
       <c r="K79" s="8"/>
       <c r="L79" s="8"/>
@@ -34850,21 +34941,21 @@
       <c r="M90" s="8"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A91" s="268" t="s">
+      <c r="A91" s="269" t="s">
         <v>106</v>
       </c>
-      <c r="B91" s="269"/>
-      <c r="C91" s="269"/>
+      <c r="B91" s="270"/>
+      <c r="C91" s="270"/>
       <c r="D91" s="44">
         <f>SUM(D81:D90)</f>
         <v>239956</v>
       </c>
       <c r="E91" s="50"/>
-      <c r="F91" s="268" t="s">
+      <c r="F91" s="269" t="s">
         <v>105</v>
       </c>
-      <c r="G91" s="269"/>
-      <c r="H91" s="270"/>
+      <c r="G91" s="270"/>
+      <c r="H91" s="271"/>
       <c r="I91" s="44">
         <f>SUM(I81:I90)</f>
         <v>239500</v>
@@ -35784,36 +35875,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>162</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -36204,21 +36295,21 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="287" t="s">
+      <c r="A19" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B19" s="288"/>
-      <c r="C19" s="288"/>
+      <c r="B19" s="289"/>
+      <c r="C19" s="289"/>
       <c r="D19" s="44">
         <f>SUM(D4:D18)</f>
         <v>717500</v>
       </c>
       <c r="E19" s="50"/>
-      <c r="F19" s="287" t="s">
+      <c r="F19" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G19" s="288"/>
-      <c r="H19" s="289"/>
+      <c r="G19" s="289"/>
+      <c r="H19" s="290"/>
       <c r="I19" s="44">
         <f>SUM(I4:I18)</f>
         <v>508500</v>
@@ -36844,36 +36935,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>269</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -37093,21 +37184,21 @@
       <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="287" t="s">
+      <c r="A14" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="288"/>
-      <c r="C14" s="288"/>
+      <c r="B14" s="289"/>
+      <c r="C14" s="289"/>
       <c r="D14" s="44">
         <f>SUM(D4:D13)</f>
         <v>120000</v>
       </c>
       <c r="E14" s="50"/>
-      <c r="F14" s="287" t="s">
+      <c r="F14" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="288"/>
-      <c r="H14" s="289"/>
+      <c r="G14" s="289"/>
+      <c r="H14" s="290"/>
       <c r="I14" s="44">
         <f>SUM(I4:I13)</f>
         <v>120000</v>
@@ -37732,36 +37823,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>266</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -37966,21 +38057,21 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="287" t="s">
+      <c r="A13" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="288"/>
-      <c r="C13" s="288"/>
+      <c r="B13" s="289"/>
+      <c r="C13" s="289"/>
       <c r="D13" s="44">
         <f>SUM(D4:D12)</f>
         <v>260000</v>
       </c>
       <c r="E13" s="50"/>
-      <c r="F13" s="287" t="s">
+      <c r="F13" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="288"/>
-      <c r="H13" s="289"/>
+      <c r="G13" s="289"/>
+      <c r="H13" s="290"/>
       <c r="I13" s="44">
         <f>SUM(I4:I12)</f>
         <v>260000</v>
@@ -38096,36 +38187,36 @@
       <c r="M19" s="8"/>
     </row>
     <row r="20" spans="1:13" ht="40.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A20" s="262" t="s">
+      <c r="A20" s="263" t="s">
         <v>265</v>
       </c>
-      <c r="B20" s="263"/>
-      <c r="C20" s="263"/>
-      <c r="D20" s="263"/>
-      <c r="E20" s="263"/>
-      <c r="F20" s="263"/>
-      <c r="G20" s="263"/>
-      <c r="H20" s="263"/>
-      <c r="I20" s="264"/>
+      <c r="B20" s="264"/>
+      <c r="C20" s="264"/>
+      <c r="D20" s="264"/>
+      <c r="E20" s="264"/>
+      <c r="F20" s="264"/>
+      <c r="G20" s="264"/>
+      <c r="H20" s="264"/>
+      <c r="I20" s="265"/>
       <c r="J20" s="8"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A21" s="265" t="s">
+      <c r="A21" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B21" s="266"/>
-      <c r="C21" s="266"/>
-      <c r="D21" s="267"/>
+      <c r="B21" s="267"/>
+      <c r="C21" s="267"/>
+      <c r="D21" s="268"/>
       <c r="E21" s="43"/>
-      <c r="F21" s="265" t="s">
+      <c r="F21" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G21" s="266"/>
-      <c r="H21" s="266"/>
-      <c r="I21" s="267"/>
+      <c r="G21" s="267"/>
+      <c r="H21" s="267"/>
+      <c r="I21" s="268"/>
       <c r="J21" s="8"/>
       <c r="K21" s="8"/>
       <c r="L21" s="8"/>
@@ -38341,21 +38432,21 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A31" s="287" t="s">
+      <c r="A31" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="288"/>
-      <c r="C31" s="288"/>
+      <c r="B31" s="289"/>
+      <c r="C31" s="289"/>
       <c r="D31" s="44">
         <f>SUM(D23:D30)</f>
         <v>413000</v>
       </c>
       <c r="E31" s="50"/>
-      <c r="F31" s="287" t="s">
+      <c r="F31" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G31" s="288"/>
-      <c r="H31" s="289"/>
+      <c r="G31" s="289"/>
+      <c r="H31" s="290"/>
       <c r="I31" s="44">
         <f>SUM(I23:I30)</f>
         <v>413000</v>
@@ -38500,36 +38591,36 @@
       <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" ht="35.700000000000003" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A40" s="262" t="s">
+      <c r="A40" s="263" t="s">
         <v>272</v>
       </c>
-      <c r="B40" s="263"/>
-      <c r="C40" s="263"/>
-      <c r="D40" s="263"/>
-      <c r="E40" s="263"/>
-      <c r="F40" s="263"/>
-      <c r="G40" s="263"/>
-      <c r="H40" s="263"/>
-      <c r="I40" s="264"/>
+      <c r="B40" s="264"/>
+      <c r="C40" s="264"/>
+      <c r="D40" s="264"/>
+      <c r="E40" s="264"/>
+      <c r="F40" s="264"/>
+      <c r="G40" s="264"/>
+      <c r="H40" s="264"/>
+      <c r="I40" s="265"/>
       <c r="J40" s="8"/>
       <c r="K40" s="8"/>
       <c r="L40" s="8"/>
       <c r="M40" s="8"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A41" s="265" t="s">
+      <c r="A41" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B41" s="266"/>
-      <c r="C41" s="266"/>
-      <c r="D41" s="267"/>
+      <c r="B41" s="267"/>
+      <c r="C41" s="267"/>
+      <c r="D41" s="268"/>
       <c r="E41" s="43"/>
-      <c r="F41" s="265" t="s">
+      <c r="F41" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G41" s="266"/>
-      <c r="H41" s="266"/>
-      <c r="I41" s="267"/>
+      <c r="G41" s="267"/>
+      <c r="H41" s="267"/>
+      <c r="I41" s="268"/>
       <c r="J41" s="8"/>
       <c r="K41" s="8"/>
       <c r="L41" s="8"/>
@@ -38795,21 +38886,21 @@
       <c r="M54" s="8"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A55" s="287" t="s">
+      <c r="A55" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="288"/>
-      <c r="C55" s="288"/>
+      <c r="B55" s="289"/>
+      <c r="C55" s="289"/>
       <c r="D55" s="44">
         <f>SUM(D43:D54)</f>
         <v>1203500</v>
       </c>
       <c r="E55" s="50"/>
-      <c r="F55" s="287" t="s">
+      <c r="F55" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G55" s="288"/>
-      <c r="H55" s="289"/>
+      <c r="G55" s="289"/>
+      <c r="H55" s="290"/>
       <c r="I55" s="44">
         <f>SUM(I43:I54)</f>
         <v>1203500</v>
@@ -38925,36 +39016,36 @@
       <c r="M61" s="8"/>
     </row>
     <row r="62" spans="1:13" ht="35.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A62" s="262" t="s">
+      <c r="A62" s="263" t="s">
         <v>292</v>
       </c>
-      <c r="B62" s="263"/>
-      <c r="C62" s="263"/>
-      <c r="D62" s="263"/>
-      <c r="E62" s="263"/>
-      <c r="F62" s="263"/>
-      <c r="G62" s="263"/>
-      <c r="H62" s="263"/>
-      <c r="I62" s="264"/>
+      <c r="B62" s="264"/>
+      <c r="C62" s="264"/>
+      <c r="D62" s="264"/>
+      <c r="E62" s="264"/>
+      <c r="F62" s="264"/>
+      <c r="G62" s="264"/>
+      <c r="H62" s="264"/>
+      <c r="I62" s="265"/>
       <c r="J62" s="8"/>
       <c r="K62" s="8"/>
       <c r="L62" s="8"/>
       <c r="M62" s="8"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A63" s="265" t="s">
+      <c r="A63" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B63" s="266"/>
-      <c r="C63" s="266"/>
-      <c r="D63" s="267"/>
+      <c r="B63" s="267"/>
+      <c r="C63" s="267"/>
+      <c r="D63" s="268"/>
       <c r="E63" s="43"/>
-      <c r="F63" s="265" t="s">
+      <c r="F63" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G63" s="266"/>
-      <c r="H63" s="266"/>
-      <c r="I63" s="267"/>
+      <c r="G63" s="267"/>
+      <c r="H63" s="267"/>
+      <c r="I63" s="268"/>
       <c r="J63" s="8"/>
       <c r="K63" s="8"/>
       <c r="L63" s="8"/>
@@ -39144,21 +39235,21 @@
       <c r="M72" s="8"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A73" s="287" t="s">
+      <c r="A73" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="288"/>
-      <c r="C73" s="288"/>
+      <c r="B73" s="289"/>
+      <c r="C73" s="289"/>
       <c r="D73" s="44">
         <f>SUM(D65:D72)</f>
         <v>103500</v>
       </c>
       <c r="E73" s="50"/>
-      <c r="F73" s="287" t="s">
+      <c r="F73" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G73" s="288"/>
-      <c r="H73" s="289"/>
+      <c r="G73" s="289"/>
+      <c r="H73" s="290"/>
       <c r="I73" s="44">
         <f>SUM(I65:I72)</f>
         <v>103500</v>
@@ -39274,36 +39365,36 @@
       <c r="M79" s="8"/>
     </row>
     <row r="80" spans="1:13" ht="32.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A80" s="262" t="s">
+      <c r="A80" s="263" t="s">
         <v>365</v>
       </c>
-      <c r="B80" s="263"/>
-      <c r="C80" s="263"/>
-      <c r="D80" s="263"/>
-      <c r="E80" s="263"/>
-      <c r="F80" s="263"/>
-      <c r="G80" s="263"/>
-      <c r="H80" s="263"/>
-      <c r="I80" s="264"/>
+      <c r="B80" s="264"/>
+      <c r="C80" s="264"/>
+      <c r="D80" s="264"/>
+      <c r="E80" s="264"/>
+      <c r="F80" s="264"/>
+      <c r="G80" s="264"/>
+      <c r="H80" s="264"/>
+      <c r="I80" s="265"/>
       <c r="J80" s="8"/>
       <c r="K80" s="8"/>
       <c r="L80" s="8"/>
       <c r="M80" s="8"/>
     </row>
     <row r="81" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A81" s="265" t="s">
+      <c r="A81" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="266"/>
-      <c r="C81" s="266"/>
-      <c r="D81" s="267"/>
+      <c r="B81" s="267"/>
+      <c r="C81" s="267"/>
+      <c r="D81" s="268"/>
       <c r="E81" s="43"/>
-      <c r="F81" s="265" t="s">
+      <c r="F81" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G81" s="266"/>
-      <c r="H81" s="266"/>
-      <c r="I81" s="267"/>
+      <c r="G81" s="267"/>
+      <c r="H81" s="267"/>
+      <c r="I81" s="268"/>
       <c r="J81" s="8"/>
       <c r="K81" s="8"/>
       <c r="L81" s="8"/>
@@ -39493,21 +39584,21 @@
       <c r="M90" s="8"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A91" s="287" t="s">
+      <c r="A91" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B91" s="288"/>
-      <c r="C91" s="288"/>
+      <c r="B91" s="289"/>
+      <c r="C91" s="289"/>
       <c r="D91" s="44">
         <f>SUM(D83:D90)</f>
         <v>120000</v>
       </c>
       <c r="E91" s="50"/>
-      <c r="F91" s="287" t="s">
+      <c r="F91" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G91" s="288"/>
-      <c r="H91" s="289"/>
+      <c r="G91" s="289"/>
+      <c r="H91" s="290"/>
       <c r="I91" s="44">
         <f>SUM(I83:I90)</f>
         <v>120000</v>
@@ -39641,36 +39732,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>156</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -40062,21 +40153,21 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="287" t="s">
+      <c r="A18" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="288"/>
-      <c r="C18" s="288"/>
+      <c r="B18" s="289"/>
+      <c r="C18" s="289"/>
       <c r="D18" s="44">
         <f>SUM(D4:D17)</f>
         <v>15210</v>
       </c>
       <c r="E18" s="50"/>
-      <c r="F18" s="287" t="s">
+      <c r="F18" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="288"/>
-      <c r="H18" s="289"/>
+      <c r="G18" s="289"/>
+      <c r="H18" s="290"/>
       <c r="I18" s="44">
         <f>SUM(I4:I17)</f>
         <v>15210</v>
@@ -40702,36 +40793,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="37.6" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="263" t="s">
         <v>161</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="263"/>
-      <c r="H1" s="263"/>
-      <c r="I1" s="264"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="264"/>
+      <c r="I1" s="265"/>
       <c r="J1" s="8"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
     </row>
     <row r="2" spans="1:13" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A2" s="265" t="s">
+      <c r="A2" s="266" t="s">
         <v>81</v>
       </c>
-      <c r="B2" s="266"/>
-      <c r="C2" s="266"/>
-      <c r="D2" s="267"/>
+      <c r="B2" s="267"/>
+      <c r="C2" s="267"/>
+      <c r="D2" s="268"/>
       <c r="E2" s="43"/>
-      <c r="F2" s="265" t="s">
+      <c r="F2" s="266" t="s">
         <v>82</v>
       </c>
-      <c r="G2" s="266"/>
-      <c r="H2" s="266"/>
-      <c r="I2" s="267"/>
+      <c r="G2" s="267"/>
+      <c r="H2" s="267"/>
+      <c r="I2" s="268"/>
       <c r="J2" s="8"/>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
@@ -40824,21 +40915,21 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="287" t="s">
+      <c r="A7" s="288" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="288"/>
-      <c r="C7" s="288"/>
+      <c r="B7" s="289"/>
+      <c r="C7" s="289"/>
       <c r="D7" s="44">
         <f>SUM(D4:D6)</f>
         <v>0</v>
       </c>
       <c r="E7" s="50"/>
-      <c r="F7" s="287" t="s">
+      <c r="F7" s="288" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="288"/>
-      <c r="H7" s="289"/>
+      <c r="G7" s="289"/>
+      <c r="H7" s="290"/>
       <c r="I7" s="44">
         <f>SUM(I4:I6)</f>
         <v>3000</v>

</xml_diff>

<commit_message>
Mazhar 18 files 1060
</commit_message>
<xml_diff>
--- a/Office Statement Expense & Expenditure.xlsx
+++ b/Office Statement Expense & Expenditure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Najeeb Associates\000FFICE\Office Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0941E80C-DC06-4100-8D64-5AC2C603EDF9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28DBE8A-9DB4-4D19-B0EE-5DE5F2031138}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="904" activeTab="15" xr2:uid="{B2A19E3B-6786-4ED5-96A6-D1A6BAD18668}"/>
   </bookViews>
@@ -2987,7 +2987,13 @@
     <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2996,13 +3002,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="15" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3014,18 +3026,6 @@
     <xf numFmtId="0" fontId="17" fillId="15" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="13" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="13" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="13" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="8" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3035,17 +3035,8 @@
     <xf numFmtId="0" fontId="10" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3065,29 +3056,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3103,6 +3088,21 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -14799,37 +14799,37 @@
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="A86:I86"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="A105:C105"/>
-    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="A140:I140"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="F141:I141"/>
+    <mergeCell ref="A163:C163"/>
+    <mergeCell ref="F163:H163"/>
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="F113:I113"/>
+    <mergeCell ref="A133:C133"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="F56:H56"/>
     <mergeCell ref="A62:I62"/>
     <mergeCell ref="A63:I63"/>
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="F64:I64"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="F79:H79"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="F113:I113"/>
-    <mergeCell ref="A133:C133"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="A140:I140"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="F141:I141"/>
-    <mergeCell ref="A163:C163"/>
-    <mergeCell ref="F163:H163"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="A105:C105"/>
+    <mergeCell ref="F105:H105"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="53" orientation="portrait" r:id="rId1"/>
@@ -14859,18 +14859,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="304" t="s">
+      <c r="A1" s="298" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="305"/>
-      <c r="C1" s="305"/>
+      <c r="B1" s="299"/>
+      <c r="C1" s="299"/>
       <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="306" t="s">
+      <c r="E1" s="291" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="306"/>
+      <c r="F1" s="291"/>
       <c r="G1" s="14">
         <v>50000</v>
       </c>
@@ -14989,17 +14989,17 @@
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A5" s="309">
+      <c r="A5" s="304">
         <v>3</v>
       </c>
-      <c r="B5" s="310">
+      <c r="B5" s="305">
         <v>44063</v>
       </c>
-      <c r="C5" s="311" t="s">
+      <c r="C5" s="306" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="312"/>
-      <c r="E5" s="313"/>
+      <c r="D5" s="307"/>
+      <c r="E5" s="308"/>
       <c r="F5" s="4">
         <v>11640</v>
       </c>
@@ -15021,11 +15021,11 @@
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A6" s="309"/>
-      <c r="B6" s="310"/>
-      <c r="C6" s="311"/>
-      <c r="D6" s="312"/>
-      <c r="E6" s="313"/>
+      <c r="A6" s="304"/>
+      <c r="B6" s="305"/>
+      <c r="C6" s="306"/>
+      <c r="D6" s="307"/>
+      <c r="E6" s="308"/>
       <c r="F6" s="4">
         <v>1700</v>
       </c>
@@ -15047,10 +15047,10 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A7" s="309">
+      <c r="A7" s="304">
         <v>4</v>
       </c>
-      <c r="B7" s="310">
+      <c r="B7" s="305">
         <v>44064</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -15079,8 +15079,8 @@
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A8" s="309"/>
-      <c r="B8" s="310"/>
+      <c r="A8" s="304"/>
+      <c r="B8" s="305"/>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -15141,10 +15141,10 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A10" s="309">
+      <c r="A10" s="304">
         <v>6</v>
       </c>
-      <c r="B10" s="310">
+      <c r="B10" s="305">
         <v>44066</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -15173,8 +15173,8 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A11" s="309"/>
-      <c r="B11" s="310"/>
+      <c r="A11" s="304"/>
+      <c r="B11" s="305"/>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
@@ -15206,7 +15206,7 @@
       <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="310">
+      <c r="B12" s="305">
         <v>44067</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -15238,7 +15238,7 @@
       <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="B13" s="310"/>
+      <c r="B13" s="305"/>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
@@ -15331,12 +15331,12 @@
       <c r="S15" s="8"/>
     </row>
     <row r="16" spans="1:19" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="291" t="s">
+      <c r="A16" s="300" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="291"/>
-      <c r="C16" s="291"/>
-      <c r="D16" s="292"/>
+      <c r="B16" s="300"/>
+      <c r="C16" s="300"/>
+      <c r="D16" s="301"/>
       <c r="E16" s="16">
         <f>SUM(E3:E15)</f>
         <v>0</v>
@@ -15363,10 +15363,10 @@
       <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="293"/>
-      <c r="B17" s="293"/>
-      <c r="C17" s="293"/>
-      <c r="D17" s="294"/>
+      <c r="A17" s="302"/>
+      <c r="B17" s="302"/>
+      <c r="C17" s="302"/>
+      <c r="D17" s="303"/>
       <c r="E17" s="17" t="s">
         <v>61</v>
       </c>
@@ -15411,18 +15411,18 @@
       <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="304" t="s">
+      <c r="A19" s="298" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="305"/>
-      <c r="C19" s="305"/>
+      <c r="B19" s="299"/>
+      <c r="C19" s="299"/>
       <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="306" t="s">
+      <c r="E19" s="291" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="306"/>
+      <c r="F19" s="291"/>
       <c r="G19" s="14">
         <v>31780</v>
       </c>
@@ -15507,10 +15507,10 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A22" s="298">
+      <c r="A22" s="295">
         <v>12</v>
       </c>
-      <c r="B22" s="295">
+      <c r="B22" s="292">
         <v>44076</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -15539,8 +15539,8 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A23" s="299"/>
-      <c r="B23" s="296"/>
+      <c r="A23" s="296"/>
+      <c r="B23" s="293"/>
       <c r="C23" s="21" t="s">
         <v>21</v>
       </c>
@@ -15567,8 +15567,8 @@
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A24" s="300"/>
-      <c r="B24" s="297"/>
+      <c r="A24" s="297"/>
+      <c r="B24" s="294"/>
       <c r="C24" s="21" t="s">
         <v>22</v>
       </c>
@@ -15597,10 +15597,10 @@
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A25" s="298">
+      <c r="A25" s="295">
         <v>13</v>
       </c>
-      <c r="B25" s="295">
+      <c r="B25" s="292">
         <v>44077</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -15631,8 +15631,8 @@
       <c r="S25" s="8"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A26" s="300"/>
-      <c r="B26" s="297"/>
+      <c r="A26" s="297"/>
+      <c r="B26" s="294"/>
       <c r="C26" s="21" t="s">
         <v>26</v>
       </c>
@@ -15661,10 +15661,10 @@
       <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A27" s="298">
+      <c r="A27" s="295">
         <v>14</v>
       </c>
-      <c r="B27" s="295">
+      <c r="B27" s="292">
         <v>44078</v>
       </c>
       <c r="C27" s="21" t="s">
@@ -15693,8 +15693,8 @@
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A28" s="300"/>
-      <c r="B28" s="297"/>
+      <c r="A28" s="297"/>
+      <c r="B28" s="294"/>
       <c r="C28" s="21" t="s">
         <v>28</v>
       </c>
@@ -15723,10 +15723,10 @@
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A29" s="298">
+      <c r="A29" s="295">
         <v>15</v>
       </c>
-      <c r="B29" s="295">
+      <c r="B29" s="292">
         <v>44079</v>
       </c>
       <c r="C29" s="21" t="s">
@@ -15755,8 +15755,8 @@
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A30" s="299"/>
-      <c r="B30" s="296"/>
+      <c r="A30" s="296"/>
+      <c r="B30" s="293"/>
       <c r="C30" s="21" t="s">
         <v>30</v>
       </c>
@@ -15785,8 +15785,8 @@
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A31" s="299"/>
-      <c r="B31" s="296"/>
+      <c r="A31" s="296"/>
+      <c r="B31" s="293"/>
       <c r="C31" s="21" t="s">
         <v>60</v>
       </c>
@@ -15813,8 +15813,8 @@
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A32" s="300"/>
-      <c r="B32" s="297"/>
+      <c r="A32" s="297"/>
+      <c r="B32" s="294"/>
       <c r="C32" s="23" t="s">
         <v>31</v>
       </c>
@@ -15841,10 +15841,10 @@
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A33" s="298">
+      <c r="A33" s="295">
         <v>16</v>
       </c>
-      <c r="B33" s="295">
+      <c r="B33" s="292">
         <v>44080</v>
       </c>
       <c r="C33" s="21" t="s">
@@ -15875,8 +15875,8 @@
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A34" s="299"/>
-      <c r="B34" s="296"/>
+      <c r="A34" s="296"/>
+      <c r="B34" s="293"/>
       <c r="C34" s="21" t="s">
         <v>33</v>
       </c>
@@ -15905,8 +15905,8 @@
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A35" s="299"/>
-      <c r="B35" s="296"/>
+      <c r="A35" s="296"/>
+      <c r="B35" s="293"/>
       <c r="C35" s="21" t="s">
         <v>36</v>
       </c>
@@ -15935,8 +15935,8 @@
       <c r="S35" s="8"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A36" s="299"/>
-      <c r="B36" s="296"/>
+      <c r="A36" s="296"/>
+      <c r="B36" s="293"/>
       <c r="C36" s="21" t="s">
         <v>37</v>
       </c>
@@ -15965,8 +15965,8 @@
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A37" s="300"/>
-      <c r="B37" s="297"/>
+      <c r="A37" s="297"/>
+      <c r="B37" s="294"/>
       <c r="C37" s="21" t="s">
         <v>39</v>
       </c>
@@ -15993,10 +15993,10 @@
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A38" s="298">
+      <c r="A38" s="295">
         <v>17</v>
       </c>
-      <c r="B38" s="295">
+      <c r="B38" s="292">
         <v>44081</v>
       </c>
       <c r="C38" s="21" t="s">
@@ -16025,8 +16025,8 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A39" s="299"/>
-      <c r="B39" s="296"/>
+      <c r="A39" s="296"/>
+      <c r="B39" s="293"/>
       <c r="C39" s="21" t="s">
         <v>28</v>
       </c>
@@ -16053,8 +16053,8 @@
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A40" s="300"/>
-      <c r="B40" s="297"/>
+      <c r="A40" s="297"/>
+      <c r="B40" s="294"/>
       <c r="C40" s="21" t="s">
         <v>40</v>
       </c>
@@ -16083,10 +16083,10 @@
       <c r="S40" s="8"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A41" s="298">
+      <c r="A41" s="295">
         <v>18</v>
       </c>
-      <c r="B41" s="295">
+      <c r="B41" s="292">
         <v>44082</v>
       </c>
       <c r="C41" s="21" t="s">
@@ -16115,8 +16115,8 @@
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A42" s="300"/>
-      <c r="B42" s="297"/>
+      <c r="A42" s="297"/>
+      <c r="B42" s="294"/>
       <c r="C42" s="21" t="s">
         <v>42</v>
       </c>
@@ -16143,10 +16143,10 @@
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A43" s="298">
+      <c r="A43" s="295">
         <v>19</v>
       </c>
-      <c r="B43" s="295">
+      <c r="B43" s="292">
         <v>44083</v>
       </c>
       <c r="C43" s="21" t="s">
@@ -16175,8 +16175,8 @@
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A44" s="300"/>
-      <c r="B44" s="297"/>
+      <c r="A44" s="297"/>
+      <c r="B44" s="294"/>
       <c r="C44" s="21" t="s">
         <v>44</v>
       </c>
@@ -16203,10 +16203,10 @@
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A45" s="298">
+      <c r="A45" s="295">
         <v>20</v>
       </c>
-      <c r="B45" s="295">
+      <c r="B45" s="292">
         <v>44084</v>
       </c>
       <c r="C45" s="21" t="s">
@@ -16235,8 +16235,8 @@
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A46" s="300"/>
-      <c r="B46" s="297"/>
+      <c r="A46" s="297"/>
+      <c r="B46" s="294"/>
       <c r="C46" s="21" t="s">
         <v>45</v>
       </c>
@@ -16263,10 +16263,10 @@
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A47" s="298">
+      <c r="A47" s="295">
         <v>21</v>
       </c>
-      <c r="B47" s="295">
+      <c r="B47" s="292">
         <v>44085</v>
       </c>
       <c r="C47" s="21" t="s">
@@ -16295,8 +16295,8 @@
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A48" s="299"/>
-      <c r="B48" s="296"/>
+      <c r="A48" s="296"/>
+      <c r="B48" s="293"/>
       <c r="C48" s="21" t="s">
         <v>46</v>
       </c>
@@ -16323,8 +16323,8 @@
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A49" s="299"/>
-      <c r="B49" s="296"/>
+      <c r="A49" s="296"/>
+      <c r="B49" s="293"/>
       <c r="C49" s="21" t="s">
         <v>47</v>
       </c>
@@ -16351,8 +16351,8 @@
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A50" s="299"/>
-      <c r="B50" s="296"/>
+      <c r="A50" s="296"/>
+      <c r="B50" s="293"/>
       <c r="C50" s="23" t="s">
         <v>31</v>
       </c>
@@ -16379,8 +16379,8 @@
       <c r="S50" s="8"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A51" s="300"/>
-      <c r="B51" s="297"/>
+      <c r="A51" s="297"/>
+      <c r="B51" s="294"/>
       <c r="C51" s="21" t="s">
         <v>44</v>
       </c>
@@ -16409,10 +16409,10 @@
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A52" s="298">
+      <c r="A52" s="295">
         <v>22</v>
       </c>
-      <c r="B52" s="295">
+      <c r="B52" s="292">
         <v>44086</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -16443,8 +16443,8 @@
       <c r="S52" s="8"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A53" s="300"/>
-      <c r="B53" s="297"/>
+      <c r="A53" s="297"/>
+      <c r="B53" s="294"/>
       <c r="C53" s="21" t="s">
         <v>50</v>
       </c>
@@ -16471,10 +16471,10 @@
       <c r="S53" s="8"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A54" s="298">
+      <c r="A54" s="295">
         <v>23</v>
       </c>
-      <c r="B54" s="295">
+      <c r="B54" s="292">
         <v>44087</v>
       </c>
       <c r="C54" s="21" t="s">
@@ -16503,8 +16503,8 @@
       <c r="S54" s="8"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A55" s="299"/>
-      <c r="B55" s="296"/>
+      <c r="A55" s="296"/>
+      <c r="B55" s="293"/>
       <c r="C55" s="21" t="s">
         <v>28</v>
       </c>
@@ -16531,8 +16531,8 @@
       <c r="S55" s="8"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A56" s="299"/>
-      <c r="B56" s="296"/>
+      <c r="A56" s="296"/>
+      <c r="B56" s="293"/>
       <c r="C56" s="21" t="s">
         <v>51</v>
       </c>
@@ -16559,8 +16559,8 @@
       <c r="S56" s="8"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A57" s="299"/>
-      <c r="B57" s="296"/>
+      <c r="A57" s="296"/>
+      <c r="B57" s="293"/>
       <c r="C57" s="23" t="s">
         <v>31</v>
       </c>
@@ -16685,10 +16685,10 @@
       <c r="S60" s="8"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A61" s="298">
+      <c r="A61" s="295">
         <v>27</v>
       </c>
-      <c r="B61" s="295">
+      <c r="B61" s="292">
         <v>44091</v>
       </c>
       <c r="C61" s="21" t="s">
@@ -16717,8 +16717,8 @@
       <c r="S61" s="8"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A62" s="300"/>
-      <c r="B62" s="297"/>
+      <c r="A62" s="297"/>
+      <c r="B62" s="294"/>
       <c r="C62" s="21" t="s">
         <v>44</v>
       </c>
@@ -16777,10 +16777,10 @@
       <c r="S63" s="8"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A64" s="298">
+      <c r="A64" s="295">
         <v>29</v>
       </c>
-      <c r="B64" s="295">
+      <c r="B64" s="292">
         <v>44093</v>
       </c>
       <c r="C64" s="21" t="s">
@@ -16809,8 +16809,8 @@
       <c r="S64" s="8"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A65" s="300"/>
-      <c r="B65" s="297"/>
+      <c r="A65" s="297"/>
+      <c r="B65" s="294"/>
       <c r="C65" s="21" t="s">
         <v>18</v>
       </c>
@@ -17005,10 +17005,10 @@
       <c r="B71" s="28">
         <v>44101</v>
       </c>
-      <c r="C71" s="307" t="s">
+      <c r="C71" s="309" t="s">
         <v>65</v>
       </c>
-      <c r="D71" s="308"/>
+      <c r="D71" s="310"/>
       <c r="E71" s="26">
         <v>0</v>
       </c>
@@ -17033,10 +17033,10 @@
       <c r="S71" s="8"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A72" s="298">
+      <c r="A72" s="295">
         <v>37</v>
       </c>
-      <c r="B72" s="295">
+      <c r="B72" s="292">
         <v>44103</v>
       </c>
       <c r="C72" s="21" t="s">
@@ -17065,12 +17065,12 @@
       <c r="S72" s="8"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A73" s="300"/>
-      <c r="B73" s="297"/>
-      <c r="C73" s="307" t="s">
+      <c r="A73" s="297"/>
+      <c r="B73" s="294"/>
+      <c r="C73" s="309" t="s">
         <v>75</v>
       </c>
-      <c r="D73" s="308"/>
+      <c r="D73" s="310"/>
       <c r="E73" s="6">
         <v>100000</v>
       </c>
@@ -17127,12 +17127,12 @@
       <c r="S74" s="8"/>
     </row>
     <row r="75" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A75" s="291" t="s">
+      <c r="A75" s="300" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="291"/>
-      <c r="C75" s="291"/>
-      <c r="D75" s="292"/>
+      <c r="B75" s="300"/>
+      <c r="C75" s="300"/>
+      <c r="D75" s="301"/>
       <c r="E75" s="16">
         <f>SUM(E21:E74)</f>
         <v>132000</v>
@@ -17159,10 +17159,10 @@
       <c r="S75" s="8"/>
     </row>
     <row r="76" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="293"/>
-      <c r="B76" s="293"/>
-      <c r="C76" s="293"/>
-      <c r="D76" s="294"/>
+      <c r="A76" s="302"/>
+      <c r="B76" s="302"/>
+      <c r="C76" s="302"/>
+      <c r="D76" s="303"/>
       <c r="E76" s="17" t="s">
         <v>61</v>
       </c>
@@ -17207,18 +17207,18 @@
       <c r="S77" s="8"/>
     </row>
     <row r="78" spans="1:19" ht="27.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="304" t="s">
+      <c r="A78" s="298" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="305"/>
-      <c r="C78" s="305"/>
+      <c r="B78" s="299"/>
+      <c r="C78" s="299"/>
       <c r="D78" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E78" s="306" t="s">
+      <c r="E78" s="291" t="s">
         <v>0</v>
       </c>
-      <c r="F78" s="306"/>
+      <c r="F78" s="291"/>
       <c r="G78" s="14">
         <f>G75</f>
         <v>137640</v>
@@ -17272,10 +17272,10 @@
       <c r="S79" s="8"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A80" s="298">
+      <c r="A80" s="295">
         <v>39</v>
       </c>
-      <c r="B80" s="295">
+      <c r="B80" s="292">
         <v>44105</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -17304,8 +17304,8 @@
       <c r="S80" s="8"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A81" s="299"/>
-      <c r="B81" s="296"/>
+      <c r="A81" s="296"/>
+      <c r="B81" s="293"/>
       <c r="C81" s="1" t="s">
         <v>70</v>
       </c>
@@ -17332,8 +17332,8 @@
       <c r="S81" s="8"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A82" s="299"/>
-      <c r="B82" s="296"/>
+      <c r="A82" s="296"/>
+      <c r="B82" s="293"/>
       <c r="C82" s="34" t="s">
         <v>76</v>
       </c>
@@ -17362,9 +17362,9 @@
       <c r="S82" s="8"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A83" s="299"/>
-      <c r="B83" s="296"/>
-      <c r="C83" s="301" t="s">
+      <c r="A83" s="296"/>
+      <c r="B83" s="293"/>
+      <c r="C83" s="311" t="s">
         <v>77</v>
       </c>
       <c r="D83" s="32" t="s">
@@ -17392,9 +17392,9 @@
       <c r="S83" s="8"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A84" s="299"/>
-      <c r="B84" s="296"/>
-      <c r="C84" s="302"/>
+      <c r="A84" s="296"/>
+      <c r="B84" s="293"/>
+      <c r="C84" s="312"/>
       <c r="D84" s="32" t="s">
         <v>71</v>
       </c>
@@ -17420,9 +17420,9 @@
       <c r="S84" s="8"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A85" s="299"/>
-      <c r="B85" s="296"/>
-      <c r="C85" s="302"/>
+      <c r="A85" s="296"/>
+      <c r="B85" s="293"/>
+      <c r="C85" s="312"/>
       <c r="D85" s="32" t="s">
         <v>73</v>
       </c>
@@ -17448,9 +17448,9 @@
       <c r="S85" s="8"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A86" s="300"/>
-      <c r="B86" s="297"/>
-      <c r="C86" s="303"/>
+      <c r="A86" s="297"/>
+      <c r="B86" s="294"/>
+      <c r="C86" s="313"/>
       <c r="D86" s="32" t="s">
         <v>74</v>
       </c>
@@ -17508,10 +17508,10 @@
       <c r="S87" s="8"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A88" s="298">
+      <c r="A88" s="295">
         <v>41</v>
       </c>
-      <c r="B88" s="295">
+      <c r="B88" s="292">
         <v>44108</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -17540,8 +17540,8 @@
       <c r="S88" s="8"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A89" s="300"/>
-      <c r="B89" s="297"/>
+      <c r="A89" s="297"/>
+      <c r="B89" s="294"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="4"/>
@@ -17630,10 +17630,10 @@
       <c r="S91" s="8"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A92" s="298">
+      <c r="A92" s="295">
         <v>44</v>
       </c>
-      <c r="B92" s="295">
+      <c r="B92" s="292">
         <v>44112</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -17662,8 +17662,8 @@
       <c r="S92" s="8"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A93" s="299"/>
-      <c r="B93" s="296"/>
+      <c r="A93" s="296"/>
+      <c r="B93" s="293"/>
       <c r="C93" s="1" t="s">
         <v>113</v>
       </c>
@@ -17690,8 +17690,8 @@
       <c r="S93" s="8"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A94" s="299"/>
-      <c r="B94" s="296"/>
+      <c r="A94" s="296"/>
+      <c r="B94" s="293"/>
       <c r="C94" s="1" t="s">
         <v>98</v>
       </c>
@@ -17720,8 +17720,8 @@
       <c r="S94" s="8"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A95" s="300"/>
-      <c r="B95" s="297"/>
+      <c r="A95" s="297"/>
+      <c r="B95" s="294"/>
       <c r="C95" s="1" t="s">
         <v>111</v>
       </c>
@@ -18180,12 +18180,12 @@
       <c r="S113" s="8"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A114" s="291" t="s">
+      <c r="A114" s="300" t="s">
         <v>57</v>
       </c>
-      <c r="B114" s="291"/>
-      <c r="C114" s="291"/>
-      <c r="D114" s="292"/>
+      <c r="B114" s="300"/>
+      <c r="C114" s="300"/>
+      <c r="D114" s="301"/>
       <c r="E114" s="16">
         <f>SUM(E80:E113)</f>
         <v>600000</v>
@@ -18212,10 +18212,10 @@
       <c r="S114" s="8"/>
     </row>
     <row r="115" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="293"/>
-      <c r="B115" s="293"/>
-      <c r="C115" s="293"/>
-      <c r="D115" s="294"/>
+      <c r="A115" s="302"/>
+      <c r="B115" s="302"/>
+      <c r="C115" s="302"/>
+      <c r="D115" s="303"/>
       <c r="E115" s="17" t="s">
         <v>61</v>
       </c>
@@ -21397,50 +21397,6 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="A16:D17"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="C73:D73"/>
     <mergeCell ref="A114:D115"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A38:A40"/>
@@ -21455,6 +21411,50 @@
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="B92:B95"/>
     <mergeCell ref="A92:A95"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A16:D17"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="73" orientation="portrait" r:id="rId1"/>
@@ -24408,7 +24408,7 @@
   <dimension ref="B2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -31880,19 +31880,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="281" t="s">
+      <c r="A1" s="285" t="s">
         <v>307</v>
       </c>
-      <c r="B1" s="282"/>
-      <c r="C1" s="282"/>
-      <c r="D1" s="282"/>
-      <c r="E1" s="283"/>
-      <c r="G1" s="280" t="s">
+      <c r="B1" s="286"/>
+      <c r="C1" s="286"/>
+      <c r="D1" s="286"/>
+      <c r="E1" s="287"/>
+      <c r="G1" s="283" t="s">
         <v>429</v>
       </c>
-      <c r="H1" s="280"/>
-      <c r="I1" s="280"/>
-      <c r="J1" s="280"/>
+      <c r="H1" s="283"/>
+      <c r="I1" s="283"/>
+      <c r="J1" s="283"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -31914,18 +31914,18 @@
         <v>4</v>
       </c>
       <c r="F2" s="238"/>
-      <c r="G2" s="275" t="s">
+      <c r="G2" s="284" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="275"/>
-      <c r="I2" s="275"/>
-      <c r="J2" s="275"/>
+      <c r="H2" s="284"/>
+      <c r="I2" s="284"/>
+      <c r="J2" s="284"/>
       <c r="K2" s="238"/>
       <c r="L2" s="238"/>
       <c r="M2" s="238"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A3" s="276">
+      <c r="A3" s="278">
         <v>1</v>
       </c>
       <c r="B3" s="211">
@@ -31937,7 +31937,7 @@
       <c r="D3" s="209">
         <v>30000</v>
       </c>
-      <c r="E3" s="278">
+      <c r="E3" s="276">
         <f>D4-D3</f>
         <v>-30000</v>
       </c>
@@ -31958,11 +31958,11 @@
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A4" s="277"/>
+      <c r="A4" s="279"/>
       <c r="B4" s="213"/>
       <c r="C4" s="214"/>
       <c r="D4" s="210"/>
-      <c r="E4" s="279"/>
+      <c r="E4" s="277"/>
       <c r="G4" s="230">
         <v>1</v>
       </c>
@@ -31998,7 +31998,7 @@
       <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A6" s="276">
+      <c r="A6" s="278">
         <v>2</v>
       </c>
       <c r="B6" s="211">
@@ -32010,7 +32010,7 @@
       <c r="D6" s="209">
         <v>5000</v>
       </c>
-      <c r="E6" s="278">
+      <c r="E6" s="276">
         <f>D7-D6</f>
         <v>-5000</v>
       </c>
@@ -32031,11 +32031,11 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A7" s="277"/>
+      <c r="A7" s="279"/>
       <c r="B7" s="213"/>
       <c r="C7" s="214"/>
       <c r="D7" s="210"/>
-      <c r="E7" s="279"/>
+      <c r="E7" s="277"/>
       <c r="G7" s="230">
         <v>3</v>
       </c>
@@ -32071,7 +32071,7 @@
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A9" s="276">
+      <c r="A9" s="278">
         <v>4</v>
       </c>
       <c r="B9" s="211">
@@ -32083,7 +32083,7 @@
       <c r="D9" s="209">
         <v>3070</v>
       </c>
-      <c r="E9" s="278">
+      <c r="E9" s="276">
         <f>D10-D9</f>
         <v>-3070</v>
       </c>
@@ -32104,11 +32104,11 @@
       <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A10" s="277"/>
+      <c r="A10" s="279"/>
       <c r="B10" s="213"/>
       <c r="C10" s="214"/>
       <c r="D10" s="210"/>
-      <c r="E10" s="279"/>
+      <c r="E10" s="277"/>
       <c r="G10" s="230">
         <v>5</v>
       </c>
@@ -32148,7 +32148,7 @@
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A12" s="276">
+      <c r="A12" s="278">
         <v>5</v>
       </c>
       <c r="B12" s="211">
@@ -32160,7 +32160,7 @@
       <c r="D12" s="209">
         <v>5000</v>
       </c>
-      <c r="E12" s="278">
+      <c r="E12" s="276">
         <f>D13-D12</f>
         <v>-5000</v>
       </c>
@@ -32181,11 +32181,11 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A13" s="277"/>
+      <c r="A13" s="279"/>
       <c r="B13" s="213"/>
       <c r="C13" s="214"/>
       <c r="D13" s="210"/>
-      <c r="E13" s="279"/>
+      <c r="E13" s="277"/>
       <c r="G13" s="1"/>
       <c r="H13" s="233"/>
       <c r="I13" s="1"/>
@@ -32209,7 +32209,7 @@
       <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A15" s="276">
+      <c r="A15" s="278">
         <v>6</v>
       </c>
       <c r="B15" s="211">
@@ -32221,7 +32221,7 @@
       <c r="D15" s="209">
         <v>5000</v>
       </c>
-      <c r="E15" s="278">
+      <c r="E15" s="276">
         <f>D16-D15</f>
         <v>-5000</v>
       </c>
@@ -32234,11 +32234,11 @@
       <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A16" s="277"/>
+      <c r="A16" s="279"/>
       <c r="B16" s="213"/>
       <c r="C16" s="214"/>
       <c r="D16" s="210"/>
-      <c r="E16" s="279"/>
+      <c r="E16" s="277"/>
       <c r="G16" s="1"/>
       <c r="H16" s="234"/>
       <c r="I16" s="1"/>
@@ -32262,7 +32262,7 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A18" s="276">
+      <c r="A18" s="278">
         <v>7</v>
       </c>
       <c r="B18" s="211">
@@ -32274,7 +32274,7 @@
       <c r="D18" s="209">
         <v>5000</v>
       </c>
-      <c r="E18" s="278">
+      <c r="E18" s="276">
         <f>D19-D18</f>
         <v>-5000</v>
       </c>
@@ -32292,11 +32292,11 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A19" s="277"/>
+      <c r="A19" s="279"/>
       <c r="B19" s="213"/>
       <c r="C19" s="214"/>
       <c r="D19" s="210"/>
-      <c r="E19" s="279"/>
+      <c r="E19" s="277"/>
       <c r="G19" s="55"/>
       <c r="H19" s="236"/>
       <c r="I19" s="55"/>
@@ -32311,18 +32311,18 @@
       <c r="C20" s="8"/>
       <c r="D20" s="240"/>
       <c r="E20" s="242"/>
-      <c r="G20" s="275" t="s">
+      <c r="G20" s="284" t="s">
         <v>411</v>
       </c>
-      <c r="H20" s="275"/>
-      <c r="I20" s="275"/>
-      <c r="J20" s="275"/>
+      <c r="H20" s="284"/>
+      <c r="I20" s="284"/>
+      <c r="J20" s="284"/>
       <c r="K20" s="8"/>
       <c r="L20" s="8"/>
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A21" s="276">
+      <c r="A21" s="278">
         <v>8</v>
       </c>
       <c r="B21" s="211">
@@ -32334,7 +32334,7 @@
       <c r="D21" s="209">
         <v>600</v>
       </c>
-      <c r="E21" s="278">
+      <c r="E21" s="276">
         <f>D22-D21</f>
         <v>-600</v>
       </c>
@@ -32355,11 +32355,11 @@
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A22" s="277"/>
+      <c r="A22" s="279"/>
       <c r="B22" s="213"/>
       <c r="C22" s="214"/>
       <c r="D22" s="210"/>
-      <c r="E22" s="279"/>
+      <c r="E22" s="277"/>
       <c r="G22" s="231">
         <v>1</v>
       </c>
@@ -32399,7 +32399,7 @@
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A24" s="276">
+      <c r="A24" s="278">
         <v>9</v>
       </c>
       <c r="B24" s="211">
@@ -32411,7 +32411,7 @@
       <c r="D24" s="209">
         <v>5000</v>
       </c>
-      <c r="E24" s="278">
+      <c r="E24" s="276">
         <f>D25-D24</f>
         <v>-5000</v>
       </c>
@@ -32424,11 +32424,11 @@
       <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A25" s="277"/>
+      <c r="A25" s="279"/>
       <c r="B25" s="213"/>
       <c r="C25" s="214"/>
       <c r="D25" s="210"/>
-      <c r="E25" s="279"/>
+      <c r="E25" s="277"/>
       <c r="G25" s="231"/>
       <c r="H25" s="234"/>
       <c r="I25" s="1"/>
@@ -32452,7 +32452,7 @@
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A27" s="276">
+      <c r="A27" s="278">
         <v>10</v>
       </c>
       <c r="B27" s="211">
@@ -32464,7 +32464,7 @@
       <c r="D27" s="209">
         <v>5000</v>
       </c>
-      <c r="E27" s="278">
+      <c r="E27" s="276">
         <f>D28-D27</f>
         <v>-5000</v>
       </c>
@@ -32477,11 +32477,11 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A28" s="277"/>
+      <c r="A28" s="279"/>
       <c r="B28" s="213"/>
       <c r="C28" s="214"/>
       <c r="D28" s="210"/>
-      <c r="E28" s="279"/>
+      <c r="E28" s="277"/>
       <c r="G28" s="231"/>
       <c r="H28" s="234"/>
       <c r="I28" s="1"/>
@@ -32505,7 +32505,7 @@
       <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A30" s="276">
+      <c r="A30" s="278">
         <v>11</v>
       </c>
       <c r="B30" s="211">
@@ -32517,7 +32517,7 @@
       <c r="D30" s="209">
         <v>5000</v>
       </c>
-      <c r="E30" s="278">
+      <c r="E30" s="276">
         <f>D31-D30</f>
         <v>-5000</v>
       </c>
@@ -32530,11 +32530,11 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A31" s="277"/>
+      <c r="A31" s="279"/>
       <c r="B31" s="213"/>
       <c r="C31" s="214"/>
       <c r="D31" s="210"/>
-      <c r="E31" s="279"/>
+      <c r="E31" s="277"/>
       <c r="G31" s="1"/>
       <c r="H31" s="233"/>
       <c r="I31" s="1"/>
@@ -32558,13 +32558,13 @@
       <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A33" s="276">
+      <c r="A33" s="278">
         <v>12</v>
       </c>
       <c r="B33" s="211"/>
       <c r="C33" s="212"/>
       <c r="D33" s="209"/>
-      <c r="E33" s="278">
+      <c r="E33" s="276">
         <f>D34-D33</f>
         <v>0</v>
       </c>
@@ -32577,11 +32577,11 @@
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A34" s="277"/>
+      <c r="A34" s="279"/>
       <c r="B34" s="213"/>
       <c r="C34" s="214"/>
       <c r="D34" s="210"/>
-      <c r="E34" s="279"/>
+      <c r="E34" s="277"/>
       <c r="G34" s="1"/>
       <c r="H34" s="234"/>
       <c r="I34" s="1"/>
@@ -32605,13 +32605,13 @@
       <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A36" s="276">
+      <c r="A36" s="278">
         <v>13</v>
       </c>
       <c r="B36" s="211"/>
       <c r="C36" s="212"/>
       <c r="D36" s="209"/>
-      <c r="E36" s="278">
+      <c r="E36" s="276">
         <f>D37-D36</f>
         <v>0</v>
       </c>
@@ -32629,11 +32629,11 @@
       <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A37" s="277"/>
+      <c r="A37" s="279"/>
       <c r="B37" s="213"/>
       <c r="C37" s="214"/>
       <c r="D37" s="210"/>
-      <c r="E37" s="279"/>
+      <c r="E37" s="277"/>
       <c r="G37" s="8"/>
       <c r="H37" s="241"/>
       <c r="I37" s="8"/>
@@ -32657,13 +32657,13 @@
       <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A39" s="276">
+      <c r="A39" s="278">
         <v>14</v>
       </c>
       <c r="B39" s="211"/>
       <c r="C39" s="212"/>
       <c r="D39" s="209"/>
-      <c r="E39" s="278">
+      <c r="E39" s="276">
         <f>D40-D39</f>
         <v>0</v>
       </c>
@@ -32676,11 +32676,11 @@
       <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A40" s="277"/>
+      <c r="A40" s="279"/>
       <c r="B40" s="213"/>
       <c r="C40" s="214"/>
       <c r="D40" s="210"/>
-      <c r="E40" s="279"/>
+      <c r="E40" s="277"/>
       <c r="G40" s="8"/>
       <c r="H40" s="241"/>
       <c r="I40" s="8"/>
@@ -32704,13 +32704,13 @@
       <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A42" s="276">
+      <c r="A42" s="278">
         <v>15</v>
       </c>
       <c r="B42" s="211"/>
       <c r="C42" s="212"/>
       <c r="D42" s="209"/>
-      <c r="E42" s="278">
+      <c r="E42" s="276">
         <f>D43-D42</f>
         <v>0</v>
       </c>
@@ -32723,11 +32723,11 @@
       <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A43" s="277"/>
+      <c r="A43" s="279"/>
       <c r="B43" s="213"/>
       <c r="C43" s="214"/>
       <c r="D43" s="210"/>
-      <c r="E43" s="279"/>
+      <c r="E43" s="277"/>
       <c r="G43" s="8"/>
       <c r="H43" s="241"/>
       <c r="I43" s="8"/>
@@ -32751,12 +32751,12 @@
       <c r="M44" s="8"/>
     </row>
     <row r="45" spans="1:13" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="285" t="s">
+      <c r="A45" s="280" t="s">
         <v>412</v>
       </c>
-      <c r="B45" s="286"/>
-      <c r="C45" s="286"/>
-      <c r="D45" s="287"/>
+      <c r="B45" s="281"/>
+      <c r="C45" s="281"/>
+      <c r="D45" s="282"/>
       <c r="E45" s="219">
         <f>SUM(E3:E44)</f>
         <v>-68670</v>
@@ -32773,8 +32773,8 @@
       <c r="A46" s="79"/>
       <c r="B46" s="239"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="284"/>
-      <c r="E46" s="284"/>
+      <c r="D46" s="275"/>
+      <c r="E46" s="275"/>
       <c r="G46" s="8"/>
       <c r="H46" s="241"/>
       <c r="I46" s="8"/>
@@ -32959,15 +32959,17 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G18:I18"/>
@@ -32984,17 +32986,15 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="E42:E43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -35822,11 +35822,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="A78:I78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="F91:H91"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="A51:C51"/>
@@ -35842,11 +35842,11 @@
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="A78:I78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="F71:H71"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -39680,31 +39680,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="F73:H73"/>
     <mergeCell ref="A80:I80"/>
     <mergeCell ref="A81:D81"/>
     <mergeCell ref="F81:I81"/>
     <mergeCell ref="A91:C91"/>
     <mergeCell ref="F91:H91"/>
-    <mergeCell ref="A62:I62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="F55:H55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update Office Statement Expense & Expenditure.xlsx
</commit_message>
<xml_diff>
--- a/Office Statement Expense & Expenditure.xlsx
+++ b/Office Statement Expense & Expenditure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Najeeb Associates\000FFICE\Office Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F4988E-AC2C-420A-8C1B-168B9BA76BEE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BEAA58B-E5A6-44C1-8CC0-290AC054FFFE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="820" activeTab="16" xr2:uid="{B2A19E3B-6786-4ED5-96A6-D1A6BAD18668}"/>
   </bookViews>
@@ -3526,8 +3526,8 @@
   </sheetPr>
   <dimension ref="A1:N897"/>
   <sheetViews>
-    <sheetView topLeftCell="A174" zoomScale="133" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H199" sqref="H199"/>
+    <sheetView topLeftCell="A165" zoomScale="133" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="C180" sqref="C180"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -7620,12 +7620,14 @@
         <v>1</v>
       </c>
       <c r="B176" s="39">
-        <v>44295</v>
+        <v>44297</v>
       </c>
       <c r="C176" s="1" t="s">
         <v>346</v>
       </c>
-      <c r="D176" s="263"/>
+      <c r="D176" s="263">
+        <v>600</v>
+      </c>
       <c r="E176" s="38"/>
       <c r="F176" s="273"/>
       <c r="G176" s="39"/>
@@ -8001,7 +8003,7 @@
       <c r="C197" s="283"/>
       <c r="D197" s="44">
         <f>SUM(D175:D196)</f>
-        <v>1446419</v>
+        <v>1447019</v>
       </c>
       <c r="E197" s="50"/>
       <c r="F197" s="282" t="s">
@@ -8043,7 +8045,7 @@
       </c>
       <c r="D199" s="58">
         <f>D197</f>
-        <v>1446419</v>
+        <v>1447019</v>
       </c>
       <c r="E199" s="8"/>
       <c r="F199" s="53"/>
@@ -8101,7 +8103,7 @@
       </c>
       <c r="D202" s="62">
         <f>D199-D200</f>
-        <v>1439579</v>
+        <v>1440179</v>
       </c>
       <c r="E202" s="8"/>
       <c r="F202" s="8"/>
@@ -25459,7 +25461,7 @@
   <dimension ref="B2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -25722,7 +25724,7 @@
   <dimension ref="E4:P34"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="122" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -25780,14 +25782,14 @@
         <v>431</v>
       </c>
       <c r="L6" s="72">
-        <v>450000</v>
+        <v>50000</v>
       </c>
       <c r="N6" t="s">
         <v>442</v>
       </c>
       <c r="O6" s="179">
         <f>O4-L19</f>
-        <v>320000</v>
+        <v>770000</v>
       </c>
     </row>
     <row r="7" spans="5:15" x14ac:dyDescent="0.5">
@@ -25858,9 +25860,7 @@
       <c r="K14" t="s">
         <v>444</v>
       </c>
-      <c r="L14" s="72">
-        <v>50000</v>
-      </c>
+      <c r="L14" s="72"/>
     </row>
     <row r="15" spans="5:15" x14ac:dyDescent="0.5">
       <c r="L15" s="179"/>
@@ -25880,7 +25880,7 @@
     <row r="19" spans="11:16" x14ac:dyDescent="0.5">
       <c r="L19" s="72">
         <f>SUM(L6:L18)</f>
-        <v>880000</v>
+        <v>430000</v>
       </c>
     </row>
     <row r="27" spans="11:16" x14ac:dyDescent="0.5">

</xml_diff>

<commit_message>
Received 17k back from muzammil
</commit_message>
<xml_diff>
--- a/Office Statement Expense & Expenditure.xlsx
+++ b/Office Statement Expense & Expenditure.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Najeeb Associates\000FFICE\Office Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F906A30D-FF66-4932-A14B-CF80BB62D47C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86A69FD8-4A26-4ECC-8AB8-01B0957E1066}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="820" activeTab="15" xr2:uid="{B2A19E3B-6786-4ED5-96A6-D1A6BAD18668}"/>
   </bookViews>
@@ -264,7 +264,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="978" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="979" uniqueCount="471">
   <si>
     <t>Opning Balance</t>
   </si>
@@ -1675,6 +1675,9 @@
   <si>
     <t>Hanovered 5k to Ibtesam - he said Kamil told</t>
   </si>
+  <si>
+    <t>Received Cash Back 17k taken for a short while now cleared</t>
+  </si>
 </sst>
 </file>
 
@@ -3052,16 +3055,28 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3088,35 +3103,14 @@
     <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3136,29 +3130,23 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3174,6 +3162,21 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -15108,42 +15111,42 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="A172:I172"/>
-    <mergeCell ref="A173:D173"/>
-    <mergeCell ref="F173:I173"/>
-    <mergeCell ref="A197:C197"/>
-    <mergeCell ref="F197:H197"/>
-    <mergeCell ref="A86:I86"/>
-    <mergeCell ref="A87:D87"/>
-    <mergeCell ref="F87:I87"/>
-    <mergeCell ref="A105:C105"/>
-    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="A140:I140"/>
+    <mergeCell ref="A141:D141"/>
+    <mergeCell ref="F141:I141"/>
+    <mergeCell ref="A165:C165"/>
+    <mergeCell ref="F165:H165"/>
+    <mergeCell ref="A112:I112"/>
+    <mergeCell ref="A113:D113"/>
+    <mergeCell ref="F113:I113"/>
+    <mergeCell ref="A133:C133"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="A34:C34"/>
+    <mergeCell ref="A41:I41"/>
+    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="F42:I42"/>
+    <mergeCell ref="A56:C56"/>
+    <mergeCell ref="F56:H56"/>
     <mergeCell ref="A62:I62"/>
     <mergeCell ref="A63:I63"/>
     <mergeCell ref="A64:D64"/>
     <mergeCell ref="F64:I64"/>
     <mergeCell ref="A79:C79"/>
     <mergeCell ref="F79:H79"/>
-    <mergeCell ref="A41:I41"/>
-    <mergeCell ref="A42:D42"/>
-    <mergeCell ref="F42:I42"/>
-    <mergeCell ref="A56:C56"/>
-    <mergeCell ref="F56:H56"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="A34:C34"/>
-    <mergeCell ref="A112:I112"/>
-    <mergeCell ref="A113:D113"/>
-    <mergeCell ref="F113:I113"/>
-    <mergeCell ref="A133:C133"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="A140:I140"/>
-    <mergeCell ref="A141:D141"/>
-    <mergeCell ref="F141:I141"/>
-    <mergeCell ref="A165:C165"/>
-    <mergeCell ref="F165:H165"/>
+    <mergeCell ref="A86:I86"/>
+    <mergeCell ref="A87:D87"/>
+    <mergeCell ref="F87:I87"/>
+    <mergeCell ref="A105:C105"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="A172:I172"/>
+    <mergeCell ref="A173:D173"/>
+    <mergeCell ref="F173:I173"/>
+    <mergeCell ref="A197:C197"/>
+    <mergeCell ref="F197:H197"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="53" orientation="portrait" r:id="rId1"/>
@@ -15594,21 +15597,21 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="283" t="s">
+      <c r="A18" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="284"/>
-      <c r="C18" s="284"/>
+      <c r="B18" s="288"/>
+      <c r="C18" s="288"/>
       <c r="D18" s="44">
         <f>SUM(D4:D17)</f>
         <v>15210</v>
       </c>
       <c r="E18" s="50"/>
-      <c r="F18" s="283" t="s">
+      <c r="F18" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="284"/>
-      <c r="H18" s="285"/>
+      <c r="G18" s="288"/>
+      <c r="H18" s="289"/>
       <c r="I18" s="44">
         <f>SUM(I4:I17)</f>
         <v>15210</v>
@@ -16356,21 +16359,21 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="283" t="s">
+      <c r="A7" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="284"/>
-      <c r="C7" s="284"/>
+      <c r="B7" s="288"/>
+      <c r="C7" s="288"/>
       <c r="D7" s="44">
         <f>SUM(D4:D6)</f>
         <v>0</v>
       </c>
       <c r="E7" s="50"/>
-      <c r="F7" s="283" t="s">
+      <c r="F7" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="284"/>
-      <c r="H7" s="285"/>
+      <c r="G7" s="288"/>
+      <c r="H7" s="289"/>
       <c r="I7" s="44">
         <f>SUM(I4:I6)</f>
         <v>3000</v>
@@ -16997,18 +17000,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="308" t="s">
+      <c r="A1" s="302" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="309"/>
-      <c r="C1" s="309"/>
+      <c r="B1" s="303"/>
+      <c r="C1" s="303"/>
       <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="310" t="s">
+      <c r="E1" s="295" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="310"/>
+      <c r="F1" s="295"/>
       <c r="G1" s="14">
         <v>50000</v>
       </c>
@@ -17127,17 +17130,17 @@
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A5" s="313">
+      <c r="A5" s="308">
         <v>3</v>
       </c>
-      <c r="B5" s="314">
+      <c r="B5" s="309">
         <v>44063</v>
       </c>
-      <c r="C5" s="315" t="s">
+      <c r="C5" s="310" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="316"/>
-      <c r="E5" s="317"/>
+      <c r="D5" s="311"/>
+      <c r="E5" s="312"/>
       <c r="F5" s="4">
         <v>11640</v>
       </c>
@@ -17159,11 +17162,11 @@
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A6" s="313"/>
-      <c r="B6" s="314"/>
-      <c r="C6" s="315"/>
-      <c r="D6" s="316"/>
-      <c r="E6" s="317"/>
+      <c r="A6" s="308"/>
+      <c r="B6" s="309"/>
+      <c r="C6" s="310"/>
+      <c r="D6" s="311"/>
+      <c r="E6" s="312"/>
       <c r="F6" s="4">
         <v>1700</v>
       </c>
@@ -17185,10 +17188,10 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A7" s="313">
+      <c r="A7" s="308">
         <v>4</v>
       </c>
-      <c r="B7" s="314">
+      <c r="B7" s="309">
         <v>44064</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -17217,8 +17220,8 @@
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A8" s="313"/>
-      <c r="B8" s="314"/>
+      <c r="A8" s="308"/>
+      <c r="B8" s="309"/>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -17279,10 +17282,10 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A10" s="313">
+      <c r="A10" s="308">
         <v>6</v>
       </c>
-      <c r="B10" s="314">
+      <c r="B10" s="309">
         <v>44066</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -17311,8 +17314,8 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A11" s="313"/>
-      <c r="B11" s="314"/>
+      <c r="A11" s="308"/>
+      <c r="B11" s="309"/>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
@@ -17344,7 +17347,7 @@
       <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="314">
+      <c r="B12" s="309">
         <v>44067</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -17376,7 +17379,7 @@
       <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="B13" s="314"/>
+      <c r="B13" s="309"/>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
@@ -17469,12 +17472,12 @@
       <c r="S15" s="8"/>
     </row>
     <row r="16" spans="1:19" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="295" t="s">
+      <c r="A16" s="304" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="295"/>
-      <c r="C16" s="295"/>
-      <c r="D16" s="296"/>
+      <c r="B16" s="304"/>
+      <c r="C16" s="304"/>
+      <c r="D16" s="305"/>
       <c r="E16" s="16">
         <f>SUM(E3:E15)</f>
         <v>0</v>
@@ -17501,10 +17504,10 @@
       <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="297"/>
-      <c r="B17" s="297"/>
-      <c r="C17" s="297"/>
-      <c r="D17" s="298"/>
+      <c r="A17" s="306"/>
+      <c r="B17" s="306"/>
+      <c r="C17" s="306"/>
+      <c r="D17" s="307"/>
       <c r="E17" s="17" t="s">
         <v>61</v>
       </c>
@@ -17549,18 +17552,18 @@
       <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="308" t="s">
+      <c r="A19" s="302" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="309"/>
-      <c r="C19" s="309"/>
+      <c r="B19" s="303"/>
+      <c r="C19" s="303"/>
       <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="310" t="s">
+      <c r="E19" s="295" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="310"/>
+      <c r="F19" s="295"/>
       <c r="G19" s="14">
         <v>31780</v>
       </c>
@@ -17645,10 +17648,10 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A22" s="302">
+      <c r="A22" s="299">
         <v>12</v>
       </c>
-      <c r="B22" s="299">
+      <c r="B22" s="296">
         <v>44076</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -17677,8 +17680,8 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A23" s="303"/>
-      <c r="B23" s="300"/>
+      <c r="A23" s="300"/>
+      <c r="B23" s="297"/>
       <c r="C23" s="21" t="s">
         <v>21</v>
       </c>
@@ -17705,8 +17708,8 @@
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A24" s="304"/>
-      <c r="B24" s="301"/>
+      <c r="A24" s="301"/>
+      <c r="B24" s="298"/>
       <c r="C24" s="21" t="s">
         <v>22</v>
       </c>
@@ -17735,10 +17738,10 @@
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A25" s="302">
+      <c r="A25" s="299">
         <v>13</v>
       </c>
-      <c r="B25" s="299">
+      <c r="B25" s="296">
         <v>44077</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -17769,8 +17772,8 @@
       <c r="S25" s="8"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A26" s="304"/>
-      <c r="B26" s="301"/>
+      <c r="A26" s="301"/>
+      <c r="B26" s="298"/>
       <c r="C26" s="21" t="s">
         <v>26</v>
       </c>
@@ -17799,10 +17802,10 @@
       <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A27" s="302">
+      <c r="A27" s="299">
         <v>14</v>
       </c>
-      <c r="B27" s="299">
+      <c r="B27" s="296">
         <v>44078</v>
       </c>
       <c r="C27" s="21" t="s">
@@ -17831,8 +17834,8 @@
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A28" s="304"/>
-      <c r="B28" s="301"/>
+      <c r="A28" s="301"/>
+      <c r="B28" s="298"/>
       <c r="C28" s="21" t="s">
         <v>28</v>
       </c>
@@ -17861,10 +17864,10 @@
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A29" s="302">
+      <c r="A29" s="299">
         <v>15</v>
       </c>
-      <c r="B29" s="299">
+      <c r="B29" s="296">
         <v>44079</v>
       </c>
       <c r="C29" s="21" t="s">
@@ -17893,8 +17896,8 @@
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A30" s="303"/>
-      <c r="B30" s="300"/>
+      <c r="A30" s="300"/>
+      <c r="B30" s="297"/>
       <c r="C30" s="21" t="s">
         <v>30</v>
       </c>
@@ -17923,8 +17926,8 @@
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A31" s="303"/>
-      <c r="B31" s="300"/>
+      <c r="A31" s="300"/>
+      <c r="B31" s="297"/>
       <c r="C31" s="21" t="s">
         <v>60</v>
       </c>
@@ -17951,8 +17954,8 @@
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A32" s="304"/>
-      <c r="B32" s="301"/>
+      <c r="A32" s="301"/>
+      <c r="B32" s="298"/>
       <c r="C32" s="23" t="s">
         <v>31</v>
       </c>
@@ -17979,10 +17982,10 @@
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A33" s="302">
+      <c r="A33" s="299">
         <v>16</v>
       </c>
-      <c r="B33" s="299">
+      <c r="B33" s="296">
         <v>44080</v>
       </c>
       <c r="C33" s="21" t="s">
@@ -18013,8 +18016,8 @@
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A34" s="303"/>
-      <c r="B34" s="300"/>
+      <c r="A34" s="300"/>
+      <c r="B34" s="297"/>
       <c r="C34" s="21" t="s">
         <v>33</v>
       </c>
@@ -18043,8 +18046,8 @@
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A35" s="303"/>
-      <c r="B35" s="300"/>
+      <c r="A35" s="300"/>
+      <c r="B35" s="297"/>
       <c r="C35" s="21" t="s">
         <v>36</v>
       </c>
@@ -18073,8 +18076,8 @@
       <c r="S35" s="8"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A36" s="303"/>
-      <c r="B36" s="300"/>
+      <c r="A36" s="300"/>
+      <c r="B36" s="297"/>
       <c r="C36" s="21" t="s">
         <v>37</v>
       </c>
@@ -18103,8 +18106,8 @@
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A37" s="304"/>
-      <c r="B37" s="301"/>
+      <c r="A37" s="301"/>
+      <c r="B37" s="298"/>
       <c r="C37" s="21" t="s">
         <v>39</v>
       </c>
@@ -18131,10 +18134,10 @@
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A38" s="302">
+      <c r="A38" s="299">
         <v>17</v>
       </c>
-      <c r="B38" s="299">
+      <c r="B38" s="296">
         <v>44081</v>
       </c>
       <c r="C38" s="21" t="s">
@@ -18163,8 +18166,8 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A39" s="303"/>
-      <c r="B39" s="300"/>
+      <c r="A39" s="300"/>
+      <c r="B39" s="297"/>
       <c r="C39" s="21" t="s">
         <v>28</v>
       </c>
@@ -18191,8 +18194,8 @@
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A40" s="304"/>
-      <c r="B40" s="301"/>
+      <c r="A40" s="301"/>
+      <c r="B40" s="298"/>
       <c r="C40" s="21" t="s">
         <v>40</v>
       </c>
@@ -18221,10 +18224,10 @@
       <c r="S40" s="8"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A41" s="302">
+      <c r="A41" s="299">
         <v>18</v>
       </c>
-      <c r="B41" s="299">
+      <c r="B41" s="296">
         <v>44082</v>
       </c>
       <c r="C41" s="21" t="s">
@@ -18253,8 +18256,8 @@
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A42" s="304"/>
-      <c r="B42" s="301"/>
+      <c r="A42" s="301"/>
+      <c r="B42" s="298"/>
       <c r="C42" s="21" t="s">
         <v>42</v>
       </c>
@@ -18281,10 +18284,10 @@
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A43" s="302">
+      <c r="A43" s="299">
         <v>19</v>
       </c>
-      <c r="B43" s="299">
+      <c r="B43" s="296">
         <v>44083</v>
       </c>
       <c r="C43" s="21" t="s">
@@ -18313,8 +18316,8 @@
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A44" s="304"/>
-      <c r="B44" s="301"/>
+      <c r="A44" s="301"/>
+      <c r="B44" s="298"/>
       <c r="C44" s="21" t="s">
         <v>44</v>
       </c>
@@ -18341,10 +18344,10 @@
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A45" s="302">
+      <c r="A45" s="299">
         <v>20</v>
       </c>
-      <c r="B45" s="299">
+      <c r="B45" s="296">
         <v>44084</v>
       </c>
       <c r="C45" s="21" t="s">
@@ -18373,8 +18376,8 @@
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A46" s="304"/>
-      <c r="B46" s="301"/>
+      <c r="A46" s="301"/>
+      <c r="B46" s="298"/>
       <c r="C46" s="21" t="s">
         <v>45</v>
       </c>
@@ -18401,10 +18404,10 @@
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A47" s="302">
+      <c r="A47" s="299">
         <v>21</v>
       </c>
-      <c r="B47" s="299">
+      <c r="B47" s="296">
         <v>44085</v>
       </c>
       <c r="C47" s="21" t="s">
@@ -18433,8 +18436,8 @@
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A48" s="303"/>
-      <c r="B48" s="300"/>
+      <c r="A48" s="300"/>
+      <c r="B48" s="297"/>
       <c r="C48" s="21" t="s">
         <v>46</v>
       </c>
@@ -18461,8 +18464,8 @@
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A49" s="303"/>
-      <c r="B49" s="300"/>
+      <c r="A49" s="300"/>
+      <c r="B49" s="297"/>
       <c r="C49" s="21" t="s">
         <v>47</v>
       </c>
@@ -18489,8 +18492,8 @@
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A50" s="303"/>
-      <c r="B50" s="300"/>
+      <c r="A50" s="300"/>
+      <c r="B50" s="297"/>
       <c r="C50" s="23" t="s">
         <v>31</v>
       </c>
@@ -18517,8 +18520,8 @@
       <c r="S50" s="8"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A51" s="304"/>
-      <c r="B51" s="301"/>
+      <c r="A51" s="301"/>
+      <c r="B51" s="298"/>
       <c r="C51" s="21" t="s">
         <v>44</v>
       </c>
@@ -18547,10 +18550,10 @@
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A52" s="302">
+      <c r="A52" s="299">
         <v>22</v>
       </c>
-      <c r="B52" s="299">
+      <c r="B52" s="296">
         <v>44086</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -18581,8 +18584,8 @@
       <c r="S52" s="8"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A53" s="304"/>
-      <c r="B53" s="301"/>
+      <c r="A53" s="301"/>
+      <c r="B53" s="298"/>
       <c r="C53" s="21" t="s">
         <v>50</v>
       </c>
@@ -18609,10 +18612,10 @@
       <c r="S53" s="8"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A54" s="302">
+      <c r="A54" s="299">
         <v>23</v>
       </c>
-      <c r="B54" s="299">
+      <c r="B54" s="296">
         <v>44087</v>
       </c>
       <c r="C54" s="21" t="s">
@@ -18641,8 +18644,8 @@
       <c r="S54" s="8"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A55" s="303"/>
-      <c r="B55" s="300"/>
+      <c r="A55" s="300"/>
+      <c r="B55" s="297"/>
       <c r="C55" s="21" t="s">
         <v>28</v>
       </c>
@@ -18669,8 +18672,8 @@
       <c r="S55" s="8"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A56" s="303"/>
-      <c r="B56" s="300"/>
+      <c r="A56" s="300"/>
+      <c r="B56" s="297"/>
       <c r="C56" s="21" t="s">
         <v>51</v>
       </c>
@@ -18697,8 +18700,8 @@
       <c r="S56" s="8"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A57" s="303"/>
-      <c r="B57" s="300"/>
+      <c r="A57" s="300"/>
+      <c r="B57" s="297"/>
       <c r="C57" s="23" t="s">
         <v>31</v>
       </c>
@@ -18823,10 +18826,10 @@
       <c r="S60" s="8"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A61" s="302">
+      <c r="A61" s="299">
         <v>27</v>
       </c>
-      <c r="B61" s="299">
+      <c r="B61" s="296">
         <v>44091</v>
       </c>
       <c r="C61" s="21" t="s">
@@ -18855,8 +18858,8 @@
       <c r="S61" s="8"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A62" s="304"/>
-      <c r="B62" s="301"/>
+      <c r="A62" s="301"/>
+      <c r="B62" s="298"/>
       <c r="C62" s="21" t="s">
         <v>44</v>
       </c>
@@ -18915,10 +18918,10 @@
       <c r="S63" s="8"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A64" s="302">
+      <c r="A64" s="299">
         <v>29</v>
       </c>
-      <c r="B64" s="299">
+      <c r="B64" s="296">
         <v>44093</v>
       </c>
       <c r="C64" s="21" t="s">
@@ -18947,8 +18950,8 @@
       <c r="S64" s="8"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A65" s="304"/>
-      <c r="B65" s="301"/>
+      <c r="A65" s="301"/>
+      <c r="B65" s="298"/>
       <c r="C65" s="21" t="s">
         <v>18</v>
       </c>
@@ -19143,10 +19146,10 @@
       <c r="B71" s="28">
         <v>44101</v>
       </c>
-      <c r="C71" s="311" t="s">
+      <c r="C71" s="313" t="s">
         <v>65</v>
       </c>
-      <c r="D71" s="312"/>
+      <c r="D71" s="314"/>
       <c r="E71" s="26">
         <v>0</v>
       </c>
@@ -19171,10 +19174,10 @@
       <c r="S71" s="8"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A72" s="302">
+      <c r="A72" s="299">
         <v>37</v>
       </c>
-      <c r="B72" s="299">
+      <c r="B72" s="296">
         <v>44103</v>
       </c>
       <c r="C72" s="21" t="s">
@@ -19203,12 +19206,12 @@
       <c r="S72" s="8"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A73" s="304"/>
-      <c r="B73" s="301"/>
-      <c r="C73" s="311" t="s">
+      <c r="A73" s="301"/>
+      <c r="B73" s="298"/>
+      <c r="C73" s="313" t="s">
         <v>75</v>
       </c>
-      <c r="D73" s="312"/>
+      <c r="D73" s="314"/>
       <c r="E73" s="6">
         <v>100000</v>
       </c>
@@ -19265,12 +19268,12 @@
       <c r="S74" s="8"/>
     </row>
     <row r="75" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A75" s="295" t="s">
+      <c r="A75" s="304" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="295"/>
-      <c r="C75" s="295"/>
-      <c r="D75" s="296"/>
+      <c r="B75" s="304"/>
+      <c r="C75" s="304"/>
+      <c r="D75" s="305"/>
       <c r="E75" s="16">
         <f>SUM(E21:E74)</f>
         <v>132000</v>
@@ -19297,10 +19300,10 @@
       <c r="S75" s="8"/>
     </row>
     <row r="76" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="297"/>
-      <c r="B76" s="297"/>
-      <c r="C76" s="297"/>
-      <c r="D76" s="298"/>
+      <c r="A76" s="306"/>
+      <c r="B76" s="306"/>
+      <c r="C76" s="306"/>
+      <c r="D76" s="307"/>
       <c r="E76" s="17" t="s">
         <v>61</v>
       </c>
@@ -19345,18 +19348,18 @@
       <c r="S77" s="8"/>
     </row>
     <row r="78" spans="1:19" ht="27.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="308" t="s">
+      <c r="A78" s="302" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="309"/>
-      <c r="C78" s="309"/>
+      <c r="B78" s="303"/>
+      <c r="C78" s="303"/>
       <c r="D78" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E78" s="310" t="s">
+      <c r="E78" s="295" t="s">
         <v>0</v>
       </c>
-      <c r="F78" s="310"/>
+      <c r="F78" s="295"/>
       <c r="G78" s="14">
         <f>G75</f>
         <v>137640</v>
@@ -19410,10 +19413,10 @@
       <c r="S79" s="8"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A80" s="302">
+      <c r="A80" s="299">
         <v>39</v>
       </c>
-      <c r="B80" s="299">
+      <c r="B80" s="296">
         <v>44105</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -19442,8 +19445,8 @@
       <c r="S80" s="8"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A81" s="303"/>
-      <c r="B81" s="300"/>
+      <c r="A81" s="300"/>
+      <c r="B81" s="297"/>
       <c r="C81" s="1" t="s">
         <v>70</v>
       </c>
@@ -19470,8 +19473,8 @@
       <c r="S81" s="8"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A82" s="303"/>
-      <c r="B82" s="300"/>
+      <c r="A82" s="300"/>
+      <c r="B82" s="297"/>
       <c r="C82" s="34" t="s">
         <v>76</v>
       </c>
@@ -19500,9 +19503,9 @@
       <c r="S82" s="8"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A83" s="303"/>
-      <c r="B83" s="300"/>
-      <c r="C83" s="305" t="s">
+      <c r="A83" s="300"/>
+      <c r="B83" s="297"/>
+      <c r="C83" s="315" t="s">
         <v>77</v>
       </c>
       <c r="D83" s="32" t="s">
@@ -19530,9 +19533,9 @@
       <c r="S83" s="8"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A84" s="303"/>
-      <c r="B84" s="300"/>
-      <c r="C84" s="306"/>
+      <c r="A84" s="300"/>
+      <c r="B84" s="297"/>
+      <c r="C84" s="316"/>
       <c r="D84" s="32" t="s">
         <v>71</v>
       </c>
@@ -19558,9 +19561,9 @@
       <c r="S84" s="8"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A85" s="303"/>
-      <c r="B85" s="300"/>
-      <c r="C85" s="306"/>
+      <c r="A85" s="300"/>
+      <c r="B85" s="297"/>
+      <c r="C85" s="316"/>
       <c r="D85" s="32" t="s">
         <v>73</v>
       </c>
@@ -19586,9 +19589,9 @@
       <c r="S85" s="8"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A86" s="304"/>
-      <c r="B86" s="301"/>
-      <c r="C86" s="307"/>
+      <c r="A86" s="301"/>
+      <c r="B86" s="298"/>
+      <c r="C86" s="317"/>
       <c r="D86" s="32" t="s">
         <v>74</v>
       </c>
@@ -19646,10 +19649,10 @@
       <c r="S87" s="8"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A88" s="302">
+      <c r="A88" s="299">
         <v>41</v>
       </c>
-      <c r="B88" s="299">
+      <c r="B88" s="296">
         <v>44108</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -19678,8 +19681,8 @@
       <c r="S88" s="8"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A89" s="304"/>
-      <c r="B89" s="301"/>
+      <c r="A89" s="301"/>
+      <c r="B89" s="298"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="4"/>
@@ -19768,10 +19771,10 @@
       <c r="S91" s="8"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A92" s="302">
+      <c r="A92" s="299">
         <v>44</v>
       </c>
-      <c r="B92" s="299">
+      <c r="B92" s="296">
         <v>44112</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -19800,8 +19803,8 @@
       <c r="S92" s="8"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A93" s="303"/>
-      <c r="B93" s="300"/>
+      <c r="A93" s="300"/>
+      <c r="B93" s="297"/>
       <c r="C93" s="1" t="s">
         <v>113</v>
       </c>
@@ -19828,8 +19831,8 @@
       <c r="S93" s="8"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A94" s="303"/>
-      <c r="B94" s="300"/>
+      <c r="A94" s="300"/>
+      <c r="B94" s="297"/>
       <c r="C94" s="1" t="s">
         <v>98</v>
       </c>
@@ -19858,8 +19861,8 @@
       <c r="S94" s="8"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A95" s="304"/>
-      <c r="B95" s="301"/>
+      <c r="A95" s="301"/>
+      <c r="B95" s="298"/>
       <c r="C95" s="1" t="s">
         <v>111</v>
       </c>
@@ -20318,12 +20321,12 @@
       <c r="S113" s="8"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A114" s="295" t="s">
+      <c r="A114" s="304" t="s">
         <v>57</v>
       </c>
-      <c r="B114" s="295"/>
-      <c r="C114" s="295"/>
-      <c r="D114" s="296"/>
+      <c r="B114" s="304"/>
+      <c r="C114" s="304"/>
+      <c r="D114" s="305"/>
       <c r="E114" s="16">
         <f>SUM(E80:E113)</f>
         <v>600000</v>
@@ -20350,10 +20353,10 @@
       <c r="S114" s="8"/>
     </row>
     <row r="115" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="297"/>
-      <c r="B115" s="297"/>
-      <c r="C115" s="297"/>
-      <c r="D115" s="298"/>
+      <c r="A115" s="306"/>
+      <c r="B115" s="306"/>
+      <c r="C115" s="306"/>
+      <c r="D115" s="307"/>
       <c r="E115" s="17" t="s">
         <v>61</v>
       </c>
@@ -23535,50 +23538,6 @@
     </row>
   </sheetData>
   <mergeCells count="58">
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A37"/>
-    <mergeCell ref="A16:D17"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="C73:D73"/>
     <mergeCell ref="A114:D115"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A38:A40"/>
@@ -23593,6 +23552,50 @@
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="B92:B95"/>
     <mergeCell ref="A92:A95"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="C73:D73"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A16:D17"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="73" orientation="portrait" r:id="rId1"/>
@@ -24421,21 +24424,21 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="283" t="s">
+      <c r="A7" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="284"/>
-      <c r="C7" s="284"/>
+      <c r="B7" s="288"/>
+      <c r="C7" s="288"/>
       <c r="D7" s="44">
         <f>SUM(D4:D6)</f>
         <v>50000</v>
       </c>
       <c r="E7" s="50"/>
-      <c r="F7" s="283" t="s">
+      <c r="F7" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="284"/>
-      <c r="H7" s="285"/>
+      <c r="G7" s="288"/>
+      <c r="H7" s="289"/>
       <c r="I7" s="44">
         <f>SUM(I4:I6)</f>
         <v>50000</v>
@@ -25044,7 +25047,7 @@
   <dimension ref="B2:N21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -25075,7 +25078,7 @@
         <v>307</v>
       </c>
       <c r="F2" s="72">
-        <v>425000</v>
+        <v>440000</v>
       </c>
       <c r="H2" s="72"/>
     </row>
@@ -25106,7 +25109,7 @@
         <v>258</v>
       </c>
       <c r="F4" s="72">
-        <v>2850</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="5" spans="2:14" x14ac:dyDescent="0.5">
@@ -25174,7 +25177,7 @@
       </c>
       <c r="C10" s="72">
         <f>Kamil!D78</f>
-        <v>-17000</v>
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>428</v>
@@ -25233,7 +25236,7 @@
       </c>
       <c r="I14" s="181">
         <f>C19-F19</f>
-        <v>507960</v>
+        <v>508010</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.5">
@@ -25281,7 +25284,7 @@
       </c>
       <c r="C19" s="242">
         <f>SUM(C2:C18)</f>
-        <v>3012810</v>
+        <v>3029810</v>
       </c>
       <c r="D19" s="241"/>
       <c r="E19" s="241" t="s">
@@ -25289,7 +25292,7 @@
       </c>
       <c r="F19" s="242">
         <f>SUM(F2:F18)</f>
-        <v>2504850</v>
+        <v>2521800</v>
       </c>
       <c r="K19" s="72">
         <v>956</v>
@@ -25313,7 +25316,7 @@
   <dimension ref="D4:I30"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -25329,7 +25332,7 @@
       </c>
       <c r="E4" s="179">
         <f>'GT Calc'!I14</f>
-        <v>507960</v>
+        <v>508010</v>
       </c>
       <c r="F4" s="84"/>
       <c r="G4" s="84"/>
@@ -25402,9 +25405,7 @@
       <c r="D14" t="s">
         <v>431</v>
       </c>
-      <c r="E14" s="72">
-        <v>20000</v>
-      </c>
+      <c r="E14" s="72"/>
     </row>
     <row r="15" spans="4:8" x14ac:dyDescent="0.5">
       <c r="E15" s="179"/>
@@ -25427,7 +25428,7 @@
       </c>
       <c r="E19" s="179">
         <f>SUM(E6:E18)</f>
-        <v>400000</v>
+        <v>380000</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.5">
@@ -25436,7 +25437,7 @@
       </c>
       <c r="E20" s="179">
         <f>E4-E19</f>
-        <v>107960</v>
+        <v>128010</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.5">
@@ -28293,11 +28294,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="A78:I78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="F91:H91"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="A51:C51"/>
@@ -28313,11 +28314,11 @@
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="A78:I78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="F71:H71"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -28347,19 +28348,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="286" t="s">
+      <c r="A1" s="290" t="s">
         <v>304</v>
       </c>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="288"/>
-      <c r="G1" s="281" t="s">
+      <c r="B1" s="291"/>
+      <c r="C1" s="291"/>
+      <c r="D1" s="291"/>
+      <c r="E1" s="292"/>
+      <c r="G1" s="285" t="s">
         <v>411</v>
       </c>
-      <c r="H1" s="281"/>
-      <c r="I1" s="281"/>
-      <c r="J1" s="281"/>
+      <c r="H1" s="285"/>
+      <c r="I1" s="285"/>
+      <c r="J1" s="285"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -28381,18 +28382,18 @@
         <v>4</v>
       </c>
       <c r="F2" s="227"/>
-      <c r="G2" s="282" t="s">
+      <c r="G2" s="286" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="282"/>
-      <c r="I2" s="282"/>
-      <c r="J2" s="282"/>
+      <c r="H2" s="286"/>
+      <c r="I2" s="286"/>
+      <c r="J2" s="286"/>
       <c r="K2" s="227"/>
       <c r="L2" s="227"/>
       <c r="M2" s="227"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A3" s="277">
+      <c r="A3" s="280">
         <v>1</v>
       </c>
       <c r="B3" s="200">
@@ -28404,7 +28405,7 @@
       <c r="D3" s="198">
         <v>30000</v>
       </c>
-      <c r="E3" s="279">
+      <c r="E3" s="278">
         <f>D4-D3</f>
         <v>-30000</v>
       </c>
@@ -28425,11 +28426,11 @@
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A4" s="278"/>
+      <c r="A4" s="281"/>
       <c r="B4" s="202"/>
       <c r="C4" s="203"/>
       <c r="D4" s="199"/>
-      <c r="E4" s="280"/>
+      <c r="E4" s="279"/>
       <c r="G4" s="219">
         <v>1</v>
       </c>
@@ -28465,7 +28466,7 @@
       <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A6" s="277">
+      <c r="A6" s="280">
         <v>2</v>
       </c>
       <c r="B6" s="200">
@@ -28477,7 +28478,7 @@
       <c r="D6" s="198">
         <v>5000</v>
       </c>
-      <c r="E6" s="279">
+      <c r="E6" s="278">
         <f>D7-D6</f>
         <v>-5000</v>
       </c>
@@ -28498,11 +28499,11 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A7" s="278"/>
+      <c r="A7" s="281"/>
       <c r="B7" s="202"/>
       <c r="C7" s="203"/>
       <c r="D7" s="199"/>
-      <c r="E7" s="280"/>
+      <c r="E7" s="279"/>
       <c r="G7" s="219">
         <v>3</v>
       </c>
@@ -28538,7 +28539,7 @@
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A9" s="277">
+      <c r="A9" s="280">
         <v>4</v>
       </c>
       <c r="B9" s="200">
@@ -28550,7 +28551,7 @@
       <c r="D9" s="198">
         <v>3070</v>
       </c>
-      <c r="E9" s="279">
+      <c r="E9" s="278">
         <f>D10-D9</f>
         <v>-3070</v>
       </c>
@@ -28571,11 +28572,11 @@
       <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A10" s="278"/>
+      <c r="A10" s="281"/>
       <c r="B10" s="202"/>
       <c r="C10" s="203"/>
       <c r="D10" s="199"/>
-      <c r="E10" s="280"/>
+      <c r="E10" s="279"/>
       <c r="G10" s="219">
         <v>5</v>
       </c>
@@ -28615,7 +28616,7 @@
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A12" s="277">
+      <c r="A12" s="280">
         <v>5</v>
       </c>
       <c r="B12" s="200">
@@ -28627,7 +28628,7 @@
       <c r="D12" s="198">
         <v>5000</v>
       </c>
-      <c r="E12" s="279">
+      <c r="E12" s="278">
         <f>D13-D12</f>
         <v>-5000</v>
       </c>
@@ -28648,11 +28649,11 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A13" s="278"/>
+      <c r="A13" s="281"/>
       <c r="B13" s="202"/>
       <c r="C13" s="203"/>
       <c r="D13" s="199"/>
-      <c r="E13" s="280"/>
+      <c r="E13" s="279"/>
       <c r="G13" s="1"/>
       <c r="H13" s="222"/>
       <c r="I13" s="1"/>
@@ -28676,7 +28677,7 @@
       <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A15" s="277">
+      <c r="A15" s="280">
         <v>6</v>
       </c>
       <c r="B15" s="200">
@@ -28688,7 +28689,7 @@
       <c r="D15" s="198">
         <v>5000</v>
       </c>
-      <c r="E15" s="279">
+      <c r="E15" s="278">
         <f>D16-D15</f>
         <v>-5000</v>
       </c>
@@ -28701,11 +28702,11 @@
       <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A16" s="278"/>
+      <c r="A16" s="281"/>
       <c r="B16" s="202"/>
       <c r="C16" s="203"/>
       <c r="D16" s="199"/>
-      <c r="E16" s="280"/>
+      <c r="E16" s="279"/>
       <c r="G16" s="1"/>
       <c r="H16" s="223"/>
       <c r="I16" s="1"/>
@@ -28729,7 +28730,7 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A18" s="277">
+      <c r="A18" s="280">
         <v>7</v>
       </c>
       <c r="B18" s="200">
@@ -28741,15 +28742,15 @@
       <c r="D18" s="198">
         <v>5000</v>
       </c>
-      <c r="E18" s="279">
+      <c r="E18" s="278">
         <f>D19-D18</f>
         <v>-5000</v>
       </c>
-      <c r="G18" s="283" t="s">
+      <c r="G18" s="287" t="s">
         <v>144</v>
       </c>
-      <c r="H18" s="284"/>
-      <c r="I18" s="285"/>
+      <c r="H18" s="288"/>
+      <c r="I18" s="289"/>
       <c r="J18" s="44">
         <f>SUM(J4:J17)</f>
         <v>0</v>
@@ -28759,11 +28760,11 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A19" s="278"/>
+      <c r="A19" s="281"/>
       <c r="B19" s="202"/>
       <c r="C19" s="203"/>
       <c r="D19" s="199"/>
-      <c r="E19" s="280"/>
+      <c r="E19" s="279"/>
       <c r="G19" s="55"/>
       <c r="H19" s="225"/>
       <c r="I19" s="55"/>
@@ -28789,7 +28790,7 @@
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A21" s="277">
+      <c r="A21" s="280">
         <v>8</v>
       </c>
       <c r="B21" s="200">
@@ -28801,7 +28802,7 @@
       <c r="D21" s="198">
         <v>600</v>
       </c>
-      <c r="E21" s="279">
+      <c r="E21" s="278">
         <f>D22-D21</f>
         <v>-600</v>
       </c>
@@ -28822,11 +28823,11 @@
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A22" s="278"/>
+      <c r="A22" s="281"/>
       <c r="B22" s="202"/>
       <c r="C22" s="203"/>
       <c r="D22" s="199"/>
-      <c r="E22" s="280"/>
+      <c r="E22" s="279"/>
       <c r="G22" s="220">
         <v>1</v>
       </c>
@@ -28866,7 +28867,7 @@
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A24" s="277">
+      <c r="A24" s="280">
         <v>9</v>
       </c>
       <c r="B24" s="200">
@@ -28878,7 +28879,7 @@
       <c r="D24" s="198">
         <v>5000</v>
       </c>
-      <c r="E24" s="279">
+      <c r="E24" s="278">
         <f>D25-D24</f>
         <v>-5000</v>
       </c>
@@ -28891,11 +28892,11 @@
       <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A25" s="278"/>
+      <c r="A25" s="281"/>
       <c r="B25" s="202"/>
       <c r="C25" s="203"/>
       <c r="D25" s="199"/>
-      <c r="E25" s="280"/>
+      <c r="E25" s="279"/>
       <c r="G25" s="220"/>
       <c r="H25" s="223"/>
       <c r="I25" s="1"/>
@@ -28919,7 +28920,7 @@
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A27" s="277">
+      <c r="A27" s="280">
         <v>10</v>
       </c>
       <c r="B27" s="200">
@@ -28931,7 +28932,7 @@
       <c r="D27" s="198">
         <v>5000</v>
       </c>
-      <c r="E27" s="279">
+      <c r="E27" s="278">
         <f>D28-D27</f>
         <v>-5000</v>
       </c>
@@ -28944,11 +28945,11 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A28" s="278"/>
+      <c r="A28" s="281"/>
       <c r="B28" s="202"/>
       <c r="C28" s="203"/>
       <c r="D28" s="199"/>
-      <c r="E28" s="280"/>
+      <c r="E28" s="279"/>
       <c r="G28" s="220"/>
       <c r="H28" s="223"/>
       <c r="I28" s="1"/>
@@ -28972,7 +28973,7 @@
       <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A30" s="277">
+      <c r="A30" s="280">
         <v>11</v>
       </c>
       <c r="B30" s="200">
@@ -28984,7 +28985,7 @@
       <c r="D30" s="198">
         <v>5000</v>
       </c>
-      <c r="E30" s="279">
+      <c r="E30" s="278">
         <f>D31-D30</f>
         <v>-5000</v>
       </c>
@@ -28997,11 +28998,11 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A31" s="278"/>
+      <c r="A31" s="281"/>
       <c r="B31" s="202"/>
       <c r="C31" s="203"/>
       <c r="D31" s="199"/>
-      <c r="E31" s="280"/>
+      <c r="E31" s="279"/>
       <c r="G31" s="1"/>
       <c r="H31" s="222"/>
       <c r="I31" s="1"/>
@@ -29025,7 +29026,7 @@
       <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A33" s="277">
+      <c r="A33" s="280">
         <v>12</v>
       </c>
       <c r="B33" s="200">
@@ -29037,7 +29038,7 @@
       <c r="D33" s="198">
         <v>2063</v>
       </c>
-      <c r="E33" s="279">
+      <c r="E33" s="278">
         <f>D34-D33</f>
         <v>0</v>
       </c>
@@ -29050,7 +29051,7 @@
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A34" s="278"/>
+      <c r="A34" s="281"/>
       <c r="B34" s="202">
         <v>44294</v>
       </c>
@@ -29060,7 +29061,7 @@
       <c r="D34" s="199">
         <v>2063</v>
       </c>
-      <c r="E34" s="280"/>
+      <c r="E34" s="279"/>
       <c r="G34" s="1"/>
       <c r="H34" s="223"/>
       <c r="I34" s="1"/>
@@ -29084,13 +29085,13 @@
       <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A36" s="277">
+      <c r="A36" s="280">
         <v>13</v>
       </c>
       <c r="B36" s="200"/>
       <c r="C36" s="201"/>
       <c r="D36" s="198"/>
-      <c r="E36" s="279">
+      <c r="E36" s="278">
         <f>D37-D36</f>
         <v>0</v>
       </c>
@@ -29108,11 +29109,11 @@
       <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A37" s="278"/>
+      <c r="A37" s="281"/>
       <c r="B37" s="202"/>
       <c r="C37" s="203"/>
       <c r="D37" s="199"/>
-      <c r="E37" s="280"/>
+      <c r="E37" s="279"/>
       <c r="G37" s="8"/>
       <c r="H37" s="230"/>
       <c r="I37" s="8"/>
@@ -29136,13 +29137,13 @@
       <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A39" s="277">
+      <c r="A39" s="280">
         <v>14</v>
       </c>
       <c r="B39" s="200"/>
       <c r="C39" s="201"/>
       <c r="D39" s="198"/>
-      <c r="E39" s="279">
+      <c r="E39" s="278">
         <f>D40-D39</f>
         <v>0</v>
       </c>
@@ -29155,11 +29156,11 @@
       <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A40" s="278"/>
+      <c r="A40" s="281"/>
       <c r="B40" s="202"/>
       <c r="C40" s="203"/>
       <c r="D40" s="199"/>
-      <c r="E40" s="280"/>
+      <c r="E40" s="279"/>
       <c r="G40" s="8"/>
       <c r="H40" s="230"/>
       <c r="I40" s="8"/>
@@ -29183,13 +29184,13 @@
       <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A42" s="277">
+      <c r="A42" s="280">
         <v>15</v>
       </c>
       <c r="B42" s="200"/>
       <c r="C42" s="201"/>
       <c r="D42" s="198"/>
-      <c r="E42" s="279">
+      <c r="E42" s="278">
         <f>D43-D42</f>
         <v>0</v>
       </c>
@@ -29202,11 +29203,11 @@
       <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A43" s="278"/>
+      <c r="A43" s="281"/>
       <c r="B43" s="202"/>
       <c r="C43" s="203"/>
       <c r="D43" s="199"/>
-      <c r="E43" s="280"/>
+      <c r="E43" s="279"/>
       <c r="G43" s="8"/>
       <c r="H43" s="230"/>
       <c r="I43" s="8"/>
@@ -29230,12 +29231,12 @@
       <c r="M44" s="8"/>
     </row>
     <row r="45" spans="1:13" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="290" t="s">
+      <c r="A45" s="282" t="s">
         <v>396</v>
       </c>
-      <c r="B45" s="291"/>
-      <c r="C45" s="291"/>
-      <c r="D45" s="292"/>
+      <c r="B45" s="283"/>
+      <c r="C45" s="283"/>
+      <c r="D45" s="284"/>
       <c r="E45" s="208">
         <f>SUM(E3:E44)</f>
         <v>-68670</v>
@@ -29252,8 +29253,8 @@
       <c r="A46" s="79"/>
       <c r="B46" s="228"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="289"/>
-      <c r="E46" s="289"/>
+      <c r="D46" s="277"/>
+      <c r="E46" s="277"/>
       <c r="G46" s="8"/>
       <c r="H46" s="230"/>
       <c r="I46" s="8"/>
@@ -29438,15 +29439,17 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A21:A22"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G18:I18"/>
@@ -29463,17 +29466,15 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="E42:E43"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -44016,21 +44017,21 @@
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="283" t="s">
+      <c r="A21" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="284"/>
-      <c r="C21" s="284"/>
+      <c r="B21" s="288"/>
+      <c r="C21" s="288"/>
       <c r="D21" s="44">
         <f>SUM(D4:D20)</f>
         <v>737500</v>
       </c>
       <c r="E21" s="50"/>
-      <c r="F21" s="283" t="s">
+      <c r="F21" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="284"/>
-      <c r="H21" s="285"/>
+      <c r="G21" s="288"/>
+      <c r="H21" s="289"/>
       <c r="I21" s="44">
         <f>SUM(I4:I20)</f>
         <v>737500</v>
@@ -45068,21 +45069,21 @@
       <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="283" t="s">
+      <c r="A17" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="284"/>
-      <c r="C17" s="284"/>
+      <c r="B17" s="288"/>
+      <c r="C17" s="288"/>
       <c r="D17" s="44">
         <f>SUM(D4:D16)</f>
         <v>284100</v>
       </c>
       <c r="E17" s="50"/>
-      <c r="F17" s="283" t="s">
+      <c r="F17" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="284"/>
-      <c r="H17" s="285"/>
+      <c r="G17" s="288"/>
+      <c r="H17" s="289"/>
       <c r="I17" s="44">
         <f>SUM(I4:I16)</f>
         <v>284115</v>
@@ -45957,21 +45958,21 @@
       <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="283" t="s">
+      <c r="A14" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="284"/>
-      <c r="C14" s="284"/>
+      <c r="B14" s="288"/>
+      <c r="C14" s="288"/>
       <c r="D14" s="44">
         <f>SUM(D4:D13)</f>
         <v>120000</v>
       </c>
       <c r="E14" s="50"/>
-      <c r="F14" s="283" t="s">
+      <c r="F14" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="284"/>
-      <c r="H14" s="285"/>
+      <c r="G14" s="288"/>
+      <c r="H14" s="289"/>
       <c r="I14" s="44">
         <f>SUM(I4:I13)</f>
         <v>120000</v>
@@ -46579,8 +46580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E03DA68B-CB4E-4FFC-8AF2-E82A88309945}">
   <dimension ref="A1:M96"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="J48" sqref="J48"/>
+    <sheetView topLeftCell="A58" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H70" sqref="H70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -46830,21 +46831,21 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="283" t="s">
+      <c r="A13" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="284"/>
-      <c r="C13" s="284"/>
+      <c r="B13" s="288"/>
+      <c r="C13" s="288"/>
       <c r="D13" s="44">
         <f>SUM(D4:D12)</f>
         <v>260000</v>
       </c>
       <c r="E13" s="50"/>
-      <c r="F13" s="283" t="s">
+      <c r="F13" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="284"/>
-      <c r="H13" s="285"/>
+      <c r="G13" s="288"/>
+      <c r="H13" s="289"/>
       <c r="I13" s="44">
         <f>SUM(I4:I12)</f>
         <v>260000</v>
@@ -47209,21 +47210,21 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A31" s="283" t="s">
+      <c r="A31" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="284"/>
-      <c r="C31" s="284"/>
+      <c r="B31" s="288"/>
+      <c r="C31" s="288"/>
       <c r="D31" s="44">
         <f>SUM(D23:D30)</f>
         <v>413000</v>
       </c>
       <c r="E31" s="50"/>
-      <c r="F31" s="283" t="s">
+      <c r="F31" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G31" s="284"/>
-      <c r="H31" s="285"/>
+      <c r="G31" s="288"/>
+      <c r="H31" s="289"/>
       <c r="I31" s="44">
         <f>SUM(I23:I30)</f>
         <v>413000</v>
@@ -47671,21 +47672,21 @@
       <c r="M54" s="8"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A55" s="283" t="s">
+      <c r="A55" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="284"/>
-      <c r="C55" s="284"/>
+      <c r="B55" s="288"/>
+      <c r="C55" s="288"/>
       <c r="D55" s="44">
         <f>SUM(D43:D54)</f>
         <v>1203500</v>
       </c>
       <c r="E55" s="50"/>
-      <c r="F55" s="283" t="s">
+      <c r="F55" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G55" s="284"/>
-      <c r="H55" s="285"/>
+      <c r="G55" s="288"/>
+      <c r="H55" s="289"/>
       <c r="I55" s="44">
         <f>SUM(I43:I54)</f>
         <v>1208500</v>
@@ -47930,10 +47931,18 @@
       <c r="M66" s="8"/>
     </row>
     <row r="67" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A67" s="170"/>
-      <c r="B67" s="39"/>
-      <c r="C67" s="1"/>
-      <c r="D67" s="40"/>
+      <c r="A67" s="170">
+        <v>3</v>
+      </c>
+      <c r="B67" s="39">
+        <v>44312</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>470</v>
+      </c>
+      <c r="D67" s="40">
+        <v>17000</v>
+      </c>
       <c r="E67" s="38"/>
       <c r="F67" s="170">
         <v>3</v>
@@ -48028,21 +48037,21 @@
       <c r="M72" s="8"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A73" s="283" t="s">
+      <c r="A73" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="284"/>
-      <c r="C73" s="284"/>
+      <c r="B73" s="288"/>
+      <c r="C73" s="288"/>
       <c r="D73" s="44">
         <f>SUM(D65:D72)</f>
-        <v>103500</v>
+        <v>120500</v>
       </c>
       <c r="E73" s="50"/>
-      <c r="F73" s="283" t="s">
+      <c r="F73" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G73" s="284"/>
-      <c r="H73" s="285"/>
+      <c r="G73" s="288"/>
+      <c r="H73" s="289"/>
       <c r="I73" s="44">
         <f>SUM(I65:I72)</f>
         <v>120500</v>
@@ -48075,7 +48084,7 @@
       </c>
       <c r="D75" s="58">
         <f>D73</f>
-        <v>103500</v>
+        <v>120500</v>
       </c>
       <c r="E75" s="8"/>
       <c r="F75" s="53"/>
@@ -48130,7 +48139,7 @@
       </c>
       <c r="D78" s="62">
         <f>D75-D76</f>
-        <v>-17000</v>
+        <v>0</v>
       </c>
       <c r="E78" s="8"/>
       <c r="F78" s="53"/>
@@ -48377,21 +48386,21 @@
       <c r="M90" s="8"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A91" s="283" t="s">
+      <c r="A91" s="287" t="s">
         <v>106</v>
       </c>
-      <c r="B91" s="284"/>
-      <c r="C91" s="284"/>
+      <c r="B91" s="288"/>
+      <c r="C91" s="288"/>
       <c r="D91" s="44">
         <f>SUM(D83:D90)</f>
         <v>120000</v>
       </c>
       <c r="E91" s="50"/>
-      <c r="F91" s="283" t="s">
+      <c r="F91" s="287" t="s">
         <v>105</v>
       </c>
-      <c r="G91" s="284"/>
-      <c r="H91" s="285"/>
+      <c r="G91" s="288"/>
+      <c r="H91" s="289"/>
       <c r="I91" s="44">
         <f>SUM(I83:I90)</f>
         <v>120000</v>
@@ -48473,31 +48482,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F31:H31"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="F73:H73"/>
     <mergeCell ref="A80:I80"/>
     <mergeCell ref="A81:D81"/>
     <mergeCell ref="F81:I81"/>
     <mergeCell ref="A91:C91"/>
     <mergeCell ref="F91:H91"/>
-    <mergeCell ref="A62:I62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="F55:H55"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
After Eif ul fitar 2021
</commit_message>
<xml_diff>
--- a/Office Statement Expense & Expenditure.xlsx
+++ b/Office Statement Expense & Expenditure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\1. Najeeb Associates\000FFICE\Office Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0949F352-8114-416B-A6C8-288E7F17F4FE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8B9691-258E-4B59-BF3E-7248F1656AE5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="820" activeTab="15" xr2:uid="{B2A19E3B-6786-4ED5-96A6-D1A6BAD18668}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="25786" windowHeight="13986" tabRatio="820" activeTab="16" xr2:uid="{B2A19E3B-6786-4ED5-96A6-D1A6BAD18668}"/>
   </bookViews>
   <sheets>
     <sheet name="BOFC" sheetId="4" r:id="rId1"/>
@@ -1583,9 +1583,6 @@
     <t>Handovered 58k Remaining from 209k of sunny - cleared</t>
   </si>
   <si>
-    <t>New Project</t>
-  </si>
-  <si>
     <t>Drinking water Office - 2 Canes</t>
   </si>
   <si>
@@ -1683,6 +1680,9 @@
   </si>
   <si>
     <t>Farooq - Going home, was ill</t>
+  </si>
+  <si>
+    <t>2 files sunny k pas hai</t>
   </si>
 </sst>
 </file>
@@ -3061,28 +3061,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="1" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3109,14 +3097,35 @@
     <xf numFmtId="0" fontId="16" fillId="13" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="11" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="11" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="10" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3136,23 +3145,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3168,21 +3183,6 @@
     </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4120,7 +4120,7 @@
         <v>44127</v>
       </c>
       <c r="H25" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="I25" s="40">
         <v>3000</v>
@@ -4252,7 +4252,7 @@
         <v>44132</v>
       </c>
       <c r="H31" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="I31" s="40">
         <v>180</v>
@@ -5256,7 +5256,7 @@
         <v>44191</v>
       </c>
       <c r="H75" s="68" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="I75" s="69">
         <v>7000</v>
@@ -7572,7 +7572,7 @@
       <c r="F173" s="258"/>
       <c r="G173" s="39"/>
       <c r="H173" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="I173" s="40">
         <v>120</v>
@@ -7604,7 +7604,7 @@
         <v>44292</v>
       </c>
       <c r="H174" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="I174" s="40">
         <v>200</v>
@@ -7624,7 +7624,7 @@
       <c r="F175" s="260"/>
       <c r="G175" s="39"/>
       <c r="H175" s="1" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="I175" s="40">
         <v>90</v>
@@ -7672,7 +7672,7 @@
         <v>44297</v>
       </c>
       <c r="H177" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="I177" s="40">
         <v>60</v>
@@ -7692,7 +7692,7 @@
       <c r="F178" s="246"/>
       <c r="G178" s="39"/>
       <c r="H178" s="1" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="I178" s="40">
         <v>150</v>
@@ -7740,7 +7740,7 @@
         <v>44299</v>
       </c>
       <c r="H180" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="I180" s="40">
         <v>120</v>
@@ -7764,7 +7764,7 @@
         <v>44308</v>
       </c>
       <c r="H181" s="1" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="I181" s="40">
         <v>400</v>
@@ -7788,7 +7788,7 @@
         <v>44309</v>
       </c>
       <c r="H182" s="1" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="I182" s="40">
         <v>230</v>
@@ -7808,7 +7808,7 @@
       <c r="F183" s="261"/>
       <c r="G183" s="39"/>
       <c r="H183" s="262" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I183" s="134">
         <v>24000</v>
@@ -7828,7 +7828,7 @@
       <c r="F184" s="263"/>
       <c r="G184" s="39"/>
       <c r="H184" s="66" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I184" s="40">
         <v>280</v>
@@ -7852,7 +7852,7 @@
         <v>44310</v>
       </c>
       <c r="H185" s="66" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="I185" s="40">
         <v>50000</v>
@@ -7876,7 +7876,7 @@
         <v>44311</v>
       </c>
       <c r="H186" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="I186" s="40">
         <v>50000</v>
@@ -7900,7 +7900,7 @@
         <v>44313</v>
       </c>
       <c r="H187" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I187" s="40">
         <v>980</v>
@@ -8066,7 +8066,7 @@
     </row>
     <row r="196" spans="1:14" ht="34" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A196" s="267" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B196" s="268"/>
       <c r="C196" s="268"/>
@@ -8175,7 +8175,7 @@
         <v>44324</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="D200" s="248">
         <v>100000</v>
@@ -8184,7 +8184,7 @@
       <c r="F200" s="264"/>
       <c r="G200" s="39"/>
       <c r="H200" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="I200" s="40">
         <v>1582</v>
@@ -8208,7 +8208,7 @@
         <v>44321</v>
       </c>
       <c r="H201" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="I201" s="40">
         <v>3650</v>
@@ -8228,7 +8228,7 @@
       <c r="F202" s="264"/>
       <c r="G202" s="39"/>
       <c r="H202" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="I202" s="40">
         <v>4572</v>
@@ -15083,47 +15083,47 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="A138:I138"/>
-    <mergeCell ref="A139:D139"/>
-    <mergeCell ref="F139:I139"/>
-    <mergeCell ref="A162:C162"/>
-    <mergeCell ref="F162:H162"/>
-    <mergeCell ref="A110:I110"/>
-    <mergeCell ref="A111:D111"/>
-    <mergeCell ref="F111:I111"/>
-    <mergeCell ref="A131:C131"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F33:H33"/>
-    <mergeCell ref="A33:C33"/>
-    <mergeCell ref="A40:I40"/>
-    <mergeCell ref="A41:D41"/>
-    <mergeCell ref="F41:I41"/>
-    <mergeCell ref="A55:C55"/>
-    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="A196:I196"/>
+    <mergeCell ref="A197:D197"/>
+    <mergeCell ref="F197:I197"/>
+    <mergeCell ref="A216:C216"/>
+    <mergeCell ref="F216:H216"/>
+    <mergeCell ref="A169:I169"/>
+    <mergeCell ref="A170:D170"/>
+    <mergeCell ref="F170:I170"/>
+    <mergeCell ref="A189:C189"/>
+    <mergeCell ref="F189:H189"/>
+    <mergeCell ref="A84:I84"/>
+    <mergeCell ref="A85:D85"/>
+    <mergeCell ref="F85:I85"/>
+    <mergeCell ref="A103:C103"/>
+    <mergeCell ref="F103:H103"/>
     <mergeCell ref="A61:I61"/>
     <mergeCell ref="A62:I62"/>
     <mergeCell ref="A63:D63"/>
     <mergeCell ref="F63:I63"/>
     <mergeCell ref="A77:C77"/>
     <mergeCell ref="F77:H77"/>
-    <mergeCell ref="A84:I84"/>
-    <mergeCell ref="A85:D85"/>
-    <mergeCell ref="F85:I85"/>
-    <mergeCell ref="A103:C103"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="A169:I169"/>
-    <mergeCell ref="A170:D170"/>
-    <mergeCell ref="F170:I170"/>
-    <mergeCell ref="A189:C189"/>
-    <mergeCell ref="F189:H189"/>
-    <mergeCell ref="A196:I196"/>
-    <mergeCell ref="A197:D197"/>
-    <mergeCell ref="F197:I197"/>
-    <mergeCell ref="A216:C216"/>
-    <mergeCell ref="F216:H216"/>
+    <mergeCell ref="A40:I40"/>
+    <mergeCell ref="A41:D41"/>
+    <mergeCell ref="F41:I41"/>
+    <mergeCell ref="A55:C55"/>
+    <mergeCell ref="F55:H55"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F33:H33"/>
+    <mergeCell ref="A33:C33"/>
+    <mergeCell ref="A110:I110"/>
+    <mergeCell ref="A111:D111"/>
+    <mergeCell ref="F111:I111"/>
+    <mergeCell ref="A131:C131"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="A138:I138"/>
+    <mergeCell ref="A139:D139"/>
+    <mergeCell ref="F139:I139"/>
+    <mergeCell ref="A162:C162"/>
+    <mergeCell ref="F162:H162"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="5" scale="10" orientation="portrait" r:id="rId1"/>
@@ -15541,7 +15541,7 @@
         <v>43954</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="I15" s="40">
         <v>500</v>
@@ -15582,21 +15582,21 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="287" t="s">
+      <c r="A18" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B18" s="288"/>
-      <c r="C18" s="288"/>
+      <c r="B18" s="284"/>
+      <c r="C18" s="284"/>
       <c r="D18" s="44">
         <f>SUM(D4:D17)</f>
         <v>15210</v>
       </c>
       <c r="E18" s="50"/>
-      <c r="F18" s="287" t="s">
+      <c r="F18" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G18" s="288"/>
-      <c r="H18" s="289"/>
+      <c r="G18" s="284"/>
+      <c r="H18" s="285"/>
       <c r="I18" s="44">
         <f>SUM(I4:I17)</f>
         <v>15710</v>
@@ -16342,21 +16342,21 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="287" t="s">
+      <c r="A7" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="288"/>
-      <c r="C7" s="288"/>
+      <c r="B7" s="284"/>
+      <c r="C7" s="284"/>
       <c r="D7" s="44">
         <f>SUM(D4:D6)</f>
         <v>0</v>
       </c>
       <c r="E7" s="50"/>
-      <c r="F7" s="287" t="s">
+      <c r="F7" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="288"/>
-      <c r="H7" s="289"/>
+      <c r="G7" s="284"/>
+      <c r="H7" s="285"/>
       <c r="I7" s="44">
         <f>SUM(I4:I6)</f>
         <v>0</v>
@@ -16983,18 +16983,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" ht="30.1" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="302" t="s">
+      <c r="A1" s="308" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="303"/>
-      <c r="C1" s="303"/>
+      <c r="B1" s="309"/>
+      <c r="C1" s="309"/>
       <c r="D1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="295" t="s">
+      <c r="E1" s="310" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="295"/>
+      <c r="F1" s="310"/>
       <c r="G1" s="14">
         <v>50000</v>
       </c>
@@ -17113,17 +17113,17 @@
       <c r="S4" s="8"/>
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A5" s="308">
+      <c r="A5" s="313">
         <v>3</v>
       </c>
-      <c r="B5" s="309">
+      <c r="B5" s="314">
         <v>44063</v>
       </c>
-      <c r="C5" s="310" t="s">
+      <c r="C5" s="315" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="311"/>
-      <c r="E5" s="312"/>
+      <c r="D5" s="316"/>
+      <c r="E5" s="317"/>
       <c r="F5" s="4">
         <v>11640</v>
       </c>
@@ -17145,11 +17145,11 @@
       <c r="S5" s="8"/>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A6" s="308"/>
-      <c r="B6" s="309"/>
-      <c r="C6" s="310"/>
-      <c r="D6" s="311"/>
-      <c r="E6" s="312"/>
+      <c r="A6" s="313"/>
+      <c r="B6" s="314"/>
+      <c r="C6" s="315"/>
+      <c r="D6" s="316"/>
+      <c r="E6" s="317"/>
       <c r="F6" s="4">
         <v>1700</v>
       </c>
@@ -17171,10 +17171,10 @@
       <c r="S6" s="8"/>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A7" s="308">
+      <c r="A7" s="313">
         <v>4</v>
       </c>
-      <c r="B7" s="309">
+      <c r="B7" s="314">
         <v>44064</v>
       </c>
       <c r="C7" s="1" t="s">
@@ -17203,8 +17203,8 @@
       <c r="S7" s="8"/>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A8" s="308"/>
-      <c r="B8" s="309"/>
+      <c r="A8" s="313"/>
+      <c r="B8" s="314"/>
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
@@ -17265,10 +17265,10 @@
       <c r="S9" s="8"/>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A10" s="308">
+      <c r="A10" s="313">
         <v>6</v>
       </c>
-      <c r="B10" s="309">
+      <c r="B10" s="314">
         <v>44066</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -17297,8 +17297,8 @@
       <c r="S10" s="8"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A11" s="308"/>
-      <c r="B11" s="309"/>
+      <c r="A11" s="313"/>
+      <c r="B11" s="314"/>
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
@@ -17330,7 +17330,7 @@
       <c r="A12" s="2">
         <v>7</v>
       </c>
-      <c r="B12" s="309">
+      <c r="B12" s="314">
         <v>44067</v>
       </c>
       <c r="C12" s="1" t="s">
@@ -17362,7 +17362,7 @@
       <c r="A13" s="2">
         <v>8</v>
       </c>
-      <c r="B13" s="309"/>
+      <c r="B13" s="314"/>
       <c r="C13" s="1" t="s">
         <v>12</v>
       </c>
@@ -17455,12 +17455,12 @@
       <c r="S15" s="8"/>
     </row>
     <row r="16" spans="1:19" ht="19.600000000000001" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A16" s="304" t="s">
+      <c r="A16" s="295" t="s">
         <v>57</v>
       </c>
-      <c r="B16" s="304"/>
-      <c r="C16" s="304"/>
-      <c r="D16" s="305"/>
+      <c r="B16" s="295"/>
+      <c r="C16" s="295"/>
+      <c r="D16" s="296"/>
       <c r="E16" s="16">
         <f>SUM(E3:E15)</f>
         <v>0</v>
@@ -17487,10 +17487,10 @@
       <c r="S16" s="8"/>
     </row>
     <row r="17" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A17" s="306"/>
-      <c r="B17" s="306"/>
-      <c r="C17" s="306"/>
-      <c r="D17" s="307"/>
+      <c r="A17" s="297"/>
+      <c r="B17" s="297"/>
+      <c r="C17" s="297"/>
+      <c r="D17" s="298"/>
       <c r="E17" s="17" t="s">
         <v>61</v>
       </c>
@@ -17535,18 +17535,18 @@
       <c r="S18" s="8"/>
     </row>
     <row r="19" spans="1:19" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="302" t="s">
+      <c r="A19" s="308" t="s">
         <v>5</v>
       </c>
-      <c r="B19" s="303"/>
-      <c r="C19" s="303"/>
+      <c r="B19" s="309"/>
+      <c r="C19" s="309"/>
       <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="295" t="s">
+      <c r="E19" s="310" t="s">
         <v>0</v>
       </c>
-      <c r="F19" s="295"/>
+      <c r="F19" s="310"/>
       <c r="G19" s="14">
         <v>31780</v>
       </c>
@@ -17631,10 +17631,10 @@
       <c r="S21" s="8"/>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A22" s="299">
+      <c r="A22" s="302">
         <v>12</v>
       </c>
-      <c r="B22" s="296">
+      <c r="B22" s="299">
         <v>44076</v>
       </c>
       <c r="C22" s="21" t="s">
@@ -17663,8 +17663,8 @@
       <c r="S22" s="8"/>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A23" s="300"/>
-      <c r="B23" s="297"/>
+      <c r="A23" s="303"/>
+      <c r="B23" s="300"/>
       <c r="C23" s="21" t="s">
         <v>21</v>
       </c>
@@ -17691,8 +17691,8 @@
       <c r="S23" s="8"/>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A24" s="301"/>
-      <c r="B24" s="298"/>
+      <c r="A24" s="304"/>
+      <c r="B24" s="301"/>
       <c r="C24" s="21" t="s">
         <v>22</v>
       </c>
@@ -17721,10 +17721,10 @@
       <c r="S24" s="8"/>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A25" s="299">
+      <c r="A25" s="302">
         <v>13</v>
       </c>
-      <c r="B25" s="296">
+      <c r="B25" s="299">
         <v>44077</v>
       </c>
       <c r="C25" s="21" t="s">
@@ -17755,8 +17755,8 @@
       <c r="S25" s="8"/>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A26" s="301"/>
-      <c r="B26" s="298"/>
+      <c r="A26" s="304"/>
+      <c r="B26" s="301"/>
       <c r="C26" s="21" t="s">
         <v>26</v>
       </c>
@@ -17785,10 +17785,10 @@
       <c r="S26" s="8"/>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A27" s="299">
+      <c r="A27" s="302">
         <v>14</v>
       </c>
-      <c r="B27" s="296">
+      <c r="B27" s="299">
         <v>44078</v>
       </c>
       <c r="C27" s="21" t="s">
@@ -17817,8 +17817,8 @@
       <c r="S27" s="8"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A28" s="301"/>
-      <c r="B28" s="298"/>
+      <c r="A28" s="304"/>
+      <c r="B28" s="301"/>
       <c r="C28" s="21" t="s">
         <v>28</v>
       </c>
@@ -17847,10 +17847,10 @@
       <c r="S28" s="8"/>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A29" s="299">
+      <c r="A29" s="302">
         <v>15</v>
       </c>
-      <c r="B29" s="296">
+      <c r="B29" s="299">
         <v>44079</v>
       </c>
       <c r="C29" s="21" t="s">
@@ -17879,8 +17879,8 @@
       <c r="S29" s="8"/>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A30" s="300"/>
-      <c r="B30" s="297"/>
+      <c r="A30" s="303"/>
+      <c r="B30" s="300"/>
       <c r="C30" s="21" t="s">
         <v>30</v>
       </c>
@@ -17909,8 +17909,8 @@
       <c r="S30" s="8"/>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A31" s="300"/>
-      <c r="B31" s="297"/>
+      <c r="A31" s="303"/>
+      <c r="B31" s="300"/>
       <c r="C31" s="21" t="s">
         <v>60</v>
       </c>
@@ -17937,8 +17937,8 @@
       <c r="S31" s="8"/>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A32" s="301"/>
-      <c r="B32" s="298"/>
+      <c r="A32" s="304"/>
+      <c r="B32" s="301"/>
       <c r="C32" s="23" t="s">
         <v>31</v>
       </c>
@@ -17965,10 +17965,10 @@
       <c r="S32" s="8"/>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A33" s="299">
+      <c r="A33" s="302">
         <v>16</v>
       </c>
-      <c r="B33" s="296">
+      <c r="B33" s="299">
         <v>44080</v>
       </c>
       <c r="C33" s="21" t="s">
@@ -17999,8 +17999,8 @@
       <c r="S33" s="8"/>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A34" s="300"/>
-      <c r="B34" s="297"/>
+      <c r="A34" s="303"/>
+      <c r="B34" s="300"/>
       <c r="C34" s="21" t="s">
         <v>33</v>
       </c>
@@ -18029,8 +18029,8 @@
       <c r="S34" s="8"/>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A35" s="300"/>
-      <c r="B35" s="297"/>
+      <c r="A35" s="303"/>
+      <c r="B35" s="300"/>
       <c r="C35" s="21" t="s">
         <v>36</v>
       </c>
@@ -18059,8 +18059,8 @@
       <c r="S35" s="8"/>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A36" s="300"/>
-      <c r="B36" s="297"/>
+      <c r="A36" s="303"/>
+      <c r="B36" s="300"/>
       <c r="C36" s="21" t="s">
         <v>37</v>
       </c>
@@ -18089,8 +18089,8 @@
       <c r="S36" s="8"/>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A37" s="301"/>
-      <c r="B37" s="298"/>
+      <c r="A37" s="304"/>
+      <c r="B37" s="301"/>
       <c r="C37" s="21" t="s">
         <v>39</v>
       </c>
@@ -18117,10 +18117,10 @@
       <c r="S37" s="8"/>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A38" s="299">
+      <c r="A38" s="302">
         <v>17</v>
       </c>
-      <c r="B38" s="296">
+      <c r="B38" s="299">
         <v>44081</v>
       </c>
       <c r="C38" s="21" t="s">
@@ -18149,8 +18149,8 @@
       <c r="S38" s="8"/>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A39" s="300"/>
-      <c r="B39" s="297"/>
+      <c r="A39" s="303"/>
+      <c r="B39" s="300"/>
       <c r="C39" s="21" t="s">
         <v>28</v>
       </c>
@@ -18177,8 +18177,8 @@
       <c r="S39" s="8"/>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A40" s="301"/>
-      <c r="B40" s="298"/>
+      <c r="A40" s="304"/>
+      <c r="B40" s="301"/>
       <c r="C40" s="21" t="s">
         <v>40</v>
       </c>
@@ -18207,10 +18207,10 @@
       <c r="S40" s="8"/>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A41" s="299">
+      <c r="A41" s="302">
         <v>18</v>
       </c>
-      <c r="B41" s="296">
+      <c r="B41" s="299">
         <v>44082</v>
       </c>
       <c r="C41" s="21" t="s">
@@ -18239,8 +18239,8 @@
       <c r="S41" s="8"/>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A42" s="301"/>
-      <c r="B42" s="298"/>
+      <c r="A42" s="304"/>
+      <c r="B42" s="301"/>
       <c r="C42" s="21" t="s">
         <v>42</v>
       </c>
@@ -18267,10 +18267,10 @@
       <c r="S42" s="8"/>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A43" s="299">
+      <c r="A43" s="302">
         <v>19</v>
       </c>
-      <c r="B43" s="296">
+      <c r="B43" s="299">
         <v>44083</v>
       </c>
       <c r="C43" s="21" t="s">
@@ -18299,8 +18299,8 @@
       <c r="S43" s="8"/>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A44" s="301"/>
-      <c r="B44" s="298"/>
+      <c r="A44" s="304"/>
+      <c r="B44" s="301"/>
       <c r="C44" s="21" t="s">
         <v>44</v>
       </c>
@@ -18327,10 +18327,10 @@
       <c r="S44" s="8"/>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A45" s="299">
+      <c r="A45" s="302">
         <v>20</v>
       </c>
-      <c r="B45" s="296">
+      <c r="B45" s="299">
         <v>44084</v>
       </c>
       <c r="C45" s="21" t="s">
@@ -18359,8 +18359,8 @@
       <c r="S45" s="8"/>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A46" s="301"/>
-      <c r="B46" s="298"/>
+      <c r="A46" s="304"/>
+      <c r="B46" s="301"/>
       <c r="C46" s="21" t="s">
         <v>45</v>
       </c>
@@ -18387,10 +18387,10 @@
       <c r="S46" s="8"/>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A47" s="299">
+      <c r="A47" s="302">
         <v>21</v>
       </c>
-      <c r="B47" s="296">
+      <c r="B47" s="299">
         <v>44085</v>
       </c>
       <c r="C47" s="21" t="s">
@@ -18419,8 +18419,8 @@
       <c r="S47" s="8"/>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A48" s="300"/>
-      <c r="B48" s="297"/>
+      <c r="A48" s="303"/>
+      <c r="B48" s="300"/>
       <c r="C48" s="21" t="s">
         <v>46</v>
       </c>
@@ -18447,8 +18447,8 @@
       <c r="S48" s="8"/>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A49" s="300"/>
-      <c r="B49" s="297"/>
+      <c r="A49" s="303"/>
+      <c r="B49" s="300"/>
       <c r="C49" s="21" t="s">
         <v>47</v>
       </c>
@@ -18475,8 +18475,8 @@
       <c r="S49" s="8"/>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A50" s="300"/>
-      <c r="B50" s="297"/>
+      <c r="A50" s="303"/>
+      <c r="B50" s="300"/>
       <c r="C50" s="23" t="s">
         <v>31</v>
       </c>
@@ -18503,8 +18503,8 @@
       <c r="S50" s="8"/>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A51" s="301"/>
-      <c r="B51" s="298"/>
+      <c r="A51" s="304"/>
+      <c r="B51" s="301"/>
       <c r="C51" s="21" t="s">
         <v>44</v>
       </c>
@@ -18533,10 +18533,10 @@
       <c r="S51" s="8"/>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A52" s="299">
+      <c r="A52" s="302">
         <v>22</v>
       </c>
-      <c r="B52" s="296">
+      <c r="B52" s="299">
         <v>44086</v>
       </c>
       <c r="C52" s="21" t="s">
@@ -18567,8 +18567,8 @@
       <c r="S52" s="8"/>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A53" s="301"/>
-      <c r="B53" s="298"/>
+      <c r="A53" s="304"/>
+      <c r="B53" s="301"/>
       <c r="C53" s="21" t="s">
         <v>50</v>
       </c>
@@ -18595,10 +18595,10 @@
       <c r="S53" s="8"/>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A54" s="299">
+      <c r="A54" s="302">
         <v>23</v>
       </c>
-      <c r="B54" s="296">
+      <c r="B54" s="299">
         <v>44087</v>
       </c>
       <c r="C54" s="21" t="s">
@@ -18627,8 +18627,8 @@
       <c r="S54" s="8"/>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A55" s="300"/>
-      <c r="B55" s="297"/>
+      <c r="A55" s="303"/>
+      <c r="B55" s="300"/>
       <c r="C55" s="21" t="s">
         <v>28</v>
       </c>
@@ -18655,8 +18655,8 @@
       <c r="S55" s="8"/>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A56" s="300"/>
-      <c r="B56" s="297"/>
+      <c r="A56" s="303"/>
+      <c r="B56" s="300"/>
       <c r="C56" s="21" t="s">
         <v>51</v>
       </c>
@@ -18683,8 +18683,8 @@
       <c r="S56" s="8"/>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A57" s="300"/>
-      <c r="B57" s="297"/>
+      <c r="A57" s="303"/>
+      <c r="B57" s="300"/>
       <c r="C57" s="23" t="s">
         <v>31</v>
       </c>
@@ -18809,10 +18809,10 @@
       <c r="S60" s="8"/>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A61" s="299">
+      <c r="A61" s="302">
         <v>27</v>
       </c>
-      <c r="B61" s="296">
+      <c r="B61" s="299">
         <v>44091</v>
       </c>
       <c r="C61" s="21" t="s">
@@ -18841,8 +18841,8 @@
       <c r="S61" s="8"/>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A62" s="301"/>
-      <c r="B62" s="298"/>
+      <c r="A62" s="304"/>
+      <c r="B62" s="301"/>
       <c r="C62" s="21" t="s">
         <v>44</v>
       </c>
@@ -18901,10 +18901,10 @@
       <c r="S63" s="8"/>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A64" s="299">
+      <c r="A64" s="302">
         <v>29</v>
       </c>
-      <c r="B64" s="296">
+      <c r="B64" s="299">
         <v>44093</v>
       </c>
       <c r="C64" s="21" t="s">
@@ -18933,8 +18933,8 @@
       <c r="S64" s="8"/>
     </row>
     <row r="65" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A65" s="301"/>
-      <c r="B65" s="298"/>
+      <c r="A65" s="304"/>
+      <c r="B65" s="301"/>
       <c r="C65" s="21" t="s">
         <v>18</v>
       </c>
@@ -19129,10 +19129,10 @@
       <c r="B71" s="28">
         <v>44101</v>
       </c>
-      <c r="C71" s="313" t="s">
+      <c r="C71" s="311" t="s">
         <v>65</v>
       </c>
-      <c r="D71" s="314"/>
+      <c r="D71" s="312"/>
       <c r="E71" s="26">
         <v>0</v>
       </c>
@@ -19157,10 +19157,10 @@
       <c r="S71" s="8"/>
     </row>
     <row r="72" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A72" s="299">
+      <c r="A72" s="302">
         <v>37</v>
       </c>
-      <c r="B72" s="296">
+      <c r="B72" s="299">
         <v>44103</v>
       </c>
       <c r="C72" s="21" t="s">
@@ -19189,12 +19189,12 @@
       <c r="S72" s="8"/>
     </row>
     <row r="73" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A73" s="301"/>
-      <c r="B73" s="298"/>
-      <c r="C73" s="313" t="s">
+      <c r="A73" s="304"/>
+      <c r="B73" s="301"/>
+      <c r="C73" s="311" t="s">
         <v>75</v>
       </c>
-      <c r="D73" s="314"/>
+      <c r="D73" s="312"/>
       <c r="E73" s="6">
         <v>100000</v>
       </c>
@@ -19251,12 +19251,12 @@
       <c r="S74" s="8"/>
     </row>
     <row r="75" spans="1:19" ht="21" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A75" s="304" t="s">
+      <c r="A75" s="295" t="s">
         <v>57</v>
       </c>
-      <c r="B75" s="304"/>
-      <c r="C75" s="304"/>
-      <c r="D75" s="305"/>
+      <c r="B75" s="295"/>
+      <c r="C75" s="295"/>
+      <c r="D75" s="296"/>
       <c r="E75" s="16">
         <f>SUM(E21:E74)</f>
         <v>132000</v>
@@ -19283,10 +19283,10 @@
       <c r="S75" s="8"/>
     </row>
     <row r="76" spans="1:19" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A76" s="306"/>
-      <c r="B76" s="306"/>
-      <c r="C76" s="306"/>
-      <c r="D76" s="307"/>
+      <c r="A76" s="297"/>
+      <c r="B76" s="297"/>
+      <c r="C76" s="297"/>
+      <c r="D76" s="298"/>
       <c r="E76" s="17" t="s">
         <v>61</v>
       </c>
@@ -19331,18 +19331,18 @@
       <c r="S77" s="8"/>
     </row>
     <row r="78" spans="1:19" ht="27.7" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A78" s="302" t="s">
+      <c r="A78" s="308" t="s">
         <v>5</v>
       </c>
-      <c r="B78" s="303"/>
-      <c r="C78" s="303"/>
+      <c r="B78" s="309"/>
+      <c r="C78" s="309"/>
       <c r="D78" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="E78" s="295" t="s">
+      <c r="E78" s="310" t="s">
         <v>0</v>
       </c>
-      <c r="F78" s="295"/>
+      <c r="F78" s="310"/>
       <c r="G78" s="14">
         <f>G75</f>
         <v>137640</v>
@@ -19396,10 +19396,10 @@
       <c r="S79" s="8"/>
     </row>
     <row r="80" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A80" s="299">
+      <c r="A80" s="302">
         <v>39</v>
       </c>
-      <c r="B80" s="296">
+      <c r="B80" s="299">
         <v>44105</v>
       </c>
       <c r="C80" s="1" t="s">
@@ -19428,8 +19428,8 @@
       <c r="S80" s="8"/>
     </row>
     <row r="81" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A81" s="300"/>
-      <c r="B81" s="297"/>
+      <c r="A81" s="303"/>
+      <c r="B81" s="300"/>
       <c r="C81" s="1" t="s">
         <v>70</v>
       </c>
@@ -19456,8 +19456,8 @@
       <c r="S81" s="8"/>
     </row>
     <row r="82" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A82" s="300"/>
-      <c r="B82" s="297"/>
+      <c r="A82" s="303"/>
+      <c r="B82" s="300"/>
       <c r="C82" s="34" t="s">
         <v>76</v>
       </c>
@@ -19486,9 +19486,9 @@
       <c r="S82" s="8"/>
     </row>
     <row r="83" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A83" s="300"/>
-      <c r="B83" s="297"/>
-      <c r="C83" s="315" t="s">
+      <c r="A83" s="303"/>
+      <c r="B83" s="300"/>
+      <c r="C83" s="305" t="s">
         <v>77</v>
       </c>
       <c r="D83" s="32" t="s">
@@ -19516,9 +19516,9 @@
       <c r="S83" s="8"/>
     </row>
     <row r="84" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A84" s="300"/>
-      <c r="B84" s="297"/>
-      <c r="C84" s="316"/>
+      <c r="A84" s="303"/>
+      <c r="B84" s="300"/>
+      <c r="C84" s="306"/>
       <c r="D84" s="32" t="s">
         <v>71</v>
       </c>
@@ -19544,9 +19544,9 @@
       <c r="S84" s="8"/>
     </row>
     <row r="85" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A85" s="300"/>
-      <c r="B85" s="297"/>
-      <c r="C85" s="316"/>
+      <c r="A85" s="303"/>
+      <c r="B85" s="300"/>
+      <c r="C85" s="306"/>
       <c r="D85" s="32" t="s">
         <v>73</v>
       </c>
@@ -19572,9 +19572,9 @@
       <c r="S85" s="8"/>
     </row>
     <row r="86" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A86" s="301"/>
-      <c r="B86" s="298"/>
-      <c r="C86" s="317"/>
+      <c r="A86" s="304"/>
+      <c r="B86" s="301"/>
+      <c r="C86" s="307"/>
       <c r="D86" s="32" t="s">
         <v>74</v>
       </c>
@@ -19632,10 +19632,10 @@
       <c r="S87" s="8"/>
     </row>
     <row r="88" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A88" s="299">
+      <c r="A88" s="302">
         <v>41</v>
       </c>
-      <c r="B88" s="296">
+      <c r="B88" s="299">
         <v>44108</v>
       </c>
       <c r="C88" s="1" t="s">
@@ -19664,8 +19664,8 @@
       <c r="S88" s="8"/>
     </row>
     <row r="89" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A89" s="301"/>
-      <c r="B89" s="298"/>
+      <c r="A89" s="304"/>
+      <c r="B89" s="301"/>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="4"/>
@@ -19754,10 +19754,10 @@
       <c r="S91" s="8"/>
     </row>
     <row r="92" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A92" s="299">
+      <c r="A92" s="302">
         <v>44</v>
       </c>
-      <c r="B92" s="296">
+      <c r="B92" s="299">
         <v>44112</v>
       </c>
       <c r="C92" s="1" t="s">
@@ -19786,8 +19786,8 @@
       <c r="S92" s="8"/>
     </row>
     <row r="93" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A93" s="300"/>
-      <c r="B93" s="297"/>
+      <c r="A93" s="303"/>
+      <c r="B93" s="300"/>
       <c r="C93" s="1" t="s">
         <v>113</v>
       </c>
@@ -19814,8 +19814,8 @@
       <c r="S93" s="8"/>
     </row>
     <row r="94" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A94" s="300"/>
-      <c r="B94" s="297"/>
+      <c r="A94" s="303"/>
+      <c r="B94" s="300"/>
       <c r="C94" s="1" t="s">
         <v>98</v>
       </c>
@@ -19844,8 +19844,8 @@
       <c r="S94" s="8"/>
     </row>
     <row r="95" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A95" s="301"/>
-      <c r="B95" s="298"/>
+      <c r="A95" s="304"/>
+      <c r="B95" s="301"/>
       <c r="C95" s="1" t="s">
         <v>111</v>
       </c>
@@ -20304,12 +20304,12 @@
       <c r="S113" s="8"/>
     </row>
     <row r="114" spans="1:19" x14ac:dyDescent="0.5">
-      <c r="A114" s="304" t="s">
+      <c r="A114" s="295" t="s">
         <v>57</v>
       </c>
-      <c r="B114" s="304"/>
-      <c r="C114" s="304"/>
-      <c r="D114" s="305"/>
+      <c r="B114" s="295"/>
+      <c r="C114" s="295"/>
+      <c r="D114" s="296"/>
       <c r="E114" s="16">
         <f>SUM(E80:E113)</f>
         <v>600000</v>
@@ -20336,10 +20336,10 @@
       <c r="S114" s="8"/>
     </row>
     <row r="115" spans="1:19" ht="14.7" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A115" s="306"/>
-      <c r="B115" s="306"/>
-      <c r="C115" s="306"/>
-      <c r="D115" s="307"/>
+      <c r="A115" s="297"/>
+      <c r="B115" s="297"/>
+      <c r="C115" s="297"/>
+      <c r="D115" s="298"/>
       <c r="E115" s="17" t="s">
         <v>61</v>
       </c>
@@ -23521,6 +23521,50 @@
     </row>
   </sheetData>
   <mergeCells count="58">
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="B22:B24"/>
+    <mergeCell ref="A22:A24"/>
+    <mergeCell ref="A19:C19"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="B25:B26"/>
+    <mergeCell ref="A25:A26"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="B27:B28"/>
+    <mergeCell ref="B29:B32"/>
+    <mergeCell ref="A29:A32"/>
+    <mergeCell ref="A33:A37"/>
+    <mergeCell ref="A16:D17"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="B64:B65"/>
+    <mergeCell ref="A64:A65"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="B33:B37"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A1:C1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="B52:B53"/>
+    <mergeCell ref="A52:A53"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B47:B51"/>
+    <mergeCell ref="A47:A51"/>
+    <mergeCell ref="C71:D71"/>
+    <mergeCell ref="B72:B73"/>
+    <mergeCell ref="A72:A73"/>
+    <mergeCell ref="C73:D73"/>
     <mergeCell ref="A114:D115"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A38:A40"/>
@@ -23535,50 +23579,6 @@
     <mergeCell ref="A88:A89"/>
     <mergeCell ref="B92:B95"/>
     <mergeCell ref="A92:A95"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="B52:B53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B47:B51"/>
-    <mergeCell ref="A47:A51"/>
-    <mergeCell ref="C71:D71"/>
-    <mergeCell ref="B72:B73"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="C73:D73"/>
-    <mergeCell ref="A1:C1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A16:D17"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="B64:B65"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="B33:B37"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="B22:B24"/>
-    <mergeCell ref="A22:A24"/>
-    <mergeCell ref="A19:C19"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="B25:B26"/>
-    <mergeCell ref="A25:A26"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B29:B32"/>
-    <mergeCell ref="A29:A32"/>
-    <mergeCell ref="A33:A37"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="73" orientation="portrait" r:id="rId1"/>
@@ -24407,21 +24407,21 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A7" s="287" t="s">
+      <c r="A7" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B7" s="288"/>
-      <c r="C7" s="288"/>
+      <c r="B7" s="284"/>
+      <c r="C7" s="284"/>
       <c r="D7" s="44">
         <f>SUM(D4:D6)</f>
         <v>50000</v>
       </c>
       <c r="E7" s="50"/>
-      <c r="F7" s="287" t="s">
+      <c r="F7" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G7" s="288"/>
-      <c r="H7" s="289"/>
+      <c r="G7" s="284"/>
+      <c r="H7" s="285"/>
       <c r="I7" s="44">
         <f>SUM(I4:I6)</f>
         <v>50000</v>
@@ -25029,8 +25029,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8095CE61-3623-466A-A99B-F028ACAC31F9}">
   <dimension ref="B2:N21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -25077,7 +25077,7 @@
         <v>177</v>
       </c>
       <c r="F3" s="70">
-        <v>9900</v>
+        <v>7900</v>
       </c>
     </row>
     <row r="4" spans="2:14" x14ac:dyDescent="0.5">
@@ -25151,10 +25151,13 @@
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="F10" s="70">
         <v>348000</v>
+      </c>
+      <c r="H10" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="11" spans="2:14" x14ac:dyDescent="0.5">
@@ -25185,7 +25188,7 @@
     </row>
     <row r="13" spans="2:14" x14ac:dyDescent="0.5">
       <c r="E13" s="70" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="J13" s="185"/>
       <c r="K13" s="70">
@@ -25205,7 +25208,7 @@
       </c>
       <c r="I14" s="177">
         <f>C19-F19</f>
-        <v>551286</v>
+        <v>553286</v>
       </c>
     </row>
     <row r="15" spans="2:14" x14ac:dyDescent="0.5">
@@ -25261,7 +25264,7 @@
       </c>
       <c r="F19" s="238">
         <f>SUM(F2:F18)</f>
-        <v>2572900</v>
+        <v>2570900</v>
       </c>
       <c r="K19" s="70">
         <v>956</v>
@@ -25284,8 +25287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{63BA9BFA-17B0-4682-BC89-677BD0B4C364}">
   <dimension ref="D4:I30"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -25297,11 +25300,11 @@
   <sheetData>
     <row r="4" spans="4:8" x14ac:dyDescent="0.5">
       <c r="D4" s="82" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E4" s="175">
         <f>'GT Calc'!I14</f>
-        <v>551286</v>
+        <v>553286</v>
       </c>
       <c r="F4" s="82"/>
       <c r="G4" s="82"/>
@@ -25383,32 +25386,27 @@
       <c r="E16" s="70"/>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.5">
-      <c r="D17" t="s">
-        <v>439</v>
-      </c>
-      <c r="E17" s="70">
-        <v>30000</v>
-      </c>
+      <c r="E17" s="70"/>
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.5">
       <c r="E18" s="70"/>
     </row>
     <row r="19" spans="4:9" x14ac:dyDescent="0.5">
       <c r="D19" s="82" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E19" s="175">
         <f>SUM(E6:E18)</f>
-        <v>410000</v>
+        <v>380000</v>
       </c>
     </row>
     <row r="20" spans="4:9" x14ac:dyDescent="0.5">
       <c r="D20" s="82" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E20" s="175">
         <f>E4-E19</f>
-        <v>141286</v>
+        <v>173286</v>
       </c>
     </row>
     <row r="23" spans="4:9" x14ac:dyDescent="0.5">
@@ -28249,11 +28247,11 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A78:I78"/>
-    <mergeCell ref="A79:D79"/>
-    <mergeCell ref="F79:I79"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A58:I58"/>
+    <mergeCell ref="A59:D59"/>
+    <mergeCell ref="F59:I59"/>
+    <mergeCell ref="A71:C71"/>
+    <mergeCell ref="F71:H71"/>
     <mergeCell ref="A39:D39"/>
     <mergeCell ref="F39:I39"/>
     <mergeCell ref="A51:C51"/>
@@ -28269,11 +28267,11 @@
     <mergeCell ref="F11:H11"/>
     <mergeCell ref="A19:D19"/>
     <mergeCell ref="F19:I19"/>
-    <mergeCell ref="A58:I58"/>
-    <mergeCell ref="A59:D59"/>
-    <mergeCell ref="F59:I59"/>
-    <mergeCell ref="A71:C71"/>
-    <mergeCell ref="F71:H71"/>
+    <mergeCell ref="A78:I78"/>
+    <mergeCell ref="A79:D79"/>
+    <mergeCell ref="F79:I79"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="F91:H91"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape" r:id="rId1"/>
@@ -28303,19 +28301,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="31.7" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="290" t="s">
+      <c r="A1" s="286" t="s">
         <v>302</v>
       </c>
-      <c r="B1" s="291"/>
-      <c r="C1" s="291"/>
-      <c r="D1" s="291"/>
-      <c r="E1" s="292"/>
-      <c r="G1" s="285" t="s">
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="288"/>
+      <c r="G1" s="281" t="s">
         <v>407</v>
       </c>
-      <c r="H1" s="285"/>
-      <c r="I1" s="285"/>
-      <c r="J1" s="285"/>
+      <c r="H1" s="281"/>
+      <c r="I1" s="281"/>
+      <c r="J1" s="281"/>
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
       <c r="M1" s="8"/>
@@ -28337,18 +28335,18 @@
         <v>4</v>
       </c>
       <c r="F2" s="223"/>
-      <c r="G2" s="286" t="s">
+      <c r="G2" s="282" t="s">
         <v>81</v>
       </c>
-      <c r="H2" s="286"/>
-      <c r="I2" s="286"/>
-      <c r="J2" s="286"/>
+      <c r="H2" s="282"/>
+      <c r="I2" s="282"/>
+      <c r="J2" s="282"/>
       <c r="K2" s="223"/>
       <c r="L2" s="223"/>
       <c r="M2" s="223"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A3" s="280">
+      <c r="A3" s="277">
         <v>1</v>
       </c>
       <c r="B3" s="196">
@@ -28360,7 +28358,7 @@
       <c r="D3" s="194">
         <v>30000</v>
       </c>
-      <c r="E3" s="278">
+      <c r="E3" s="279">
         <f>D4-D3</f>
         <v>-30000</v>
       </c>
@@ -28381,11 +28379,11 @@
       <c r="M3" s="8"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A4" s="281"/>
+      <c r="A4" s="278"/>
       <c r="B4" s="198"/>
       <c r="C4" s="199"/>
       <c r="D4" s="195"/>
-      <c r="E4" s="279"/>
+      <c r="E4" s="280"/>
       <c r="G4" s="215">
         <v>1</v>
       </c>
@@ -28421,7 +28419,7 @@
       <c r="M5" s="8"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A6" s="280">
+      <c r="A6" s="277">
         <v>2</v>
       </c>
       <c r="B6" s="196">
@@ -28433,7 +28431,7 @@
       <c r="D6" s="194">
         <v>5000</v>
       </c>
-      <c r="E6" s="278">
+      <c r="E6" s="279">
         <f>D7-D6</f>
         <v>-5000</v>
       </c>
@@ -28454,11 +28452,11 @@
       <c r="M6" s="8"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A7" s="281"/>
+      <c r="A7" s="278"/>
       <c r="B7" s="198"/>
       <c r="C7" s="199"/>
       <c r="D7" s="195"/>
-      <c r="E7" s="279"/>
+      <c r="E7" s="280"/>
       <c r="G7" s="215">
         <v>3</v>
       </c>
@@ -28494,7 +28492,7 @@
       <c r="M8" s="8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A9" s="280">
+      <c r="A9" s="277">
         <v>4</v>
       </c>
       <c r="B9" s="196">
@@ -28506,7 +28504,7 @@
       <c r="D9" s="194">
         <v>3070</v>
       </c>
-      <c r="E9" s="278">
+      <c r="E9" s="279">
         <f>D10-D9</f>
         <v>-3070</v>
       </c>
@@ -28527,11 +28525,11 @@
       <c r="M9" s="8"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A10" s="281"/>
+      <c r="A10" s="278"/>
       <c r="B10" s="198"/>
       <c r="C10" s="199"/>
       <c r="D10" s="195"/>
-      <c r="E10" s="279"/>
+      <c r="E10" s="280"/>
       <c r="G10" s="215">
         <v>5</v>
       </c>
@@ -28571,7 +28569,7 @@
       <c r="M11" s="8"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A12" s="280">
+      <c r="A12" s="277">
         <v>5</v>
       </c>
       <c r="B12" s="196">
@@ -28583,7 +28581,7 @@
       <c r="D12" s="194">
         <v>5000</v>
       </c>
-      <c r="E12" s="278">
+      <c r="E12" s="279">
         <f>D13-D12</f>
         <v>-5000</v>
       </c>
@@ -28604,11 +28602,11 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A13" s="281"/>
+      <c r="A13" s="278"/>
       <c r="B13" s="198"/>
       <c r="C13" s="199"/>
       <c r="D13" s="195"/>
-      <c r="E13" s="279"/>
+      <c r="E13" s="280"/>
       <c r="G13" s="1"/>
       <c r="H13" s="218"/>
       <c r="I13" s="1"/>
@@ -28632,7 +28630,7 @@
       <c r="M14" s="8"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A15" s="280">
+      <c r="A15" s="277">
         <v>6</v>
       </c>
       <c r="B15" s="196">
@@ -28644,7 +28642,7 @@
       <c r="D15" s="194">
         <v>5000</v>
       </c>
-      <c r="E15" s="278">
+      <c r="E15" s="279">
         <f>D16-D15</f>
         <v>-5000</v>
       </c>
@@ -28657,11 +28655,11 @@
       <c r="M15" s="8"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A16" s="281"/>
+      <c r="A16" s="278"/>
       <c r="B16" s="198"/>
       <c r="C16" s="199"/>
       <c r="D16" s="195"/>
-      <c r="E16" s="279"/>
+      <c r="E16" s="280"/>
       <c r="G16" s="1"/>
       <c r="H16" s="219"/>
       <c r="I16" s="1"/>
@@ -28685,7 +28683,7 @@
       <c r="M17" s="8"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A18" s="280">
+      <c r="A18" s="277">
         <v>7</v>
       </c>
       <c r="B18" s="196">
@@ -28697,15 +28695,15 @@
       <c r="D18" s="194">
         <v>5000</v>
       </c>
-      <c r="E18" s="278">
+      <c r="E18" s="279">
         <f>D19-D18</f>
         <v>-5000</v>
       </c>
-      <c r="G18" s="287" t="s">
+      <c r="G18" s="283" t="s">
         <v>143</v>
       </c>
-      <c r="H18" s="288"/>
-      <c r="I18" s="289"/>
+      <c r="H18" s="284"/>
+      <c r="I18" s="285"/>
       <c r="J18" s="44">
         <f>SUM(J4:J17)</f>
         <v>0</v>
@@ -28715,11 +28713,11 @@
       <c r="M18" s="8"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A19" s="281"/>
+      <c r="A19" s="278"/>
       <c r="B19" s="198"/>
       <c r="C19" s="199"/>
       <c r="D19" s="195"/>
-      <c r="E19" s="279"/>
+      <c r="E19" s="280"/>
       <c r="G19" s="55"/>
       <c r="H19" s="221"/>
       <c r="I19" s="55"/>
@@ -28745,7 +28743,7 @@
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A21" s="280">
+      <c r="A21" s="277">
         <v>8</v>
       </c>
       <c r="B21" s="196">
@@ -28757,7 +28755,7 @@
       <c r="D21" s="194">
         <v>600</v>
       </c>
-      <c r="E21" s="278">
+      <c r="E21" s="279">
         <f>D22-D21</f>
         <v>-600</v>
       </c>
@@ -28778,11 +28776,11 @@
       <c r="M21" s="8"/>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A22" s="281"/>
+      <c r="A22" s="278"/>
       <c r="B22" s="198"/>
       <c r="C22" s="199"/>
       <c r="D22" s="195"/>
-      <c r="E22" s="279"/>
+      <c r="E22" s="280"/>
       <c r="G22" s="216">
         <v>1</v>
       </c>
@@ -28822,7 +28820,7 @@
       <c r="M23" s="8"/>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A24" s="280">
+      <c r="A24" s="277">
         <v>9</v>
       </c>
       <c r="B24" s="196">
@@ -28834,7 +28832,7 @@
       <c r="D24" s="194">
         <v>5000</v>
       </c>
-      <c r="E24" s="278">
+      <c r="E24" s="279">
         <f>D25-D24</f>
         <v>-5000</v>
       </c>
@@ -28847,11 +28845,11 @@
       <c r="M24" s="8"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A25" s="281"/>
+      <c r="A25" s="278"/>
       <c r="B25" s="198"/>
       <c r="C25" s="199"/>
       <c r="D25" s="195"/>
-      <c r="E25" s="279"/>
+      <c r="E25" s="280"/>
       <c r="G25" s="216"/>
       <c r="H25" s="219"/>
       <c r="I25" s="1"/>
@@ -28875,7 +28873,7 @@
       <c r="M26" s="8"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A27" s="280">
+      <c r="A27" s="277">
         <v>10</v>
       </c>
       <c r="B27" s="196">
@@ -28887,7 +28885,7 @@
       <c r="D27" s="194">
         <v>5000</v>
       </c>
-      <c r="E27" s="278">
+      <c r="E27" s="279">
         <f>D28-D27</f>
         <v>-5000</v>
       </c>
@@ -28900,11 +28898,11 @@
       <c r="M27" s="8"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A28" s="281"/>
+      <c r="A28" s="278"/>
       <c r="B28" s="198"/>
       <c r="C28" s="199"/>
       <c r="D28" s="195"/>
-      <c r="E28" s="279"/>
+      <c r="E28" s="280"/>
       <c r="G28" s="216"/>
       <c r="H28" s="219"/>
       <c r="I28" s="1"/>
@@ -28928,7 +28926,7 @@
       <c r="M29" s="8"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A30" s="280">
+      <c r="A30" s="277">
         <v>11</v>
       </c>
       <c r="B30" s="196">
@@ -28940,7 +28938,7 @@
       <c r="D30" s="194">
         <v>5000</v>
       </c>
-      <c r="E30" s="278">
+      <c r="E30" s="279">
         <f>D31-D30</f>
         <v>-5000</v>
       </c>
@@ -28953,11 +28951,11 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A31" s="281"/>
+      <c r="A31" s="278"/>
       <c r="B31" s="198"/>
       <c r="C31" s="199"/>
       <c r="D31" s="195"/>
-      <c r="E31" s="279"/>
+      <c r="E31" s="280"/>
       <c r="G31" s="1"/>
       <c r="H31" s="218"/>
       <c r="I31" s="1"/>
@@ -28981,19 +28979,19 @@
       <c r="M32" s="8"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A33" s="280">
+      <c r="A33" s="277">
         <v>12</v>
       </c>
       <c r="B33" s="196">
         <v>44293</v>
       </c>
       <c r="C33" s="197" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D33" s="194">
         <v>2063</v>
       </c>
-      <c r="E33" s="278">
+      <c r="E33" s="279">
         <f>D34-D33</f>
         <v>0</v>
       </c>
@@ -29006,17 +29004,17 @@
       <c r="M33" s="8"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A34" s="281"/>
+      <c r="A34" s="278"/>
       <c r="B34" s="198">
         <v>44294</v>
       </c>
       <c r="C34" s="199" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D34" s="195">
         <v>2063</v>
       </c>
-      <c r="E34" s="279"/>
+      <c r="E34" s="280"/>
       <c r="G34" s="1"/>
       <c r="H34" s="219"/>
       <c r="I34" s="1"/>
@@ -29040,13 +29038,13 @@
       <c r="M35" s="8"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A36" s="280">
+      <c r="A36" s="277">
         <v>13</v>
       </c>
       <c r="B36" s="196"/>
       <c r="C36" s="197"/>
       <c r="D36" s="194"/>
-      <c r="E36" s="278">
+      <c r="E36" s="279">
         <f>D37-D36</f>
         <v>0</v>
       </c>
@@ -29064,11 +29062,11 @@
       <c r="M36" s="8"/>
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A37" s="281"/>
+      <c r="A37" s="278"/>
       <c r="B37" s="198"/>
       <c r="C37" s="199"/>
       <c r="D37" s="195"/>
-      <c r="E37" s="279"/>
+      <c r="E37" s="280"/>
       <c r="G37" s="8"/>
       <c r="H37" s="226"/>
       <c r="I37" s="8"/>
@@ -29092,13 +29090,13 @@
       <c r="M38" s="8"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A39" s="280">
+      <c r="A39" s="277">
         <v>14</v>
       </c>
       <c r="B39" s="196"/>
       <c r="C39" s="197"/>
       <c r="D39" s="194"/>
-      <c r="E39" s="278">
+      <c r="E39" s="279">
         <f>D40-D39</f>
         <v>0</v>
       </c>
@@ -29111,11 +29109,11 @@
       <c r="M39" s="8"/>
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A40" s="281"/>
+      <c r="A40" s="278"/>
       <c r="B40" s="198"/>
       <c r="C40" s="199"/>
       <c r="D40" s="195"/>
-      <c r="E40" s="279"/>
+      <c r="E40" s="280"/>
       <c r="G40" s="8"/>
       <c r="H40" s="226"/>
       <c r="I40" s="8"/>
@@ -29139,13 +29137,13 @@
       <c r="M41" s="8"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A42" s="280">
+      <c r="A42" s="277">
         <v>15</v>
       </c>
       <c r="B42" s="196"/>
       <c r="C42" s="197"/>
       <c r="D42" s="194"/>
-      <c r="E42" s="278">
+      <c r="E42" s="279">
         <f>D43-D42</f>
         <v>0</v>
       </c>
@@ -29158,11 +29156,11 @@
       <c r="M42" s="8"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A43" s="281"/>
+      <c r="A43" s="278"/>
       <c r="B43" s="198"/>
       <c r="C43" s="199"/>
       <c r="D43" s="195"/>
-      <c r="E43" s="279"/>
+      <c r="E43" s="280"/>
       <c r="G43" s="8"/>
       <c r="H43" s="226"/>
       <c r="I43" s="8"/>
@@ -29186,12 +29184,12 @@
       <c r="M44" s="8"/>
     </row>
     <row r="45" spans="1:13" ht="29.35" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A45" s="282" t="s">
+      <c r="A45" s="290" t="s">
         <v>392</v>
       </c>
-      <c r="B45" s="283"/>
-      <c r="C45" s="283"/>
-      <c r="D45" s="284"/>
+      <c r="B45" s="291"/>
+      <c r="C45" s="291"/>
+      <c r="D45" s="292"/>
       <c r="E45" s="204">
         <f>SUM(E3:E44)</f>
         <v>-68670</v>
@@ -29208,8 +29206,8 @@
       <c r="A46" s="77"/>
       <c r="B46" s="224"/>
       <c r="C46" s="8"/>
-      <c r="D46" s="277"/>
-      <c r="E46" s="277"/>
+      <c r="D46" s="289"/>
+      <c r="E46" s="289"/>
       <c r="G46" s="8"/>
       <c r="H46" s="226"/>
       <c r="I46" s="8"/>
@@ -29394,17 +29392,15 @@
     </row>
   </sheetData>
   <mergeCells count="36">
-    <mergeCell ref="G20:J20"/>
-    <mergeCell ref="G36:I36"/>
-    <mergeCell ref="A33:A34"/>
-    <mergeCell ref="E33:E34"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="E30:E31"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="E36:E37"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="A21:A22"/>
+    <mergeCell ref="D46:E46"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="A27:A28"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A45:D45"/>
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="E39:E40"/>
+    <mergeCell ref="A42:A43"/>
+    <mergeCell ref="E42:E43"/>
     <mergeCell ref="G1:J1"/>
     <mergeCell ref="G2:J2"/>
     <mergeCell ref="G18:I18"/>
@@ -29421,15 +29417,17 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="E18:E19"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="E21:E22"/>
-    <mergeCell ref="A27:A28"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="A45:D45"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="E39:E40"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="G20:J20"/>
+    <mergeCell ref="G36:I36"/>
+    <mergeCell ref="A33:A34"/>
+    <mergeCell ref="E33:E34"/>
+    <mergeCell ref="A30:A31"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="E36:E37"/>
+    <mergeCell ref="A24:A25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="A21:A22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -43972,21 +43970,21 @@
       <c r="M20" s="8"/>
     </row>
     <row r="21" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="287" t="s">
+      <c r="A21" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B21" s="288"/>
-      <c r="C21" s="288"/>
+      <c r="B21" s="284"/>
+      <c r="C21" s="284"/>
       <c r="D21" s="44">
         <f>SUM(D4:D20)</f>
         <v>737500</v>
       </c>
       <c r="E21" s="50"/>
-      <c r="F21" s="287" t="s">
+      <c r="F21" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G21" s="288"/>
-      <c r="H21" s="289"/>
+      <c r="G21" s="284"/>
+      <c r="H21" s="285"/>
       <c r="I21" s="44">
         <f>SUM(I4:I20)</f>
         <v>737500</v>
@@ -44901,7 +44899,7 @@
         <v>44294</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D11" s="40">
         <v>1100</v>
@@ -45024,21 +45022,21 @@
       <c r="M16" s="8"/>
     </row>
     <row r="17" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="287" t="s">
+      <c r="A17" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B17" s="288"/>
-      <c r="C17" s="288"/>
+      <c r="B17" s="284"/>
+      <c r="C17" s="284"/>
       <c r="D17" s="44">
         <f>SUM(D4:D16)</f>
         <v>284100</v>
       </c>
       <c r="E17" s="50"/>
-      <c r="F17" s="287" t="s">
+      <c r="F17" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G17" s="288"/>
-      <c r="H17" s="289"/>
+      <c r="G17" s="284"/>
+      <c r="H17" s="285"/>
       <c r="I17" s="44">
         <f>SUM(I4:I16)</f>
         <v>284115</v>
@@ -45913,21 +45911,21 @@
       <c r="M13" s="8"/>
     </row>
     <row r="14" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A14" s="287" t="s">
+      <c r="A14" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B14" s="288"/>
-      <c r="C14" s="288"/>
+      <c r="B14" s="284"/>
+      <c r="C14" s="284"/>
       <c r="D14" s="44">
         <f>SUM(D4:D13)</f>
         <v>120000</v>
       </c>
       <c r="E14" s="50"/>
-      <c r="F14" s="287" t="s">
+      <c r="F14" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G14" s="288"/>
-      <c r="H14" s="289"/>
+      <c r="G14" s="284"/>
+      <c r="H14" s="285"/>
       <c r="I14" s="44">
         <f>SUM(I4:I13)</f>
         <v>120000</v>
@@ -46786,21 +46784,21 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" ht="17.25" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A13" s="287" t="s">
+      <c r="A13" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B13" s="288"/>
-      <c r="C13" s="288"/>
+      <c r="B13" s="284"/>
+      <c r="C13" s="284"/>
       <c r="D13" s="44">
         <f>SUM(D4:D12)</f>
         <v>260000</v>
       </c>
       <c r="E13" s="50"/>
-      <c r="F13" s="287" t="s">
+      <c r="F13" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G13" s="288"/>
-      <c r="H13" s="289"/>
+      <c r="G13" s="284"/>
+      <c r="H13" s="285"/>
       <c r="I13" s="44">
         <f>SUM(I4:I12)</f>
         <v>260000</v>
@@ -47165,21 +47163,21 @@
       <c r="M30" s="8"/>
     </row>
     <row r="31" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A31" s="287" t="s">
+      <c r="A31" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="288"/>
-      <c r="C31" s="288"/>
+      <c r="B31" s="284"/>
+      <c r="C31" s="284"/>
       <c r="D31" s="44">
         <f>SUM(D23:D30)</f>
         <v>413000</v>
       </c>
       <c r="E31" s="50"/>
-      <c r="F31" s="287" t="s">
+      <c r="F31" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G31" s="288"/>
-      <c r="H31" s="289"/>
+      <c r="G31" s="284"/>
+      <c r="H31" s="285"/>
       <c r="I31" s="44">
         <f>SUM(I23:I30)</f>
         <v>413000</v>
@@ -47511,7 +47509,7 @@
         <v>44310</v>
       </c>
       <c r="H47" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I47" s="40">
         <v>5000</v>
@@ -47627,21 +47625,21 @@
       <c r="M54" s="8"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A55" s="287" t="s">
+      <c r="A55" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B55" s="288"/>
-      <c r="C55" s="288"/>
+      <c r="B55" s="284"/>
+      <c r="C55" s="284"/>
       <c r="D55" s="44">
         <f>SUM(D43:D54)</f>
         <v>1203500</v>
       </c>
       <c r="E55" s="50"/>
-      <c r="F55" s="287" t="s">
+      <c r="F55" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G55" s="288"/>
-      <c r="H55" s="289"/>
+      <c r="G55" s="284"/>
+      <c r="H55" s="285"/>
       <c r="I55" s="44">
         <f>SUM(I43:I54)</f>
         <v>1208500</v>
@@ -47893,7 +47891,7 @@
         <v>44312</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="D67" s="40">
         <v>17000</v>
@@ -47906,7 +47904,7 @@
         <v>44309</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="I67" s="40">
         <v>17000</v>
@@ -47992,21 +47990,21 @@
       <c r="M72" s="8"/>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A73" s="287" t="s">
+      <c r="A73" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B73" s="288"/>
-      <c r="C73" s="288"/>
+      <c r="B73" s="284"/>
+      <c r="C73" s="284"/>
       <c r="D73" s="44">
         <f>SUM(D65:D72)</f>
         <v>120500</v>
       </c>
       <c r="E73" s="50"/>
-      <c r="F73" s="287" t="s">
+      <c r="F73" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G73" s="288"/>
-      <c r="H73" s="289"/>
+      <c r="G73" s="284"/>
+      <c r="H73" s="285"/>
       <c r="I73" s="44">
         <f>SUM(I65:I72)</f>
         <v>120500</v>
@@ -48341,21 +48339,21 @@
       <c r="M90" s="8"/>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.5">
-      <c r="A91" s="287" t="s">
+      <c r="A91" s="283" t="s">
         <v>106</v>
       </c>
-      <c r="B91" s="288"/>
-      <c r="C91" s="288"/>
+      <c r="B91" s="284"/>
+      <c r="C91" s="284"/>
       <c r="D91" s="44">
         <f>SUM(D83:D90)</f>
         <v>120000</v>
       </c>
       <c r="E91" s="50"/>
-      <c r="F91" s="287" t="s">
+      <c r="F91" s="283" t="s">
         <v>105</v>
       </c>
-      <c r="G91" s="288"/>
-      <c r="H91" s="289"/>
+      <c r="G91" s="284"/>
+      <c r="H91" s="285"/>
       <c r="I91" s="44">
         <f>SUM(I83:I90)</f>
         <v>120000</v>
@@ -48437,31 +48435,31 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A80:I80"/>
+    <mergeCell ref="A81:D81"/>
+    <mergeCell ref="F81:I81"/>
+    <mergeCell ref="A91:C91"/>
+    <mergeCell ref="F91:H91"/>
+    <mergeCell ref="A62:I62"/>
+    <mergeCell ref="A63:D63"/>
+    <mergeCell ref="F63:I63"/>
+    <mergeCell ref="A73:C73"/>
+    <mergeCell ref="F73:H73"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="F2:I2"/>
+    <mergeCell ref="A13:C13"/>
+    <mergeCell ref="F13:H13"/>
+    <mergeCell ref="A20:I20"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="F21:I21"/>
+    <mergeCell ref="A31:C31"/>
+    <mergeCell ref="F31:H31"/>
     <mergeCell ref="A40:I40"/>
     <mergeCell ref="A41:D41"/>
     <mergeCell ref="F41:I41"/>
     <mergeCell ref="A55:C55"/>
     <mergeCell ref="F55:H55"/>
-    <mergeCell ref="A20:I20"/>
-    <mergeCell ref="A21:D21"/>
-    <mergeCell ref="F21:I21"/>
-    <mergeCell ref="A31:C31"/>
-    <mergeCell ref="F31:H31"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="F2:I2"/>
-    <mergeCell ref="A13:C13"/>
-    <mergeCell ref="F13:H13"/>
-    <mergeCell ref="A62:I62"/>
-    <mergeCell ref="A63:D63"/>
-    <mergeCell ref="F63:I63"/>
-    <mergeCell ref="A73:C73"/>
-    <mergeCell ref="F73:H73"/>
-    <mergeCell ref="A80:I80"/>
-    <mergeCell ref="A81:D81"/>
-    <mergeCell ref="F81:I81"/>
-    <mergeCell ref="A91:C91"/>
-    <mergeCell ref="F91:H91"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>